<commit_message>
BUILD_NUMBER 7 (picked as an arbitrary starting point
</commit_message>
<xml_diff>
--- a/syscon_usb/DACS_V1_0_ISE/tools/dacs_memory_map.xlsx
+++ b/syscon_usb/DACS_V1_0_ISE/tools/dacs_memory_map.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="15" windowWidth="19035" windowHeight="12015" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="15" windowWidth="19035" windowHeight="12015"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -15,8 +15,42 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Norton Allen</author>
+  </authors>
+  <commentList>
+    <comment ref="B10" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Norton Allen:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+This upper range is for real! Needed for status.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="179">
   <si>
     <t>DACS Memory Map</t>
   </si>
@@ -24,9 +58,6 @@
     <t>0C00</t>
   </si>
   <si>
-    <t>0DFE</t>
-  </si>
-  <si>
     <t>AI</t>
   </si>
   <si>
@@ -529,13 +560,40 @@
   </si>
   <si>
     <t>0338</t>
+  </si>
+  <si>
+    <t>0E00</t>
+  </si>
+  <si>
+    <t>0040</t>
+  </si>
+  <si>
+    <t>Syscon</t>
+  </si>
+  <si>
+    <t>INTA</t>
+  </si>
+  <si>
+    <t>0080</t>
+  </si>
+  <si>
+    <t>DACS</t>
+  </si>
+  <si>
+    <t>Build Number</t>
+  </si>
+  <si>
+    <t>0082</t>
+  </si>
+  <si>
+    <t>Build Name</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -557,6 +615,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -626,7 +697,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
@@ -662,6 +733,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -674,11 +751,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -973,88 +1045,130 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="4" max="4" width="14.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="2" spans="1:4">
+      <c r="A2" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="C2" t="s">
+        <v>172</v>
+      </c>
+      <c r="D2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" t="s">
+        <v>175</v>
+      </c>
+      <c r="D3" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" t="s">
+        <v>175</v>
+      </c>
+      <c r="D4" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C5" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="1" t="s">
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="C6" t="s">
         <v>5</v>
       </c>
-      <c r="C4" t="s">
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="1" t="s">
+      <c r="B7" t="s">
         <v>7</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="1" t="s">
+      <c r="B8" t="s">
         <v>9</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C8" t="s">
         <v>10</v>
       </c>
-      <c r="C6" t="s">
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" t="s">
+      <c r="B9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" t="s">
         <v>12</v>
       </c>
-      <c r="B7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" t="s">
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" t="s">
         <v>1</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B10" s="22" t="s">
+        <v>170</v>
+      </c>
+      <c r="C10" t="s">
         <v>2</v>
-      </c>
-      <c r="C8" t="s">
-        <v>3</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1062,7 +1176,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H85"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A31" sqref="A31:C31"/>
     </sheetView>
   </sheetViews>
@@ -1076,153 +1190,153 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="23" t="s">
-        <v>17</v>
-      </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="23"/>
+      <c r="A1" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="20"/>
+      <c r="C1" s="19"/>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" t="s">
         <v>18</v>
-      </c>
-      <c r="C3" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" t="s">
         <v>20</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" t="s">
         <v>22</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" t="s">
         <v>24</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" t="s">
         <v>26</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C12" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C13" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C14" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C15" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -1230,350 +1344,350 @@
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B17" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17" t="s">
         <v>18</v>
-      </c>
-      <c r="C17" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C18" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C19" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C20" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C21" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C22" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C23" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C24" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C25" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C26" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C27" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C28" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C29" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="31" spans="1:3">
-      <c r="A31" s="25" t="s">
-        <v>6</v>
-      </c>
-      <c r="B31" s="24"/>
-      <c r="C31" s="23"/>
+      <c r="A31" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="B31" s="20"/>
+      <c r="C31" s="19"/>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B33" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B33" s="4" t="s">
+      <c r="C33" t="s">
         <v>41</v>
-      </c>
-      <c r="C33" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C34" t="s">
         <v>43</v>
-      </c>
-      <c r="B34" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C34" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="35" spans="1:3">
       <c r="A35" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C35" t="s">
         <v>45</v>
-      </c>
-      <c r="B35" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C35" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="36" spans="1:3">
       <c r="A36" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C36" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="37" spans="1:3">
       <c r="A37" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C37" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="38" spans="1:3">
       <c r="A38" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C38" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="39" spans="1:3">
       <c r="A39" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C39" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="40" spans="1:3">
       <c r="A40" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C40" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="41" spans="1:3">
       <c r="A41" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C41" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="42" spans="1:3">
       <c r="A42" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C42" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="43" spans="1:3">
       <c r="A43" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C43" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="44" spans="1:3">
       <c r="A44" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C44" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="45" spans="1:3">
       <c r="A45" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C45" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="46" spans="1:3">
       <c r="A46" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C46" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="47" spans="1:3">
       <c r="A47" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C47" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="48" spans="1:3">
       <c r="A48" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C48" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="50" spans="1:8">
       <c r="A50" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="51" spans="1:8">
       <c r="D51" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="E51" s="19" t="s">
         <v>86</v>
       </c>
-      <c r="F51" s="19"/>
+      <c r="E51" s="23" t="s">
+        <v>85</v>
+      </c>
+      <c r="F51" s="23"/>
     </row>
     <row r="52" spans="1:8">
       <c r="A52" s="3">
         <v>600</v>
       </c>
       <c r="C52" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="53" spans="1:8">
@@ -1581,7 +1695,7 @@
         <v>602</v>
       </c>
       <c r="C53" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F53" s="8"/>
       <c r="G53" s="8"/>
@@ -1591,16 +1705,16 @@
         <v>610</v>
       </c>
       <c r="C54" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D54" s="4">
         <v>0</v>
       </c>
       <c r="E54" s="10" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F54" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G54" s="8"/>
       <c r="H54" s="9"/>
@@ -1610,16 +1724,16 @@
         <v>612</v>
       </c>
       <c r="C55" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D55" s="4">
         <v>0</v>
       </c>
       <c r="E55" s="10" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F55" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="56" spans="1:8">
@@ -1627,16 +1741,16 @@
         <v>614</v>
       </c>
       <c r="C56" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D56" s="4">
         <v>1</v>
       </c>
       <c r="E56" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="F56" s="7" t="s">
         <v>90</v>
-      </c>
-      <c r="F56" s="7" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="57" spans="1:8">
@@ -1644,16 +1758,16 @@
         <v>616</v>
       </c>
       <c r="C57" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D57" s="4">
         <v>1</v>
       </c>
       <c r="E57" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="F57" s="7" t="s">
         <v>90</v>
-      </c>
-      <c r="F57" s="7" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="58" spans="1:8">
@@ -1661,83 +1775,83 @@
         <v>618</v>
       </c>
       <c r="C58" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D58" s="4">
         <v>2</v>
       </c>
       <c r="E58" s="9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F58" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="59" spans="1:8">
       <c r="A59" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C59" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D59" s="4">
         <v>2</v>
       </c>
       <c r="E59" s="9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F59" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="60" spans="1:8">
       <c r="A60" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C60" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D60" s="4">
         <v>3</v>
       </c>
       <c r="E60" s="9" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F60" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="61" spans="1:8">
       <c r="A61" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C61" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D61" s="4">
         <v>3</v>
       </c>
       <c r="E61" s="9" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F61" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="63" spans="1:8">
       <c r="A63" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C63" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="64" spans="1:8">
       <c r="A64" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C64" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="65" spans="1:8">
@@ -1745,16 +1859,16 @@
         <v>630</v>
       </c>
       <c r="C65" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D65" s="4">
         <v>4</v>
       </c>
       <c r="E65" s="9" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F65" s="7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="66" spans="1:8">
@@ -1762,16 +1876,16 @@
         <v>632</v>
       </c>
       <c r="C66" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D66" s="4">
         <v>4</v>
       </c>
       <c r="E66" s="9" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F66" s="7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="67" spans="1:8">
@@ -1779,16 +1893,16 @@
         <v>634</v>
       </c>
       <c r="C67" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D67" s="4">
         <v>5</v>
       </c>
       <c r="E67" s="9" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F67" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="68" spans="1:8">
@@ -1796,16 +1910,16 @@
         <v>636</v>
       </c>
       <c r="C68" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D68" s="4">
         <v>5</v>
       </c>
       <c r="E68" s="9" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F68" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="69" spans="1:8">
@@ -1813,67 +1927,67 @@
         <v>638</v>
       </c>
       <c r="C69" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D69" s="4">
         <v>6</v>
       </c>
       <c r="E69" s="9" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F69" s="7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="70" spans="1:8">
       <c r="A70" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C70" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D70" s="4">
         <v>6</v>
       </c>
       <c r="E70" s="9" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F70" s="7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="71" spans="1:8">
       <c r="A71" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C71" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D71" s="4">
         <v>7</v>
       </c>
       <c r="E71" s="9" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F71" s="7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="72" spans="1:8">
       <c r="A72" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C72" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D72" s="4">
         <v>7</v>
       </c>
       <c r="E72" s="9" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F72" s="7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="74" spans="1:8">
@@ -1881,7 +1995,7 @@
         <v>640</v>
       </c>
       <c r="C74" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="75" spans="1:8">
@@ -1889,7 +2003,7 @@
         <v>642</v>
       </c>
       <c r="C75" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="76" spans="1:8">
@@ -1897,16 +2011,16 @@
         <v>650</v>
       </c>
       <c r="C76" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D76" s="4">
         <v>8</v>
       </c>
       <c r="E76" s="9" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F76" s="7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="77" spans="1:8">
@@ -1914,16 +2028,16 @@
         <v>652</v>
       </c>
       <c r="C77" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D77" s="4">
         <v>8</v>
       </c>
       <c r="E77" s="9" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F77" s="7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="78" spans="1:8">
@@ -1931,16 +2045,16 @@
         <v>654</v>
       </c>
       <c r="C78" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D78" s="4">
         <v>9</v>
       </c>
       <c r="E78" s="9" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F78" s="7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H78" s="9"/>
     </row>
@@ -1949,16 +2063,16 @@
         <v>656</v>
       </c>
       <c r="C79" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D79" s="4">
         <v>9</v>
       </c>
       <c r="E79" s="9" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F79" s="7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H79" s="9"/>
     </row>
@@ -1967,71 +2081,71 @@
         <v>658</v>
       </c>
       <c r="C80" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D80" s="4">
         <v>10</v>
       </c>
       <c r="E80" s="9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F80" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="H80" s="9"/>
     </row>
     <row r="81" spans="1:8">
       <c r="A81" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C81" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D81" s="4">
         <v>10</v>
       </c>
       <c r="E81" s="9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F81" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="H81" s="9"/>
     </row>
     <row r="82" spans="1:8">
       <c r="A82" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C82" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D82" s="4">
         <v>11</v>
       </c>
       <c r="E82" s="11" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="83" spans="1:8">
       <c r="A83" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C83" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D83" s="4">
         <v>11</v>
       </c>
       <c r="E83" s="11" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="85" spans="1:8">
       <c r="A85" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="C85" t="s">
         <v>119</v>
-      </c>
-      <c r="C85" t="s">
-        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -2066,40 +2180,40 @@
   <sheetData>
     <row r="1" spans="1:11" ht="23.25">
       <c r="A1" s="18" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="3" spans="1:11">
-      <c r="B3" s="20" t="s">
+      <c r="B3" s="24" t="s">
+        <v>120</v>
+      </c>
+      <c r="C3" s="24"/>
+      <c r="D3" s="24" t="s">
         <v>121</v>
       </c>
-      <c r="C3" s="20"/>
-      <c r="D3" s="20" t="s">
-        <v>122</v>
-      </c>
-      <c r="E3" s="20"/>
-      <c r="H3" s="20" t="s">
+      <c r="E3" s="24"/>
+      <c r="H3" s="24" t="s">
+        <v>120</v>
+      </c>
+      <c r="I3" s="24"/>
+      <c r="J3" s="24" t="s">
         <v>121</v>
       </c>
-      <c r="I3" s="20"/>
-      <c r="J3" s="20" t="s">
-        <v>122</v>
-      </c>
-      <c r="K3" s="20"/>
+      <c r="K3" s="24"/>
     </row>
     <row r="4" spans="1:11">
       <c r="A4" s="13">
         <v>800</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C4" s="15">
         <f>E4+1</f>
         <v>1</v>
       </c>
       <c r="D4" s="14" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E4" s="15">
         <v>0</v>
@@ -2108,14 +2222,14 @@
         <v>840</v>
       </c>
       <c r="H4" s="14" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="I4" s="15">
         <f>K4+1</f>
         <v>13</v>
       </c>
       <c r="J4" s="14" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="K4" s="15">
         <f>E20+6</f>
@@ -2127,14 +2241,14 @@
         <v>802</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C5" s="15">
         <f t="shared" ref="C5:C6" si="0">C4+2</f>
         <v>3</v>
       </c>
       <c r="D5" s="14" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E5" s="15">
         <f>E4+2</f>
@@ -2144,14 +2258,14 @@
         <v>842</v>
       </c>
       <c r="H5" s="14" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="I5" s="15">
         <f t="shared" ref="I5:I6" si="1">I4+2</f>
         <v>15</v>
       </c>
       <c r="J5" s="14" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="K5" s="15">
         <f>K4+2</f>
@@ -2163,14 +2277,14 @@
         <v>804</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C6" s="15">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="D6" s="14" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E6" s="15">
         <f>E5+2</f>
@@ -2180,14 +2294,14 @@
         <v>844</v>
       </c>
       <c r="H6" s="14" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="I6" s="15">
         <f t="shared" si="1"/>
         <v>17</v>
       </c>
       <c r="J6" s="14" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="K6" s="15">
         <f>K5+2</f>
@@ -2198,25 +2312,25 @@
       <c r="A7" s="13">
         <v>806</v>
       </c>
-      <c r="B7" s="21" t="s">
+      <c r="B7" s="25" t="s">
+        <v>122</v>
+      </c>
+      <c r="C7" s="26"/>
+      <c r="D7" s="25" t="s">
         <v>123</v>
       </c>
-      <c r="C7" s="22"/>
-      <c r="D7" s="21" t="s">
-        <v>124</v>
-      </c>
-      <c r="E7" s="22"/>
+      <c r="E7" s="26"/>
       <c r="G7" s="13">
         <v>846</v>
       </c>
-      <c r="H7" s="21" t="s">
+      <c r="H7" s="25" t="s">
+        <v>122</v>
+      </c>
+      <c r="I7" s="26"/>
+      <c r="J7" s="25" t="s">
         <v>123</v>
       </c>
-      <c r="I7" s="22"/>
-      <c r="J7" s="21" t="s">
-        <v>124</v>
-      </c>
-      <c r="K7" s="22"/>
+      <c r="K7" s="26"/>
     </row>
     <row r="8" spans="1:11">
       <c r="A8" s="13">
@@ -2225,7 +2339,7 @@
       <c r="B8" s="14"/>
       <c r="C8" s="15"/>
       <c r="D8" s="14" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E8" s="15">
         <f>E4</f>
@@ -2237,7 +2351,7 @@
       <c r="H8" s="14"/>
       <c r="I8" s="15"/>
       <c r="J8" s="14" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="K8" s="15">
         <f>K4</f>
@@ -2246,24 +2360,24 @@
     </row>
     <row r="9" spans="1:11">
       <c r="A9" s="13" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B9" s="14"/>
       <c r="C9" s="15"/>
       <c r="D9" s="14" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E9" s="15">
         <f t="shared" ref="E9:E10" si="2">E5</f>
         <v>2</v>
       </c>
       <c r="G9" s="13" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H9" s="14"/>
       <c r="I9" s="15"/>
       <c r="J9" s="14" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="K9" s="15">
         <f t="shared" ref="K9:K10" si="3">K5</f>
@@ -2272,24 +2386,24 @@
     </row>
     <row r="10" spans="1:11">
       <c r="A10" s="13" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B10" s="14"/>
       <c r="C10" s="15"/>
       <c r="D10" s="14" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E10" s="15">
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="G10" s="13" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H10" s="14"/>
       <c r="I10" s="15"/>
       <c r="J10" s="14" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="K10" s="15">
         <f t="shared" si="3"/>
@@ -2298,30 +2412,30 @@
     </row>
     <row r="11" spans="1:11">
       <c r="A11" s="13" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B11" s="14"/>
       <c r="C11" s="15"/>
-      <c r="D11" s="21" t="s">
-        <v>124</v>
-      </c>
-      <c r="E11" s="22"/>
+      <c r="D11" s="25" t="s">
+        <v>123</v>
+      </c>
+      <c r="E11" s="26"/>
       <c r="G11" s="13" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H11" s="14"/>
       <c r="I11" s="15"/>
-      <c r="J11" s="21" t="s">
-        <v>124</v>
-      </c>
-      <c r="K11" s="22"/>
+      <c r="J11" s="25" t="s">
+        <v>123</v>
+      </c>
+      <c r="K11" s="26"/>
     </row>
     <row r="12" spans="1:11">
       <c r="A12" s="13">
         <v>810</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C12" s="15">
         <f>C4</f>
@@ -2333,7 +2447,7 @@
         <v>850</v>
       </c>
       <c r="H12" s="14" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="I12" s="15">
         <f>I4</f>
@@ -2347,7 +2461,7 @@
         <v>812</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C13" s="15">
         <f t="shared" ref="C13:C14" si="4">C5</f>
@@ -2359,7 +2473,7 @@
         <v>852</v>
       </c>
       <c r="H13" s="14" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="I13" s="15">
         <f t="shared" ref="I13:I14" si="5">I5</f>
@@ -2373,7 +2487,7 @@
         <v>814</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C14" s="15">
         <f t="shared" si="4"/>
@@ -2385,7 +2499,7 @@
         <v>854</v>
       </c>
       <c r="H14" s="14" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="I14" s="15">
         <f t="shared" si="5"/>
@@ -2398,19 +2512,19 @@
       <c r="A15" s="13">
         <v>816</v>
       </c>
-      <c r="B15" s="21" t="s">
-        <v>123</v>
-      </c>
-      <c r="C15" s="22"/>
+      <c r="B15" s="25" t="s">
+        <v>122</v>
+      </c>
+      <c r="C15" s="26"/>
       <c r="D15" s="16"/>
       <c r="E15" s="17"/>
       <c r="G15" s="13">
         <v>856</v>
       </c>
-      <c r="H15" s="21" t="s">
-        <v>123</v>
-      </c>
-      <c r="I15" s="22"/>
+      <c r="H15" s="25" t="s">
+        <v>122</v>
+      </c>
+      <c r="I15" s="26"/>
       <c r="J15" s="16"/>
       <c r="K15" s="17"/>
     </row>
@@ -2418,95 +2532,95 @@
       <c r="A16" s="13">
         <v>818</v>
       </c>
-      <c r="B16" s="20" t="s">
-        <v>128</v>
-      </c>
-      <c r="C16" s="20"/>
-      <c r="D16" s="20"/>
-      <c r="E16" s="20"/>
+      <c r="B16" s="24" t="s">
+        <v>127</v>
+      </c>
+      <c r="C16" s="24"/>
+      <c r="D16" s="24"/>
+      <c r="E16" s="24"/>
       <c r="G16" s="13">
         <v>858</v>
       </c>
-      <c r="H16" s="20" t="s">
-        <v>128</v>
-      </c>
-      <c r="I16" s="20"/>
-      <c r="J16" s="20"/>
-      <c r="K16" s="20"/>
+      <c r="H16" s="24" t="s">
+        <v>127</v>
+      </c>
+      <c r="I16" s="24"/>
+      <c r="J16" s="24"/>
+      <c r="K16" s="24"/>
     </row>
     <row r="17" spans="1:11">
       <c r="A17" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="B17" s="24" t="s">
         <v>129</v>
       </c>
-      <c r="B17" s="20" t="s">
-        <v>130</v>
-      </c>
-      <c r="C17" s="20"/>
-      <c r="D17" s="20"/>
-      <c r="E17" s="20"/>
+      <c r="C17" s="24"/>
+      <c r="D17" s="24"/>
+      <c r="E17" s="24"/>
       <c r="G17" s="13" t="s">
-        <v>144</v>
-      </c>
-      <c r="H17" s="20" t="s">
-        <v>130</v>
-      </c>
-      <c r="I17" s="20"/>
-      <c r="J17" s="20"/>
-      <c r="K17" s="20"/>
+        <v>143</v>
+      </c>
+      <c r="H17" s="24" t="s">
+        <v>129</v>
+      </c>
+      <c r="I17" s="24"/>
+      <c r="J17" s="24"/>
+      <c r="K17" s="24"/>
     </row>
     <row r="18" spans="1:11">
       <c r="A18" s="13" t="s">
-        <v>131</v>
-      </c>
-      <c r="B18" s="20" t="s">
-        <v>133</v>
-      </c>
-      <c r="C18" s="20"/>
-      <c r="D18" s="20"/>
-      <c r="E18" s="20"/>
+        <v>130</v>
+      </c>
+      <c r="B18" s="24" t="s">
+        <v>132</v>
+      </c>
+      <c r="C18" s="24"/>
+      <c r="D18" s="24"/>
+      <c r="E18" s="24"/>
       <c r="G18" s="13" t="s">
-        <v>145</v>
-      </c>
-      <c r="H18" s="20" t="s">
-        <v>133</v>
-      </c>
-      <c r="I18" s="20"/>
-      <c r="J18" s="20"/>
-      <c r="K18" s="20"/>
+        <v>144</v>
+      </c>
+      <c r="H18" s="24" t="s">
+        <v>132</v>
+      </c>
+      <c r="I18" s="24"/>
+      <c r="J18" s="24"/>
+      <c r="K18" s="24"/>
     </row>
     <row r="19" spans="1:11">
       <c r="A19" s="13" t="s">
+        <v>131</v>
+      </c>
+      <c r="B19" s="24" t="s">
         <v>132</v>
       </c>
-      <c r="B19" s="20" t="s">
-        <v>133</v>
-      </c>
-      <c r="C19" s="20"/>
-      <c r="D19" s="20"/>
-      <c r="E19" s="20"/>
+      <c r="C19" s="24"/>
+      <c r="D19" s="24"/>
+      <c r="E19" s="24"/>
       <c r="G19" s="13" t="s">
-        <v>146</v>
-      </c>
-      <c r="H19" s="20" t="s">
-        <v>133</v>
-      </c>
-      <c r="I19" s="20"/>
-      <c r="J19" s="20"/>
-      <c r="K19" s="20"/>
+        <v>145</v>
+      </c>
+      <c r="H19" s="24" t="s">
+        <v>132</v>
+      </c>
+      <c r="I19" s="24"/>
+      <c r="J19" s="24"/>
+      <c r="K19" s="24"/>
     </row>
     <row r="20" spans="1:11">
       <c r="A20" s="13">
         <v>820</v>
       </c>
       <c r="B20" s="14" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C20" s="15">
         <f>E20+1</f>
         <v>7</v>
       </c>
       <c r="D20" s="14" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E20" s="15">
         <f>E4+6</f>
@@ -2516,14 +2630,14 @@
         <v>860</v>
       </c>
       <c r="H20" s="14" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="I20" s="15">
         <f>K20+1</f>
         <v>19</v>
       </c>
       <c r="J20" s="14" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="K20" s="15">
         <f>K4+6</f>
@@ -2535,14 +2649,14 @@
         <v>822</v>
       </c>
       <c r="B21" s="14" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C21" s="15">
         <f t="shared" ref="C21:C22" si="6">C20+2</f>
         <v>9</v>
       </c>
       <c r="D21" s="14" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E21" s="15">
         <f>E20+2</f>
@@ -2552,14 +2666,14 @@
         <v>862</v>
       </c>
       <c r="H21" s="14" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="I21" s="15">
         <f t="shared" ref="I21:I22" si="7">I20+2</f>
         <v>21</v>
       </c>
       <c r="J21" s="14" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="K21" s="15">
         <f>K20+2</f>
@@ -2571,14 +2685,14 @@
         <v>824</v>
       </c>
       <c r="B22" s="14" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C22" s="15">
         <f t="shared" si="6"/>
         <v>11</v>
       </c>
       <c r="D22" s="14" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E22" s="15">
         <f>E21+2</f>
@@ -2588,14 +2702,14 @@
         <v>864</v>
       </c>
       <c r="H22" s="14" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="I22" s="15">
         <f t="shared" si="7"/>
         <v>23</v>
       </c>
       <c r="J22" s="14" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="K22" s="15">
         <f>K21+2</f>
@@ -2606,25 +2720,25 @@
       <c r="A23" s="13">
         <v>826</v>
       </c>
-      <c r="B23" s="21" t="s">
+      <c r="B23" s="25" t="s">
+        <v>122</v>
+      </c>
+      <c r="C23" s="26"/>
+      <c r="D23" s="25" t="s">
         <v>123</v>
       </c>
-      <c r="C23" s="22"/>
-      <c r="D23" s="21" t="s">
-        <v>124</v>
-      </c>
-      <c r="E23" s="22"/>
+      <c r="E23" s="26"/>
       <c r="G23" s="13">
         <v>866</v>
       </c>
-      <c r="H23" s="21" t="s">
+      <c r="H23" s="25" t="s">
+        <v>122</v>
+      </c>
+      <c r="I23" s="26"/>
+      <c r="J23" s="25" t="s">
         <v>123</v>
       </c>
-      <c r="I23" s="22"/>
-      <c r="J23" s="21" t="s">
-        <v>124</v>
-      </c>
-      <c r="K23" s="22"/>
+      <c r="K23" s="26"/>
     </row>
     <row r="24" spans="1:11">
       <c r="A24" s="13">
@@ -2633,7 +2747,7 @@
       <c r="B24" s="14"/>
       <c r="C24" s="15"/>
       <c r="D24" s="14" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E24" s="15">
         <f>E20</f>
@@ -2645,7 +2759,7 @@
       <c r="H24" s="14"/>
       <c r="I24" s="15"/>
       <c r="J24" s="14" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="K24" s="15">
         <f>K20</f>
@@ -2654,24 +2768,24 @@
     </row>
     <row r="25" spans="1:11">
       <c r="A25" s="13" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B25" s="14"/>
       <c r="C25" s="15"/>
       <c r="D25" s="14" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E25" s="15">
         <f t="shared" ref="E25:E26" si="8">E21</f>
         <v>8</v>
       </c>
       <c r="G25" s="13" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H25" s="14"/>
       <c r="I25" s="15"/>
       <c r="J25" s="14" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="K25" s="15">
         <f t="shared" ref="K25:K26" si="9">K21</f>
@@ -2680,24 +2794,24 @@
     </row>
     <row r="26" spans="1:11">
       <c r="A26" s="13" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B26" s="14"/>
       <c r="C26" s="15"/>
       <c r="D26" s="14" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E26" s="15">
         <f t="shared" si="8"/>
         <v>10</v>
       </c>
       <c r="G26" s="13" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="H26" s="14"/>
       <c r="I26" s="15"/>
       <c r="J26" s="14" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="K26" s="15">
         <f t="shared" si="9"/>
@@ -2706,30 +2820,30 @@
     </row>
     <row r="27" spans="1:11">
       <c r="A27" s="13" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B27" s="14"/>
       <c r="C27" s="15"/>
-      <c r="D27" s="21" t="s">
-        <v>124</v>
-      </c>
-      <c r="E27" s="22"/>
+      <c r="D27" s="25" t="s">
+        <v>123</v>
+      </c>
+      <c r="E27" s="26"/>
       <c r="G27" s="13" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="H27" s="14"/>
       <c r="I27" s="15"/>
-      <c r="J27" s="21" t="s">
-        <v>124</v>
-      </c>
-      <c r="K27" s="22"/>
+      <c r="J27" s="25" t="s">
+        <v>123</v>
+      </c>
+      <c r="K27" s="26"/>
     </row>
     <row r="28" spans="1:11">
       <c r="A28" s="13">
         <v>830</v>
       </c>
       <c r="B28" s="14" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C28" s="15">
         <f>C20</f>
@@ -2741,7 +2855,7 @@
         <v>870</v>
       </c>
       <c r="H28" s="14" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="I28" s="15">
         <f>I20</f>
@@ -2755,7 +2869,7 @@
         <v>832</v>
       </c>
       <c r="B29" s="14" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C29" s="15">
         <f t="shared" ref="C29:C30" si="10">C21</f>
@@ -2767,7 +2881,7 @@
         <v>872</v>
       </c>
       <c r="H29" s="14" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="I29" s="15">
         <f t="shared" ref="I29:I30" si="11">I21</f>
@@ -2781,7 +2895,7 @@
         <v>834</v>
       </c>
       <c r="B30" s="14" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C30" s="15">
         <f t="shared" si="10"/>
@@ -2793,7 +2907,7 @@
         <v>874</v>
       </c>
       <c r="H30" s="14" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="I30" s="15">
         <f t="shared" si="11"/>
@@ -2806,19 +2920,19 @@
       <c r="A31" s="13">
         <v>836</v>
       </c>
-      <c r="B31" s="21" t="s">
-        <v>123</v>
-      </c>
-      <c r="C31" s="22"/>
+      <c r="B31" s="25" t="s">
+        <v>122</v>
+      </c>
+      <c r="C31" s="26"/>
       <c r="D31" s="16"/>
       <c r="E31" s="17"/>
       <c r="G31" s="13">
         <v>876</v>
       </c>
-      <c r="H31" s="21" t="s">
-        <v>123</v>
-      </c>
-      <c r="I31" s="22"/>
+      <c r="H31" s="25" t="s">
+        <v>122</v>
+      </c>
+      <c r="I31" s="26"/>
       <c r="J31" s="16"/>
       <c r="K31" s="17"/>
     </row>
@@ -2826,96 +2940,94 @@
       <c r="A32" s="13">
         <v>838</v>
       </c>
-      <c r="B32" s="20" t="s">
-        <v>128</v>
-      </c>
-      <c r="C32" s="20"/>
-      <c r="D32" s="20"/>
-      <c r="E32" s="20"/>
+      <c r="B32" s="24" t="s">
+        <v>127</v>
+      </c>
+      <c r="C32" s="24"/>
+      <c r="D32" s="24"/>
+      <c r="E32" s="24"/>
       <c r="G32" s="13">
         <v>878</v>
       </c>
-      <c r="H32" s="20" t="s">
-        <v>128</v>
-      </c>
-      <c r="I32" s="20"/>
-      <c r="J32" s="20"/>
-      <c r="K32" s="20"/>
+      <c r="H32" s="24" t="s">
+        <v>127</v>
+      </c>
+      <c r="I32" s="24"/>
+      <c r="J32" s="24"/>
+      <c r="K32" s="24"/>
     </row>
     <row r="33" spans="1:11">
       <c r="A33" s="13" t="s">
-        <v>137</v>
-      </c>
-      <c r="B33" s="20" t="s">
-        <v>130</v>
-      </c>
-      <c r="C33" s="20"/>
-      <c r="D33" s="20"/>
-      <c r="E33" s="20"/>
+        <v>136</v>
+      </c>
+      <c r="B33" s="24" t="s">
+        <v>129</v>
+      </c>
+      <c r="C33" s="24"/>
+      <c r="D33" s="24"/>
+      <c r="E33" s="24"/>
       <c r="G33" s="13" t="s">
-        <v>150</v>
-      </c>
-      <c r="H33" s="20" t="s">
-        <v>130</v>
-      </c>
-      <c r="I33" s="20"/>
-      <c r="J33" s="20"/>
-      <c r="K33" s="20"/>
+        <v>149</v>
+      </c>
+      <c r="H33" s="24" t="s">
+        <v>129</v>
+      </c>
+      <c r="I33" s="24"/>
+      <c r="J33" s="24"/>
+      <c r="K33" s="24"/>
     </row>
     <row r="34" spans="1:11">
       <c r="A34" s="13" t="s">
-        <v>138</v>
-      </c>
-      <c r="B34" s="20" t="s">
-        <v>133</v>
-      </c>
-      <c r="C34" s="20"/>
-      <c r="D34" s="20"/>
-      <c r="E34" s="20"/>
+        <v>137</v>
+      </c>
+      <c r="B34" s="24" t="s">
+        <v>132</v>
+      </c>
+      <c r="C34" s="24"/>
+      <c r="D34" s="24"/>
+      <c r="E34" s="24"/>
       <c r="G34" s="13" t="s">
-        <v>151</v>
-      </c>
-      <c r="H34" s="20" t="s">
-        <v>133</v>
-      </c>
-      <c r="I34" s="20"/>
-      <c r="J34" s="20"/>
-      <c r="K34" s="20"/>
+        <v>150</v>
+      </c>
+      <c r="H34" s="24" t="s">
+        <v>132</v>
+      </c>
+      <c r="I34" s="24"/>
+      <c r="J34" s="24"/>
+      <c r="K34" s="24"/>
     </row>
     <row r="35" spans="1:11">
       <c r="A35" s="13" t="s">
-        <v>139</v>
-      </c>
-      <c r="B35" s="20" t="s">
-        <v>133</v>
-      </c>
-      <c r="C35" s="20"/>
-      <c r="D35" s="20"/>
-      <c r="E35" s="20"/>
+        <v>138</v>
+      </c>
+      <c r="B35" s="24" t="s">
+        <v>132</v>
+      </c>
+      <c r="C35" s="24"/>
+      <c r="D35" s="24"/>
+      <c r="E35" s="24"/>
       <c r="G35" s="13" t="s">
-        <v>152</v>
-      </c>
-      <c r="H35" s="20" t="s">
-        <v>133</v>
-      </c>
-      <c r="I35" s="20"/>
-      <c r="J35" s="20"/>
-      <c r="K35" s="20"/>
+        <v>151</v>
+      </c>
+      <c r="H35" s="24" t="s">
+        <v>132</v>
+      </c>
+      <c r="I35" s="24"/>
+      <c r="J35" s="24"/>
+      <c r="K35" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="36">
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="J3:K3"/>
     <mergeCell ref="B17:E17"/>
     <mergeCell ref="B18:E18"/>
     <mergeCell ref="B19:E19"/>
-    <mergeCell ref="H23:I23"/>
-    <mergeCell ref="J23:K23"/>
+    <mergeCell ref="B16:E16"/>
     <mergeCell ref="H7:I7"/>
     <mergeCell ref="J7:K7"/>
     <mergeCell ref="J11:K11"/>
     <mergeCell ref="H15:I15"/>
-    <mergeCell ref="B16:E16"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="J3:K3"/>
     <mergeCell ref="H34:K34"/>
     <mergeCell ref="H35:K35"/>
     <mergeCell ref="B3:C3"/>
@@ -2940,6 +3052,8 @@
     <mergeCell ref="B31:C31"/>
     <mergeCell ref="J27:K27"/>
     <mergeCell ref="H31:I31"/>
+    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="J23:K23"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Documentation of changes needed for carbon isotopes
</commit_message>
<xml_diff>
--- a/syscon_usb/DACS_V1_0_ISE/tools/dacs_memory_map.xlsx
+++ b/syscon_usb/DACS_V1_0_ISE/tools/dacs_memory_map.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="15" windowWidth="19035" windowHeight="12015" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="15" windowWidth="19035" windowHeight="12015" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="505" uniqueCount="227">
   <si>
     <t>DACS Memory Map</t>
   </si>
@@ -685,6 +685,54 @@
   </si>
   <si>
     <t>PTRHm</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SHT21 Reset Acknowledge</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> MS5607 Reset Acknowledge</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> MS5607 Config 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> MS5607 Config 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> MS5607 Config 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> MS5607 Config 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> MS5607 Config 5</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> MS5607 Config 6</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SHT21 T</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SHT21 RH</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> MS5607 D1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> MS5607 D2</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Select Error</t>
+  </si>
+  <si>
+    <t>Bit</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>HCI</t>
   </si>
 </sst>
 </file>
@@ -742,7 +790,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -791,11 +839,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
@@ -851,6 +910,29 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1280,7 +1362,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="A31" sqref="A31:C31"/>
     </sheetView>
   </sheetViews>
@@ -2263,27 +2345,29 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E28"/>
+  <dimension ref="A1:E43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="6.5703125" style="4" customWidth="1"/>
-    <col min="3" max="3" width="24.42578125" customWidth="1"/>
+    <col min="3" max="3" width="26.28515625" customWidth="1"/>
     <col min="4" max="4" width="9.140625" style="4"/>
     <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="19"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
     </row>
     <row r="2" spans="1:5">
       <c r="B2" t="s">
@@ -2452,58 +2536,65 @@
     <row r="16" spans="1:5">
       <c r="A16" s="2"/>
     </row>
-    <row r="17" spans="1:4">
-      <c r="A17" t="s">
+    <row r="17" spans="1:5">
+      <c r="A17" s="34" t="s">
         <v>194</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="B17" s="35"/>
+      <c r="C17" s="35" t="s">
         <v>204</v>
       </c>
-      <c r="D17" s="4" t="s">
+      <c r="D17" s="35" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="18" spans="1:4">
+      <c r="E17" s="35" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
       <c r="B18" s="23" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="19" spans="1:4">
+      <c r="E18" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
       <c r="B19" s="23" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:5">
       <c r="B20" s="23" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:5">
       <c r="B21" s="23" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:5">
       <c r="B22" s="23" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:5">
       <c r="B23" s="23" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:5">
       <c r="B24" s="23" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:5">
       <c r="B25" s="23" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:5">
       <c r="B26" s="23" t="s">
         <v>15</v>
       </c>
@@ -2514,7 +2605,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:5">
       <c r="B27" s="23" t="s">
         <v>157</v>
       </c>
@@ -2525,7 +2616,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:5">
       <c r="B28" s="23" t="s">
         <v>206</v>
       </c>
@@ -2533,7 +2624,122 @@
         <v>209</v>
       </c>
     </row>
+    <row r="30" spans="1:5">
+      <c r="A30" s="31" t="s">
+        <v>75</v>
+      </c>
+      <c r="B30" s="32"/>
+      <c r="C30" s="33"/>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="B31" s="29" t="s">
+        <v>224</v>
+      </c>
+      <c r="C31" s="30" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="B32" s="28">
+        <v>0</v>
+      </c>
+      <c r="C32" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3">
+      <c r="B33" s="28">
+        <v>1</v>
+      </c>
+      <c r="C33" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3">
+      <c r="B34" s="28">
+        <v>2</v>
+      </c>
+      <c r="C34" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3">
+      <c r="B35" s="28">
+        <v>3</v>
+      </c>
+      <c r="C35" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="36" spans="2:3">
+      <c r="B36" s="28">
+        <v>4</v>
+      </c>
+      <c r="C36" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="37" spans="2:3">
+      <c r="B37" s="28">
+        <v>5</v>
+      </c>
+      <c r="C37" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="38" spans="2:3">
+      <c r="B38" s="28">
+        <v>6</v>
+      </c>
+      <c r="C38" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="39" spans="2:3">
+      <c r="B39" s="28">
+        <v>7</v>
+      </c>
+      <c r="C39" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="40" spans="2:3">
+      <c r="B40" s="28">
+        <v>8</v>
+      </c>
+      <c r="C40" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="41" spans="2:3">
+      <c r="B41" s="28">
+        <v>9</v>
+      </c>
+      <c r="C41" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="42" spans="2:3">
+      <c r="B42" s="28">
+        <v>10</v>
+      </c>
+      <c r="C42" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="43" spans="2:3">
+      <c r="B43" s="28">
+        <v>11</v>
+      </c>
+      <c r="C43" t="s">
+        <v>222</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A30:C30"/>
+    <mergeCell ref="A1:E1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -2541,27 +2747,29 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E27"/>
+  <dimension ref="A1:E44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="6.5703125" style="4" customWidth="1"/>
-    <col min="3" max="3" width="24.42578125" customWidth="1"/>
+    <col min="3" max="3" width="26.85546875" customWidth="1"/>
     <col min="4" max="4" width="9.140625" style="4"/>
     <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="19"/>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="33"/>
     </row>
     <row r="2" spans="1:5">
       <c r="B2" t="s">
@@ -2730,15 +2938,18 @@
     <row r="16" spans="1:5">
       <c r="A16" s="2"/>
     </row>
-    <row r="17" spans="1:3">
-      <c r="A17" t="s">
+    <row r="17" spans="1:5">
+      <c r="A17" s="36" t="s">
         <v>194</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="B17" s="36"/>
+      <c r="C17" s="35" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="18" spans="1:3">
+      <c r="D17" s="35"/>
+      <c r="E17" s="34"/>
+    </row>
+    <row r="18" spans="1:5">
       <c r="B18" s="23" t="s">
         <v>179</v>
       </c>
@@ -2746,52 +2957,179 @@
         <v>202</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:5">
       <c r="B19" s="23" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:5">
       <c r="B20" s="23" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:5">
       <c r="B21" s="23" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:5">
       <c r="B22" s="23" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:5">
       <c r="B23" s="23" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:5">
       <c r="B24" s="23" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:5">
       <c r="B25" s="23" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:5">
       <c r="B26" s="23" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:5">
       <c r="B27" s="23" t="s">
         <v>157</v>
       </c>
     </row>
+    <row r="29" spans="1:5">
+      <c r="A29" s="31" t="s">
+        <v>75</v>
+      </c>
+      <c r="B29" s="32"/>
+      <c r="C29" s="33"/>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="B30" s="29" t="s">
+        <v>224</v>
+      </c>
+      <c r="C30" s="30" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="B31" s="28">
+        <v>0</v>
+      </c>
+      <c r="C31" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="B32" s="28">
+        <v>1</v>
+      </c>
+      <c r="C32" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3">
+      <c r="B33" s="28">
+        <v>2</v>
+      </c>
+      <c r="C33" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3">
+      <c r="B34" s="28">
+        <v>3</v>
+      </c>
+      <c r="C34" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3">
+      <c r="B35" s="28">
+        <v>4</v>
+      </c>
+      <c r="C35" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="36" spans="2:3">
+      <c r="B36" s="28">
+        <v>5</v>
+      </c>
+      <c r="C36" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="37" spans="2:3">
+      <c r="B37" s="28">
+        <v>6</v>
+      </c>
+      <c r="C37" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="38" spans="2:3">
+      <c r="B38" s="28">
+        <v>7</v>
+      </c>
+      <c r="C38" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="39" spans="2:3">
+      <c r="B39" s="28">
+        <v>8</v>
+      </c>
+      <c r="C39" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="40" spans="2:3">
+      <c r="B40" s="28">
+        <v>9</v>
+      </c>
+      <c r="C40" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="41" spans="2:3">
+      <c r="B41" s="28">
+        <v>10</v>
+      </c>
+      <c r="C41" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="42" spans="2:3">
+      <c r="B42" s="28">
+        <v>11</v>
+      </c>
+      <c r="C42" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="43" spans="2:3">
+      <c r="B43" s="28"/>
+    </row>
+    <row r="44" spans="2:3">
+      <c r="B44" s="28">
+        <v>12</v>
+      </c>
+      <c r="C44" t="s">
+        <v>223</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A29:C29"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A17:B17"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
@@ -3661,16 +3999,16 @@
     </row>
   </sheetData>
   <mergeCells count="36">
-    <mergeCell ref="B32:E32"/>
-    <mergeCell ref="B33:E33"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="H32:K32"/>
-    <mergeCell ref="H33:K33"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="J27:K27"/>
-    <mergeCell ref="H31:I31"/>
-    <mergeCell ref="H23:I23"/>
-    <mergeCell ref="J23:K23"/>
+    <mergeCell ref="B17:E17"/>
+    <mergeCell ref="B18:E18"/>
+    <mergeCell ref="B19:E19"/>
+    <mergeCell ref="B16:E16"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="J11:K11"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="J3:K3"/>
     <mergeCell ref="H34:K34"/>
     <mergeCell ref="H35:K35"/>
     <mergeCell ref="B3:C3"/>
@@ -3687,16 +4025,16 @@
     <mergeCell ref="H19:K19"/>
     <mergeCell ref="D23:E23"/>
     <mergeCell ref="D27:E27"/>
-    <mergeCell ref="J7:K7"/>
-    <mergeCell ref="J11:K11"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="J3:K3"/>
-    <mergeCell ref="B17:E17"/>
-    <mergeCell ref="B18:E18"/>
-    <mergeCell ref="B19:E19"/>
-    <mergeCell ref="B16:E16"/>
-    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="B32:E32"/>
+    <mergeCell ref="B33:E33"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="H32:K32"/>
+    <mergeCell ref="H33:K33"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="J27:K27"/>
+    <mergeCell ref="H31:I31"/>
+    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="J23:K23"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Development of LCD display interface
</commit_message>
<xml_diff>
--- a/syscon_usb/DACS_V1_0_ISE/tools/dacs_memory_map.xlsx
+++ b/syscon_usb/DACS_V1_0_ISE/tools/dacs_memory_map.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="15" windowWidth="19035" windowHeight="12015" activeTab="4"/>
+    <workbookView xWindow="120" yWindow="15" windowWidth="19035" windowHeight="12015" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -89,7 +89,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="796" uniqueCount="371">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="810" uniqueCount="378">
   <si>
     <t>DACS Memory Map</t>
   </si>
@@ -1225,6 +1225,27 @@
   </si>
   <si>
     <t>ctrlr_status(15) &lt;= '0';</t>
+  </si>
+  <si>
+    <t>102C</t>
+  </si>
+  <si>
+    <t>1100</t>
+  </si>
+  <si>
+    <t>1102</t>
+  </si>
+  <si>
+    <t>LK204</t>
+  </si>
+  <si>
+    <t>Write Character Data</t>
+  </si>
+  <si>
+    <t>Read Keypad Data</t>
+  </si>
+  <si>
+    <t>Read Switch and Status</t>
   </si>
 </sst>
 </file>
@@ -1848,10 +1869,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1997,15 +2018,29 @@
       <c r="A13" s="1" t="s">
         <v>226</v>
       </c>
+      <c r="B13" t="s">
+        <v>371</v>
+      </c>
       <c r="C13" t="s">
         <v>227</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="C14" t="s">
+        <v>374</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="A2:A4 B2 B5 B12 A8:A10 A13 A6:B6 A7:B7 A5" numberStoredAsText="1"/>
+    <ignoredError sqref="A2:A4 B2 B5 B12 A8:A10 A13:A14 A6:B6 A7:B7 A5 B14" numberStoredAsText="1"/>
   </ignoredErrors>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
@@ -2013,10 +2048,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H100"/>
+  <dimension ref="A1:H105"/>
   <sheetViews>
-    <sheetView topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="E93" sqref="E93:F96"/>
+    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="B108" sqref="B108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3149,6 +3184,46 @@
         <v>240</v>
       </c>
     </row>
+    <row r="102" spans="1:3">
+      <c r="A102" s="19" t="s">
+        <v>374</v>
+      </c>
+      <c r="B102" s="20"/>
+      <c r="C102" s="19"/>
+    </row>
+    <row r="103" spans="1:3">
+      <c r="A103" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="B103" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="C103" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3">
+      <c r="A104" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="B104" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C104" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3">
+      <c r="A105" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="B105" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C105" t="s">
+        <v>377</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="E57:F57"/>
@@ -3156,7 +3231,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="A94:A98 A32:A35 A19:A29 A69:A70" numberStoredAsText="1"/>
+    <ignoredError sqref="A94:A98 A32:A35 A19:A29 A69:A70 A103:A105" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -3981,7 +4056,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:U35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="T4" sqref="T4:U9"/>
     </sheetView>
   </sheetViews>
@@ -5262,34 +5337,16 @@
     </row>
   </sheetData>
   <mergeCells count="54">
-    <mergeCell ref="N33:Q33"/>
-    <mergeCell ref="N34:Q34"/>
-    <mergeCell ref="N35:Q35"/>
-    <mergeCell ref="N23:O23"/>
-    <mergeCell ref="P23:Q23"/>
-    <mergeCell ref="P27:Q27"/>
-    <mergeCell ref="N31:O31"/>
-    <mergeCell ref="N32:Q32"/>
-    <mergeCell ref="N15:O15"/>
-    <mergeCell ref="N16:Q16"/>
-    <mergeCell ref="N17:Q17"/>
-    <mergeCell ref="N18:Q18"/>
-    <mergeCell ref="N19:Q19"/>
-    <mergeCell ref="N3:O3"/>
-    <mergeCell ref="P3:Q3"/>
-    <mergeCell ref="N7:O7"/>
-    <mergeCell ref="P7:Q7"/>
-    <mergeCell ref="P11:Q11"/>
-    <mergeCell ref="B17:E17"/>
-    <mergeCell ref="B18:E18"/>
-    <mergeCell ref="B19:E19"/>
-    <mergeCell ref="B16:E16"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="J7:K7"/>
-    <mergeCell ref="J11:K11"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="B32:E32"/>
+    <mergeCell ref="B33:E33"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="H32:K32"/>
+    <mergeCell ref="H33:K33"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="J27:K27"/>
+    <mergeCell ref="H31:I31"/>
+    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="J23:K23"/>
     <mergeCell ref="H34:K34"/>
     <mergeCell ref="H35:K35"/>
     <mergeCell ref="B3:C3"/>
@@ -5306,16 +5363,34 @@
     <mergeCell ref="H19:K19"/>
     <mergeCell ref="D23:E23"/>
     <mergeCell ref="D27:E27"/>
-    <mergeCell ref="B32:E32"/>
-    <mergeCell ref="B33:E33"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="H32:K32"/>
-    <mergeCell ref="H33:K33"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="J27:K27"/>
-    <mergeCell ref="H31:I31"/>
-    <mergeCell ref="H23:I23"/>
-    <mergeCell ref="J23:K23"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="J11:K11"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="B17:E17"/>
+    <mergeCell ref="B18:E18"/>
+    <mergeCell ref="B19:E19"/>
+    <mergeCell ref="B16:E16"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="N3:O3"/>
+    <mergeCell ref="P3:Q3"/>
+    <mergeCell ref="N7:O7"/>
+    <mergeCell ref="P7:Q7"/>
+    <mergeCell ref="P11:Q11"/>
+    <mergeCell ref="N15:O15"/>
+    <mergeCell ref="N16:Q16"/>
+    <mergeCell ref="N17:Q17"/>
+    <mergeCell ref="N18:Q18"/>
+    <mergeCell ref="N19:Q19"/>
+    <mergeCell ref="N33:Q33"/>
+    <mergeCell ref="N34:Q34"/>
+    <mergeCell ref="N35:Q35"/>
+    <mergeCell ref="N23:O23"/>
+    <mergeCell ref="P23:Q23"/>
+    <mergeCell ref="P27:Q27"/>
+    <mergeCell ref="N31:O31"/>
+    <mergeCell ref="N32:Q32"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Moved dacs.ucf into vhdl (long overdue). Added temp_*.vhd*
</commit_message>
<xml_diff>
--- a/syscon_usb/DACS_V1_0_ISE/tools/dacs_memory_map.xlsx
+++ b/syscon_usb/DACS_V1_0_ISE/tools/dacs_memory_map.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="15" windowWidth="19035" windowHeight="12015" activeTab="4"/>
+    <workbookView xWindow="120" yWindow="15" windowWidth="19035" windowHeight="12015"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
     <author>Norton Allen</author>
   </authors>
   <commentList>
-    <comment ref="B12" authorId="0">
+    <comment ref="B13" authorId="0">
       <text>
         <r>
           <rPr>
@@ -91,7 +91,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="910" uniqueCount="437">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="968" uniqueCount="477">
   <si>
     <t>DACS Memory Map</t>
   </si>
@@ -1425,6 +1425,126 @@
   </si>
   <si>
     <t>High Word</t>
+  </si>
+  <si>
+    <t>0480</t>
+  </si>
+  <si>
+    <t>04A2</t>
+  </si>
+  <si>
+    <t>TS</t>
+  </si>
+  <si>
+    <t>Temp Sensor</t>
+  </si>
+  <si>
+    <t>480</t>
+  </si>
+  <si>
+    <t>Sensor 1 Count</t>
+  </si>
+  <si>
+    <t>482</t>
+  </si>
+  <si>
+    <t>Sensor 1 LSB</t>
+  </si>
+  <si>
+    <t>484</t>
+  </si>
+  <si>
+    <t>Sensor 1 MSB</t>
+  </si>
+  <si>
+    <t>486</t>
+  </si>
+  <si>
+    <t>488</t>
+  </si>
+  <si>
+    <t>48A</t>
+  </si>
+  <si>
+    <t>48C</t>
+  </si>
+  <si>
+    <t>48E</t>
+  </si>
+  <si>
+    <t>490</t>
+  </si>
+  <si>
+    <t>492</t>
+  </si>
+  <si>
+    <t>494</t>
+  </si>
+  <si>
+    <t>496</t>
+  </si>
+  <si>
+    <t>498</t>
+  </si>
+  <si>
+    <t>49A</t>
+  </si>
+  <si>
+    <t>49C</t>
+  </si>
+  <si>
+    <t>Sensor 2 Count</t>
+  </si>
+  <si>
+    <t>Sensor 2 LSB</t>
+  </si>
+  <si>
+    <t>Sensor 2 MSB</t>
+  </si>
+  <si>
+    <t>Sensor 3 Count</t>
+  </si>
+  <si>
+    <t>Sensor 3 LSB</t>
+  </si>
+  <si>
+    <t>Sensor 3 MSB</t>
+  </si>
+  <si>
+    <t>Sensor 4 Count</t>
+  </si>
+  <si>
+    <t>Sensor 4 LSB</t>
+  </si>
+  <si>
+    <t>Sensor 4 MSB</t>
+  </si>
+  <si>
+    <t>Sensor 5 Count</t>
+  </si>
+  <si>
+    <t>Sensor 5 LSB</t>
+  </si>
+  <si>
+    <t>Sensor 5 MSB</t>
+  </si>
+  <si>
+    <t>49E</t>
+  </si>
+  <si>
+    <t>4A0</t>
+  </si>
+  <si>
+    <t>4A2</t>
+  </si>
+  <si>
+    <t>Sensor 6 Count</t>
+  </si>
+  <si>
+    <t>Sensor 6 LSB</t>
+  </si>
+  <si>
+    <t>Sensor 6 MSB</t>
   </si>
 </sst>
 </file>
@@ -2062,10 +2182,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2165,78 +2285,89 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" t="s">
-        <v>7</v>
+        <v>437</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>438</v>
       </c>
       <c r="C9" t="s">
-        <v>14</v>
+        <v>439</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B11" t="s">
         <v>9</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C11" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11" t="s">
-        <v>13</v>
-      </c>
-      <c r="C11" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" t="s">
         <v>1</v>
       </c>
-      <c r="B12" s="22" t="s">
+      <c r="B13" s="22" t="s">
         <v>170</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C13" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
-      <c r="A13" s="22" t="s">
+    <row r="14" spans="1:4">
+      <c r="A14" s="22" t="s">
         <v>432</v>
       </c>
-      <c r="B13" s="22" t="s">
+      <c r="B14" s="22" t="s">
         <v>433</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C14" t="s">
         <v>434</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="A14" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="B14" t="s">
-        <v>371</v>
-      </c>
-      <c r="C14" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="B15" t="s">
+        <v>371</v>
+      </c>
+      <c r="C15" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="1" t="s">
         <v>372</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B16" s="1" t="s">
         <v>373</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C16" t="s">
         <v>374</v>
       </c>
     </row>
@@ -2244,7 +2375,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="A2:A4 B2 B5 B12 A8:A10 A14:A15 A6:B6 A7:B7 A5 B15" numberStoredAsText="1"/>
+    <ignoredError sqref="A2:A4 B2 B13 A10:A11 A15:A16 A5:B7 B16 A8" numberStoredAsText="1"/>
   </ignoredErrors>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
@@ -2529,10 +2660,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H115"/>
+  <dimension ref="A1:H135"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="C93" sqref="C93"/>
+    <sheetView topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="C68" sqref="C68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3022,7 +3153,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="49" spans="1:8">
+    <row r="49" spans="1:3">
       <c r="A49" s="1" t="s">
         <v>63</v>
       </c>
@@ -3033,7 +3164,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="50" spans="1:8">
+    <row r="50" spans="1:3">
       <c r="A50" s="1" t="s">
         <v>64</v>
       </c>
@@ -3044,7 +3175,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="51" spans="1:8">
+    <row r="51" spans="1:3">
       <c r="A51" s="1" t="s">
         <v>68</v>
       </c>
@@ -3055,7 +3186,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="52" spans="1:8">
+    <row r="52" spans="1:3">
       <c r="A52" s="1" t="s">
         <v>69</v>
       </c>
@@ -3066,7 +3197,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="53" spans="1:8">
+    <row r="53" spans="1:3">
       <c r="A53" s="1" t="s">
         <v>70</v>
       </c>
@@ -3077,7 +3208,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="54" spans="1:8">
+    <row r="54" spans="1:3">
       <c r="A54" s="1" t="s">
         <v>71</v>
       </c>
@@ -3088,700 +3219,908 @@
         <v>58</v>
       </c>
     </row>
-    <row r="56" spans="1:8">
+    <row r="55" spans="1:3">
+      <c r="A55" s="1"/>
+    </row>
+    <row r="56" spans="1:3">
       <c r="A56" s="19" t="s">
-        <v>14</v>
+        <v>440</v>
       </c>
       <c r="B56" s="20"/>
       <c r="C56" s="19"/>
     </row>
-    <row r="57" spans="1:8">
-      <c r="D57" s="12" t="s">
+    <row r="57" spans="1:3">
+      <c r="A57" s="1" t="s">
+        <v>441</v>
+      </c>
+      <c r="B57" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C57" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3">
+      <c r="A58" s="1" t="s">
+        <v>443</v>
+      </c>
+      <c r="B58" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C58" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3">
+      <c r="A59" s="1" t="s">
+        <v>445</v>
+      </c>
+      <c r="B59" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C59" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3">
+      <c r="A60" s="1" t="s">
+        <v>447</v>
+      </c>
+      <c r="B60" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C60" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3">
+      <c r="A61" s="1" t="s">
+        <v>448</v>
+      </c>
+      <c r="B61" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C61" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3">
+      <c r="A62" s="1" t="s">
+        <v>449</v>
+      </c>
+      <c r="B62" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C62" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3">
+      <c r="A63" s="1" t="s">
+        <v>450</v>
+      </c>
+      <c r="B63" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C63" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3">
+      <c r="A64" s="1" t="s">
+        <v>451</v>
+      </c>
+      <c r="B64" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C64" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8">
+      <c r="A65" s="1" t="s">
+        <v>452</v>
+      </c>
+      <c r="B65" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C65" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8">
+      <c r="A66" s="1" t="s">
+        <v>453</v>
+      </c>
+      <c r="B66" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C66" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8">
+      <c r="A67" s="1" t="s">
+        <v>454</v>
+      </c>
+      <c r="B67" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C67" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8">
+      <c r="A68" s="1" t="s">
+        <v>455</v>
+      </c>
+      <c r="B68" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C68" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8">
+      <c r="A69" s="1" t="s">
+        <v>456</v>
+      </c>
+      <c r="B69" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C69" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8">
+      <c r="A70" s="1" t="s">
+        <v>457</v>
+      </c>
+      <c r="B70" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C70" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8">
+      <c r="A71" s="1" t="s">
+        <v>458</v>
+      </c>
+      <c r="B71" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C71" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8">
+      <c r="A72" s="1" t="s">
+        <v>471</v>
+      </c>
+      <c r="B72" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C72" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8">
+      <c r="A73" s="1" t="s">
+        <v>472</v>
+      </c>
+      <c r="B73" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C73" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8">
+      <c r="A74" s="1" t="s">
+        <v>473</v>
+      </c>
+      <c r="B74" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C74" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8">
+      <c r="A76" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="B76" s="20"/>
+      <c r="C76" s="19"/>
+    </row>
+    <row r="77" spans="1:8">
+      <c r="D77" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="E57" s="63" t="s">
+      <c r="E77" s="63" t="s">
         <v>85</v>
       </c>
-      <c r="F57" s="63"/>
-    </row>
-    <row r="58" spans="1:8">
-      <c r="A58" s="3">
+      <c r="F77" s="63"/>
+    </row>
+    <row r="78" spans="1:8">
+      <c r="A78" s="3">
         <v>600</v>
       </c>
-      <c r="C58" t="s">
+      <c r="C78" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="59" spans="1:8">
-      <c r="A59" s="3">
+    <row r="79" spans="1:8">
+      <c r="A79" s="3">
         <v>602</v>
       </c>
-      <c r="C59" t="s">
+      <c r="C79" t="s">
         <v>76</v>
       </c>
-      <c r="F59" s="8"/>
-      <c r="G59" s="8"/>
-    </row>
-    <row r="60" spans="1:8">
-      <c r="A60" s="6">
+      <c r="F79" s="8"/>
+      <c r="G79" s="8"/>
+    </row>
+    <row r="80" spans="1:8">
+      <c r="A80" s="6">
         <v>610</v>
       </c>
-      <c r="C60" s="5" t="s">
+      <c r="C80" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="D60" s="4">
+      <c r="D80" s="4">
         <v>0</v>
       </c>
-      <c r="E60" s="10" t="s">
+      <c r="E80" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="F60" s="7" t="s">
+      <c r="F80" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="G60" s="8"/>
-      <c r="H60" s="9"/>
-    </row>
-    <row r="61" spans="1:8">
-      <c r="A61" s="6">
+      <c r="G80" s="8"/>
+      <c r="H80" s="9"/>
+    </row>
+    <row r="81" spans="1:6">
+      <c r="A81" s="6">
         <v>612</v>
       </c>
-      <c r="C61" s="5" t="s">
+      <c r="C81" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="D61" s="4">
+      <c r="D81" s="4">
         <v>0</v>
       </c>
-      <c r="E61" s="10" t="s">
+      <c r="E81" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="F61" s="7" t="s">
+      <c r="F81" s="7" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="62" spans="1:8">
-      <c r="A62" s="6">
+    <row r="82" spans="1:6">
+      <c r="A82" s="6">
         <v>614</v>
       </c>
-      <c r="C62" s="5" t="s">
+      <c r="C82" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="D62" s="4">
+      <c r="D82" s="4">
         <v>1</v>
       </c>
-      <c r="E62" s="9" t="s">
+      <c r="E82" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="F62" s="7" t="s">
+      <c r="F82" s="7" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="63" spans="1:8">
-      <c r="A63" s="6">
+    <row r="83" spans="1:6">
+      <c r="A83" s="6">
         <v>616</v>
       </c>
-      <c r="C63" s="5" t="s">
+      <c r="C83" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="D63" s="4">
+      <c r="D83" s="4">
         <v>1</v>
       </c>
-      <c r="E63" s="9" t="s">
+      <c r="E83" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="F63" s="7" t="s">
+      <c r="F83" s="7" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="64" spans="1:8">
-      <c r="A64" s="6">
+    <row r="84" spans="1:6">
+      <c r="A84" s="6">
         <v>618</v>
       </c>
-      <c r="C64" s="5" t="s">
+      <c r="C84" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="D64" s="4">
+      <c r="D84" s="4">
         <v>2</v>
       </c>
-      <c r="E64" s="9" t="s">
+      <c r="E84" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="F64" s="7" t="s">
+      <c r="F84" s="7" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="65" spans="1:6">
-      <c r="A65" s="6" t="s">
+    <row r="85" spans="1:6">
+      <c r="A85" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="C65" s="5" t="s">
+      <c r="C85" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="D65" s="4">
+      <c r="D85" s="4">
         <v>2</v>
       </c>
-      <c r="E65" s="9" t="s">
+      <c r="E85" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="F65" s="7" t="s">
+      <c r="F85" s="7" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="66" spans="1:6">
-      <c r="A66" s="6" t="s">
+    <row r="86" spans="1:6">
+      <c r="A86" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="C66" s="5" t="s">
+      <c r="C86" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="D66" s="4">
+      <c r="D86" s="4">
         <v>3</v>
       </c>
-      <c r="E66" s="9" t="s">
+      <c r="E86" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="F66" s="7" t="s">
+      <c r="F86" s="7" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="67" spans="1:6">
-      <c r="A67" s="6" t="s">
+    <row r="87" spans="1:6">
+      <c r="A87" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="C67" s="5" t="s">
+      <c r="C87" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="D67" s="4">
+      <c r="D87" s="4">
         <v>3</v>
       </c>
-      <c r="E67" s="9" t="s">
+      <c r="E87" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="F67" s="7" t="s">
+      <c r="F87" s="7" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="69" spans="1:6">
-      <c r="A69" s="3" t="s">
+    <row r="89" spans="1:6">
+      <c r="A89" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="C69" t="s">
+      <c r="C89" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="70" spans="1:6">
-      <c r="A70" s="3" t="s">
+    <row r="90" spans="1:6">
+      <c r="A90" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="C70" t="s">
+      <c r="C90" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="71" spans="1:6">
-      <c r="A71" s="6">
+    <row r="91" spans="1:6">
+      <c r="A91" s="6">
         <v>630</v>
       </c>
-      <c r="C71" s="5" t="s">
+      <c r="C91" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="D71" s="4">
+      <c r="D91" s="4">
         <v>4</v>
       </c>
-      <c r="E71" s="9" t="s">
+      <c r="E91" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="F71" s="7" t="s">
+      <c r="F91" s="7" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="72" spans="1:6">
-      <c r="A72" s="6">
+    <row r="92" spans="1:6">
+      <c r="A92" s="6">
         <v>632</v>
       </c>
-      <c r="C72" s="5" t="s">
+      <c r="C92" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="D72" s="4">
+      <c r="D92" s="4">
         <v>4</v>
       </c>
-      <c r="E72" s="9" t="s">
+      <c r="E92" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="F72" s="7" t="s">
+      <c r="F92" s="7" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="73" spans="1:6">
-      <c r="A73" s="6">
+    <row r="93" spans="1:6">
+      <c r="A93" s="6">
         <v>634</v>
       </c>
-      <c r="C73" s="5" t="s">
+      <c r="C93" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="D73" s="4">
+      <c r="D93" s="4">
         <v>5</v>
       </c>
-      <c r="E73" s="9" t="s">
+      <c r="E93" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="F73" s="7" t="s">
+      <c r="F93" s="7" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="74" spans="1:6">
-      <c r="A74" s="6">
+    <row r="94" spans="1:6">
+      <c r="A94" s="6">
         <v>636</v>
       </c>
-      <c r="C74" s="5" t="s">
+      <c r="C94" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="D74" s="4">
+      <c r="D94" s="4">
         <v>5</v>
       </c>
-      <c r="E74" s="9" t="s">
+      <c r="E94" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="F74" s="7" t="s">
+      <c r="F94" s="7" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="75" spans="1:6">
-      <c r="A75" s="6">
+    <row r="95" spans="1:6">
+      <c r="A95" s="6">
         <v>638</v>
       </c>
-      <c r="C75" s="5" t="s">
+      <c r="C95" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="D75" s="4">
+      <c r="D95" s="4">
         <v>6</v>
       </c>
-      <c r="E75" s="9" t="s">
+      <c r="E95" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="F75" s="7" t="s">
+      <c r="F95" s="7" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="76" spans="1:6">
-      <c r="A76" s="6" t="s">
+    <row r="96" spans="1:6">
+      <c r="A96" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="C76" s="5" t="s">
+      <c r="C96" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="D76" s="4">
+      <c r="D96" s="4">
         <v>6</v>
       </c>
-      <c r="E76" s="9" t="s">
+      <c r="E96" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="F76" s="7" t="s">
+      <c r="F96" s="7" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="77" spans="1:6">
-      <c r="A77" s="6" t="s">
+    <row r="97" spans="1:8">
+      <c r="A97" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="C77" s="5" t="s">
+      <c r="C97" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="D77" s="4">
+      <c r="D97" s="4">
         <v>7</v>
       </c>
-      <c r="E77" s="9" t="s">
+      <c r="E97" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="F77" s="7" t="s">
+      <c r="F97" s="7" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="78" spans="1:6">
-      <c r="A78" s="6" t="s">
+    <row r="98" spans="1:8">
+      <c r="A98" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="C78" s="5" t="s">
+      <c r="C98" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="D78" s="4">
+      <c r="D98" s="4">
         <v>7</v>
       </c>
-      <c r="E78" s="9" t="s">
+      <c r="E98" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="F78" s="7" t="s">
+      <c r="F98" s="7" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="80" spans="1:6">
-      <c r="A80" s="3">
+    <row r="100" spans="1:8">
+      <c r="A100" s="3">
         <v>640</v>
       </c>
-      <c r="C80" t="s">
+      <c r="C100" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="81" spans="1:8">
-      <c r="A81" s="3">
+    <row r="101" spans="1:8">
+      <c r="A101" s="3">
         <v>642</v>
       </c>
-      <c r="C81" t="s">
+      <c r="C101" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="82" spans="1:8">
-      <c r="A82" s="6">
+    <row r="102" spans="1:8">
+      <c r="A102" s="6">
         <v>650</v>
       </c>
-      <c r="C82" s="5" t="s">
+      <c r="C102" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="D82" s="4">
+      <c r="D102" s="4">
         <v>8</v>
       </c>
-      <c r="E82" s="9" t="s">
+      <c r="E102" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="F82" s="7" t="s">
+      <c r="F102" s="7" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="83" spans="1:8">
-      <c r="A83" s="6">
+    <row r="103" spans="1:8">
+      <c r="A103" s="6">
         <v>652</v>
       </c>
-      <c r="C83" s="5" t="s">
+      <c r="C103" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="D83" s="4">
+      <c r="D103" s="4">
         <v>8</v>
       </c>
-      <c r="E83" s="9" t="s">
+      <c r="E103" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="F83" s="7" t="s">
+      <c r="F103" s="7" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="84" spans="1:8">
-      <c r="A84" s="6">
+    <row r="104" spans="1:8">
+      <c r="A104" s="6">
         <v>654</v>
       </c>
-      <c r="C84" s="5" t="s">
+      <c r="C104" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="D84" s="4">
+      <c r="D104" s="4">
         <v>9</v>
       </c>
-      <c r="E84" s="9" t="s">
+      <c r="E104" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="F84" s="7" t="s">
+      <c r="F104" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="H84" s="9"/>
-    </row>
-    <row r="85" spans="1:8">
-      <c r="A85" s="6">
+      <c r="H104" s="9"/>
+    </row>
+    <row r="105" spans="1:8">
+      <c r="A105" s="6">
         <v>656</v>
       </c>
-      <c r="C85" s="5" t="s">
+      <c r="C105" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="D85" s="4">
+      <c r="D105" s="4">
         <v>9</v>
       </c>
-      <c r="E85" s="9" t="s">
+      <c r="E105" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="F85" s="7" t="s">
+      <c r="F105" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="H85" s="9"/>
-    </row>
-    <row r="86" spans="1:8">
-      <c r="A86" s="6">
+      <c r="H105" s="9"/>
+    </row>
+    <row r="106" spans="1:8">
+      <c r="A106" s="6">
         <v>658</v>
       </c>
-      <c r="C86" s="5" t="s">
+      <c r="C106" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="D86" s="4">
+      <c r="D106" s="4">
         <v>10</v>
       </c>
-      <c r="E86" s="9" t="s">
+      <c r="E106" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="F86" s="7" t="s">
+      <c r="F106" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="H86" s="9"/>
-    </row>
-    <row r="87" spans="1:8">
-      <c r="A87" s="6" t="s">
+      <c r="H106" s="9"/>
+    </row>
+    <row r="107" spans="1:8">
+      <c r="A107" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="C87" s="5" t="s">
+      <c r="C107" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="D87" s="4">
+      <c r="D107" s="4">
         <v>10</v>
       </c>
-      <c r="E87" s="9" t="s">
+      <c r="E107" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="F87" s="7" t="s">
+      <c r="F107" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="H87" s="9"/>
-    </row>
-    <row r="88" spans="1:8">
-      <c r="A88" s="6" t="s">
+      <c r="H107" s="9"/>
+    </row>
+    <row r="108" spans="1:8">
+      <c r="A108" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="C88" s="5" t="s">
+      <c r="C108" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="D88" s="4">
+      <c r="D108" s="4">
         <v>11</v>
       </c>
-      <c r="E88" s="11" t="s">
+      <c r="E108" s="11" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="89" spans="1:8">
-      <c r="A89" s="6" t="s">
+    <row r="109" spans="1:8">
+      <c r="A109" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="C89" s="5" t="s">
+      <c r="C109" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="D89" s="4">
+      <c r="D109" s="4">
         <v>11</v>
       </c>
-      <c r="E89" s="11" t="s">
+      <c r="E109" s="11" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="91" spans="1:8">
-      <c r="A91" s="30" t="s">
+    <row r="111" spans="1:8">
+      <c r="A111" s="30" t="s">
         <v>434</v>
       </c>
-      <c r="B91" s="20"/>
-      <c r="C91" s="19"/>
-    </row>
-    <row r="92" spans="1:8">
-      <c r="A92" s="62" t="s">
+      <c r="B111" s="20"/>
+      <c r="C111" s="19"/>
+    </row>
+    <row r="112" spans="1:8">
+      <c r="A112" s="62" t="s">
         <v>432</v>
       </c>
-      <c r="B92" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C92" t="s">
+      <c r="B112" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C112" t="s">
         <v>435</v>
       </c>
     </row>
-    <row r="93" spans="1:8">
-      <c r="A93" s="62" t="s">
+    <row r="113" spans="1:6">
+      <c r="A113" s="62" t="s">
         <v>433</v>
       </c>
-      <c r="B93" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C93" t="s">
+      <c r="B113" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C113" t="s">
         <v>436</v>
       </c>
     </row>
-    <row r="95" spans="1:8">
-      <c r="A95" s="30" t="s">
+    <row r="115" spans="1:6">
+      <c r="A115" s="30" t="s">
         <v>118</v>
       </c>
-      <c r="B95" s="20"/>
-      <c r="C95" s="19" t="s">
+      <c r="B115" s="20"/>
+      <c r="C115" s="19" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="97" spans="1:6">
-      <c r="A97" s="19" t="s">
+    <row r="117" spans="1:6">
+      <c r="A117" s="19" t="s">
         <v>227</v>
       </c>
-      <c r="B97" s="20"/>
-      <c r="C97" s="19" t="s">
+      <c r="B117" s="20"/>
+      <c r="C117" s="19" t="s">
         <v>423</v>
       </c>
-      <c r="F97" s="19" t="s">
+      <c r="F117" s="19" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="98" spans="1:6">
-      <c r="A98" s="1" t="s">
+    <row r="118" spans="1:6">
+      <c r="A118" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="B98" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C98" t="s">
+      <c r="B118" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C118" t="s">
         <v>228</v>
       </c>
-      <c r="E98">
+      <c r="E118">
         <v>1000</v>
       </c>
-      <c r="F98" t="s">
+      <c r="F118" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="99" spans="1:6">
-      <c r="A99" s="1" t="s">
+    <row r="119" spans="1:6">
+      <c r="A119" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="B99" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C99" t="s">
+      <c r="B119" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C119" t="s">
         <v>230</v>
       </c>
-      <c r="E99">
+      <c r="E119">
         <v>1010</v>
       </c>
-      <c r="F99" t="s">
+      <c r="F119" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="100" spans="1:6">
-      <c r="A100" s="1" t="s">
+    <row r="120" spans="1:6">
+      <c r="A120" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="B100" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C100" t="s">
+      <c r="B120" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C120" t="s">
         <v>232</v>
       </c>
-      <c r="E100">
+      <c r="E120">
         <v>1020</v>
       </c>
-      <c r="F100" t="s">
+      <c r="F120" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="101" spans="1:6">
-      <c r="A101" s="1" t="s">
+    <row r="121" spans="1:6">
+      <c r="A121" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="B101" s="4" t="s">
+      <c r="B121" s="4" t="s">
         <v>234</v>
       </c>
-      <c r="C101" t="s">
+      <c r="C121" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="102" spans="1:6">
-      <c r="A102" s="1" t="s">
+    <row r="122" spans="1:6">
+      <c r="A122" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="B102" s="4" t="s">
+      <c r="B122" s="4" t="s">
         <v>234</v>
       </c>
-      <c r="C102" t="s">
+      <c r="C122" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="103" spans="1:6">
-      <c r="A103" s="1" t="s">
+    <row r="123" spans="1:6">
+      <c r="A123" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="B103" s="4" t="s">
+      <c r="B123" s="4" t="s">
         <v>234</v>
       </c>
-      <c r="C103" t="s">
+      <c r="C123" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="104" spans="1:6">
-      <c r="A104" s="1" t="s">
+    <row r="124" spans="1:6">
+      <c r="A124" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="B104" s="4" t="s">
+      <c r="B124" s="4" t="s">
         <v>234</v>
       </c>
-      <c r="C104" t="s">
+      <c r="C124" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="106" spans="1:6">
-      <c r="A106" s="19" t="s">
+    <row r="126" spans="1:6">
+      <c r="A126" s="19" t="s">
         <v>374</v>
       </c>
-      <c r="B106" s="20"/>
-      <c r="C106" s="61" t="s">
+      <c r="B126" s="20"/>
+      <c r="C126" s="61" t="s">
         <v>422</v>
       </c>
     </row>
-    <row r="107" spans="1:6">
-      <c r="A107" s="58" t="s">
+    <row r="127" spans="1:6">
+      <c r="A127" s="58" t="s">
         <v>372</v>
       </c>
-      <c r="B107" s="57" t="s">
+      <c r="B127" s="57" t="s">
         <v>234</v>
       </c>
-      <c r="C107" s="45" t="s">
+      <c r="C127" s="45" t="s">
         <v>378</v>
       </c>
     </row>
-    <row r="108" spans="1:6">
-      <c r="A108" s="1" t="s">
+    <row r="128" spans="1:6">
+      <c r="A128" s="1" t="s">
         <v>373</v>
       </c>
-      <c r="B108" s="4" t="s">
+      <c r="B128" s="4" t="s">
         <v>234</v>
       </c>
-      <c r="C108" t="s">
+      <c r="C128" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="109" spans="1:6">
-      <c r="A109" s="1" t="s">
+    <row r="129" spans="1:4">
+      <c r="A129" s="1" t="s">
         <v>373</v>
       </c>
-      <c r="B109" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C109" t="s">
+      <c r="B129" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C129" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="110" spans="1:6">
-      <c r="A110" s="1" t="s">
+    <row r="130" spans="1:4">
+      <c r="A130" s="1" t="s">
         <v>379</v>
       </c>
-      <c r="B110" s="4" t="s">
+      <c r="B130" s="4" t="s">
         <v>234</v>
       </c>
-      <c r="C110" t="s">
+      <c r="C130" t="s">
         <v>380</v>
       </c>
     </row>
-    <row r="111" spans="1:6">
-      <c r="A111" s="1" t="s">
+    <row r="131" spans="1:4">
+      <c r="A131" s="1" t="s">
         <v>379</v>
       </c>
-      <c r="B111" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C111" t="s">
+      <c r="B131" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C131" t="s">
         <v>377</v>
       </c>
     </row>
-    <row r="115" spans="4:4">
-      <c r="D115" s="59"/>
+    <row r="135" spans="1:4">
+      <c r="D135" s="59"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="E57:F57"/>
+    <mergeCell ref="E77:F77"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="A98:A102 A32:A35 A19:A29 A69:A70" numberStoredAsText="1"/>
+    <ignoredError sqref="A118:A122 A32:A35 A19:A29 A89:A90" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -4583,7 +4922,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
@@ -6289,16 +6628,34 @@
     </row>
   </sheetData>
   <mergeCells count="54">
-    <mergeCell ref="B32:E32"/>
-    <mergeCell ref="B33:E33"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="H32:K32"/>
-    <mergeCell ref="H33:K33"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="J27:K27"/>
-    <mergeCell ref="H31:I31"/>
-    <mergeCell ref="H23:I23"/>
-    <mergeCell ref="J23:K23"/>
+    <mergeCell ref="N33:Q33"/>
+    <mergeCell ref="N34:Q34"/>
+    <mergeCell ref="N35:Q35"/>
+    <mergeCell ref="N23:O23"/>
+    <mergeCell ref="P23:Q23"/>
+    <mergeCell ref="P27:Q27"/>
+    <mergeCell ref="N31:O31"/>
+    <mergeCell ref="N32:Q32"/>
+    <mergeCell ref="N15:O15"/>
+    <mergeCell ref="N16:Q16"/>
+    <mergeCell ref="N17:Q17"/>
+    <mergeCell ref="N18:Q18"/>
+    <mergeCell ref="N19:Q19"/>
+    <mergeCell ref="N3:O3"/>
+    <mergeCell ref="P3:Q3"/>
+    <mergeCell ref="N7:O7"/>
+    <mergeCell ref="P7:Q7"/>
+    <mergeCell ref="P11:Q11"/>
+    <mergeCell ref="B17:E17"/>
+    <mergeCell ref="B18:E18"/>
+    <mergeCell ref="B19:E19"/>
+    <mergeCell ref="B16:E16"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="J11:K11"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="J3:K3"/>
     <mergeCell ref="H34:K34"/>
     <mergeCell ref="H35:K35"/>
     <mergeCell ref="B3:C3"/>
@@ -6315,34 +6672,16 @@
     <mergeCell ref="H19:K19"/>
     <mergeCell ref="D23:E23"/>
     <mergeCell ref="D27:E27"/>
-    <mergeCell ref="J7:K7"/>
-    <mergeCell ref="J11:K11"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="J3:K3"/>
-    <mergeCell ref="B17:E17"/>
-    <mergeCell ref="B18:E18"/>
-    <mergeCell ref="B19:E19"/>
-    <mergeCell ref="B16:E16"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="N3:O3"/>
-    <mergeCell ref="P3:Q3"/>
-    <mergeCell ref="N7:O7"/>
-    <mergeCell ref="P7:Q7"/>
-    <mergeCell ref="P11:Q11"/>
-    <mergeCell ref="N15:O15"/>
-    <mergeCell ref="N16:Q16"/>
-    <mergeCell ref="N17:Q17"/>
-    <mergeCell ref="N18:Q18"/>
-    <mergeCell ref="N19:Q19"/>
-    <mergeCell ref="N33:Q33"/>
-    <mergeCell ref="N34:Q34"/>
-    <mergeCell ref="N35:Q35"/>
-    <mergeCell ref="N23:O23"/>
-    <mergeCell ref="P23:Q23"/>
-    <mergeCell ref="P27:Q27"/>
-    <mergeCell ref="N31:O31"/>
-    <mergeCell ref="N32:Q32"/>
+    <mergeCell ref="B32:E32"/>
+    <mergeCell ref="B33:E33"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="H32:K32"/>
+    <mergeCell ref="H33:K33"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="J27:K27"/>
+    <mergeCell ref="H31:I31"/>
+    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="J23:K23"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Major reconfiguration of PDACS_HCl for flight
</commit_message>
<xml_diff>
--- a/syscon_usb/DACS_V1_0_ISE/tools/dacs_memory_map.xlsx
+++ b/syscon_usb/DACS_V1_0_ISE/tools/dacs_memory_map.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="15" windowWidth="19035" windowHeight="12015"/>
+    <workbookView xWindow="120" yWindow="15" windowWidth="19035" windowHeight="12015" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -91,7 +91,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="968" uniqueCount="477">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="972" uniqueCount="478">
   <si>
     <t>DACS Memory Map</t>
   </si>
@@ -1545,6 +1545,9 @@
   </si>
   <si>
     <t>Sensor 6 MSB</t>
+  </si>
+  <si>
+    <t>HCl</t>
   </si>
 </sst>
 </file>
@@ -2184,7 +2187,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
@@ -4922,8 +4925,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E43"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5122,9 +5125,14 @@
       <c r="D17" s="28" t="s">
         <v>206</v>
       </c>
-      <c r="E17" s="27"/>
+      <c r="E17" s="28" t="s">
+        <v>477</v>
+      </c>
     </row>
     <row r="18" spans="1:5">
+      <c r="A18">
+        <v>0</v>
+      </c>
       <c r="B18" s="23" t="s">
         <v>178</v>
       </c>
@@ -5134,8 +5142,15 @@
       <c r="D18" s="4" t="s">
         <v>175</v>
       </c>
+      <c r="E18" s="4" t="s">
+        <v>175</v>
+      </c>
     </row>
     <row r="19" spans="1:5">
+      <c r="A19">
+        <f>A18+1</f>
+        <v>1</v>
+      </c>
       <c r="B19" s="23" t="s">
         <v>194</v>
       </c>
@@ -5145,8 +5160,15 @@
       <c r="D19" s="4" t="s">
         <v>207</v>
       </c>
+      <c r="E19" s="4" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="20" spans="1:5">
+      <c r="A20">
+        <f t="shared" ref="A20:A26" si="0">A19+1</f>
+        <v>2</v>
+      </c>
       <c r="B20" s="23" t="s">
         <v>195</v>
       </c>
@@ -5156,8 +5178,15 @@
       <c r="D20" s="4" t="s">
         <v>208</v>
       </c>
+      <c r="E20" s="4" t="s">
+        <v>208</v>
+      </c>
     </row>
     <row r="21" spans="1:5">
+      <c r="A21">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
       <c r="B21" s="23" t="s">
         <v>196</v>
       </c>
@@ -5166,6 +5195,10 @@
       </c>
     </row>
     <row r="22" spans="1:5">
+      <c r="A22">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
       <c r="B22" s="23" t="s">
         <v>197</v>
       </c>
@@ -5174,6 +5207,10 @@
       </c>
     </row>
     <row r="23" spans="1:5">
+      <c r="A23">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
       <c r="B23" s="23" t="s">
         <v>198</v>
       </c>
@@ -5182,6 +5219,10 @@
       </c>
     </row>
     <row r="24" spans="1:5">
+      <c r="A24">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
       <c r="B24" s="23" t="s">
         <v>199</v>
       </c>
@@ -5190,6 +5231,10 @@
       </c>
     </row>
     <row r="25" spans="1:5">
+      <c r="A25">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
       <c r="B25" s="23" t="s">
         <v>200</v>
       </c>
@@ -5198,6 +5243,10 @@
       </c>
     </row>
     <row r="26" spans="1:5">
+      <c r="A26">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
       <c r="B26" s="23" t="s">
         <v>15</v>
       </c>
@@ -6628,34 +6677,16 @@
     </row>
   </sheetData>
   <mergeCells count="54">
-    <mergeCell ref="N33:Q33"/>
-    <mergeCell ref="N34:Q34"/>
-    <mergeCell ref="N35:Q35"/>
-    <mergeCell ref="N23:O23"/>
-    <mergeCell ref="P23:Q23"/>
-    <mergeCell ref="P27:Q27"/>
-    <mergeCell ref="N31:O31"/>
-    <mergeCell ref="N32:Q32"/>
-    <mergeCell ref="N15:O15"/>
-    <mergeCell ref="N16:Q16"/>
-    <mergeCell ref="N17:Q17"/>
-    <mergeCell ref="N18:Q18"/>
-    <mergeCell ref="N19:Q19"/>
-    <mergeCell ref="N3:O3"/>
-    <mergeCell ref="P3:Q3"/>
-    <mergeCell ref="N7:O7"/>
-    <mergeCell ref="P7:Q7"/>
-    <mergeCell ref="P11:Q11"/>
-    <mergeCell ref="B17:E17"/>
-    <mergeCell ref="B18:E18"/>
-    <mergeCell ref="B19:E19"/>
-    <mergeCell ref="B16:E16"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="J7:K7"/>
-    <mergeCell ref="J11:K11"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="B32:E32"/>
+    <mergeCell ref="B33:E33"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="H32:K32"/>
+    <mergeCell ref="H33:K33"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="J27:K27"/>
+    <mergeCell ref="H31:I31"/>
+    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="J23:K23"/>
     <mergeCell ref="H34:K34"/>
     <mergeCell ref="H35:K35"/>
     <mergeCell ref="B3:C3"/>
@@ -6672,16 +6703,34 @@
     <mergeCell ref="H19:K19"/>
     <mergeCell ref="D23:E23"/>
     <mergeCell ref="D27:E27"/>
-    <mergeCell ref="B32:E32"/>
-    <mergeCell ref="B33:E33"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="H32:K32"/>
-    <mergeCell ref="H33:K33"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="J27:K27"/>
-    <mergeCell ref="H31:I31"/>
-    <mergeCell ref="H23:I23"/>
-    <mergeCell ref="J23:K23"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="J11:K11"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="B17:E17"/>
+    <mergeCell ref="B18:E18"/>
+    <mergeCell ref="B19:E19"/>
+    <mergeCell ref="B16:E16"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="N3:O3"/>
+    <mergeCell ref="P3:Q3"/>
+    <mergeCell ref="N7:O7"/>
+    <mergeCell ref="P7:Q7"/>
+    <mergeCell ref="P11:Q11"/>
+    <mergeCell ref="N15:O15"/>
+    <mergeCell ref="N16:Q16"/>
+    <mergeCell ref="N17:Q17"/>
+    <mergeCell ref="N18:Q18"/>
+    <mergeCell ref="N19:Q19"/>
+    <mergeCell ref="N33:Q33"/>
+    <mergeCell ref="N34:Q34"/>
+    <mergeCell ref="N35:Q35"/>
+    <mergeCell ref="N23:O23"/>
+    <mergeCell ref="P23:Q23"/>
+    <mergeCell ref="P27:Q27"/>
+    <mergeCell ref="N31:O31"/>
+    <mergeCell ref="N32:Q32"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Temp Sensor: Always reinit if not responsive General repo cleanup
</commit_message>
<xml_diff>
--- a/syscon_usb/DACS_V1_0_ISE/tools/dacs_memory_map.xlsx
+++ b/syscon_usb/DACS_V1_0_ISE/tools/dacs_memory_map.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="15" windowWidth="19035" windowHeight="12015" activeTab="4"/>
+    <workbookView xWindow="120" yWindow="15" windowWidth="19035" windowHeight="12015" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -91,7 +91,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="972" uniqueCount="478">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="973" uniqueCount="479">
   <si>
     <t>DACS Memory Map</t>
   </si>
@@ -1548,6 +1548,9 @@
   </si>
   <si>
     <t>HCl</t>
+  </si>
+  <si>
+    <t>Each DACS VM interface supports two power monitor boards configured at I2C addresses D0 and D2 respectively. Each board reports a single V/I pair.</t>
   </si>
 </sst>
 </file>
@@ -1732,7 +1735,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
@@ -1854,6 +1857,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1890,6 +1896,9 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3441,10 +3450,10 @@
       <c r="D77" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="E77" s="63" t="s">
+      <c r="E77" s="64" t="s">
         <v>85</v>
       </c>
-      <c r="F77" s="63"/>
+      <c r="F77" s="64"/>
     </row>
     <row r="78" spans="1:8">
       <c r="A78" s="3">
@@ -4145,29 +4154,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21">
-      <c r="A1" s="64" t="s">
+      <c r="A1" s="65" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="64"/>
-      <c r="C1" s="64"/>
-      <c r="D1" s="64"/>
-      <c r="E1" s="64"/>
-      <c r="F1" s="64"/>
-      <c r="G1" s="64"/>
-      <c r="H1" s="64"/>
-      <c r="I1" s="64"/>
-      <c r="J1" s="64"/>
-      <c r="K1" s="64"/>
-      <c r="L1" s="64"/>
-      <c r="M1" s="64"/>
-      <c r="N1" s="64"/>
-      <c r="O1" s="64"/>
-      <c r="P1" s="64"/>
-      <c r="Q1" s="64"/>
-      <c r="R1" s="64"/>
-      <c r="S1" s="64"/>
-      <c r="T1" s="64"/>
-      <c r="U1" s="64"/>
+      <c r="B1" s="65"/>
+      <c r="C1" s="65"/>
+      <c r="D1" s="65"/>
+      <c r="E1" s="65"/>
+      <c r="F1" s="65"/>
+      <c r="G1" s="65"/>
+      <c r="H1" s="65"/>
+      <c r="I1" s="65"/>
+      <c r="J1" s="65"/>
+      <c r="K1" s="65"/>
+      <c r="L1" s="65"/>
+      <c r="M1" s="65"/>
+      <c r="N1" s="65"/>
+      <c r="O1" s="65"/>
+      <c r="P1" s="65"/>
+      <c r="Q1" s="65"/>
+      <c r="R1" s="65"/>
+      <c r="S1" s="65"/>
+      <c r="T1" s="65"/>
+      <c r="U1" s="65"/>
     </row>
     <row r="3" spans="1:21">
       <c r="B3" t="s">
@@ -4270,19 +4279,19 @@
       <c r="J6" s="60">
         <v>0</v>
       </c>
-      <c r="K6" s="65" t="s">
+      <c r="K6" s="66" t="s">
         <v>393</v>
       </c>
-      <c r="L6" s="65"/>
-      <c r="M6" s="65"/>
+      <c r="L6" s="66"/>
+      <c r="M6" s="66"/>
       <c r="N6" s="60" t="s">
         <v>394</v>
       </c>
-      <c r="O6" s="65" t="s">
+      <c r="O6" s="66" t="s">
         <v>395</v>
       </c>
-      <c r="P6" s="65"/>
-      <c r="Q6" s="65"/>
+      <c r="P6" s="66"/>
+      <c r="Q6" s="66"/>
       <c r="R6" s="60">
         <v>0</v>
       </c>
@@ -4326,19 +4335,19 @@
       <c r="J8" s="60">
         <v>1</v>
       </c>
-      <c r="K8" s="65" t="s">
+      <c r="K8" s="66" t="s">
         <v>400</v>
       </c>
-      <c r="L8" s="65"/>
-      <c r="M8" s="65"/>
+      <c r="L8" s="66"/>
+      <c r="M8" s="66"/>
       <c r="N8" s="60" t="s">
         <v>394</v>
       </c>
-      <c r="O8" s="65" t="s">
+      <c r="O8" s="66" t="s">
         <v>401</v>
       </c>
-      <c r="P8" s="65"/>
-      <c r="Q8" s="65"/>
+      <c r="P8" s="66"/>
+      <c r="Q8" s="66"/>
       <c r="R8" s="60">
         <v>0</v>
       </c>
@@ -4419,30 +4428,30 @@
       </c>
     </row>
     <row r="16" spans="1:21">
-      <c r="C16" s="65" t="s">
+      <c r="C16" s="66" t="s">
         <v>406</v>
       </c>
-      <c r="D16" s="65"/>
-      <c r="E16" s="65"/>
-      <c r="F16" s="65"/>
-      <c r="G16" s="65"/>
-      <c r="H16" s="65"/>
-      <c r="I16" s="65"/>
+      <c r="D16" s="66"/>
+      <c r="E16" s="66"/>
+      <c r="F16" s="66"/>
+      <c r="G16" s="66"/>
+      <c r="H16" s="66"/>
+      <c r="I16" s="66"/>
       <c r="J16" s="60" t="s">
         <v>407</v>
       </c>
-      <c r="K16" s="65" t="s">
+      <c r="K16" s="66" t="s">
         <v>400</v>
       </c>
-      <c r="L16" s="65"/>
-      <c r="M16" s="65"/>
-      <c r="N16" s="65" t="s">
+      <c r="L16" s="66"/>
+      <c r="M16" s="66"/>
+      <c r="N16" s="66" t="s">
         <v>405</v>
       </c>
-      <c r="O16" s="65"/>
-      <c r="P16" s="65"/>
-      <c r="Q16" s="65"/>
-      <c r="R16" s="65"/>
+      <c r="O16" s="66"/>
+      <c r="P16" s="66"/>
+      <c r="Q16" s="66"/>
+      <c r="R16" s="66"/>
       <c r="T16" t="s">
         <v>409</v>
       </c>
@@ -4472,32 +4481,32 @@
       </c>
     </row>
     <row r="22" spans="2:21">
-      <c r="C22" s="65" t="s">
+      <c r="C22" s="66" t="s">
         <v>406</v>
       </c>
-      <c r="D22" s="65"/>
-      <c r="E22" s="65"/>
-      <c r="F22" s="65"/>
-      <c r="G22" s="65" t="s">
+      <c r="D22" s="66"/>
+      <c r="E22" s="66"/>
+      <c r="F22" s="66"/>
+      <c r="G22" s="66" t="s">
         <v>415</v>
       </c>
-      <c r="H22" s="65"/>
-      <c r="I22" s="65"/>
-      <c r="J22" s="65"/>
+      <c r="H22" s="66"/>
+      <c r="I22" s="66"/>
+      <c r="J22" s="66"/>
       <c r="K22" s="60">
         <v>0</v>
       </c>
-      <c r="L22" s="65" t="s">
+      <c r="L22" s="66" t="s">
         <v>416</v>
       </c>
-      <c r="M22" s="65"/>
-      <c r="N22" s="65" t="s">
+      <c r="M22" s="66"/>
+      <c r="N22" s="66" t="s">
         <v>417</v>
       </c>
-      <c r="O22" s="65"/>
-      <c r="P22" s="65"/>
-      <c r="Q22" s="65"/>
-      <c r="R22" s="65"/>
+      <c r="O22" s="66"/>
+      <c r="P22" s="66"/>
+      <c r="Q22" s="66"/>
+      <c r="R22" s="66"/>
     </row>
   </sheetData>
   <mergeCells count="12">
@@ -4537,13 +4546,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="64" t="s">
+      <c r="A1" s="65" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="64"/>
-      <c r="C1" s="64"/>
-      <c r="D1" s="64"/>
-      <c r="E1" s="64"/>
+      <c r="B1" s="65"/>
+      <c r="C1" s="65"/>
+      <c r="D1" s="65"/>
+      <c r="E1" s="65"/>
     </row>
     <row r="2" spans="1:5">
       <c r="B2" t="s">
@@ -4801,11 +4810,11 @@
       </c>
     </row>
     <row r="30" spans="1:5">
-      <c r="A30" s="66" t="s">
+      <c r="A30" s="67" t="s">
         <v>75</v>
       </c>
-      <c r="B30" s="67"/>
-      <c r="C30" s="68"/>
+      <c r="B30" s="68"/>
+      <c r="C30" s="69"/>
     </row>
     <row r="31" spans="1:5">
       <c r="B31" s="25" t="s">
@@ -4925,7 +4934,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
@@ -4939,13 +4948,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="66" t="s">
+      <c r="A1" s="67" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="67"/>
-      <c r="C1" s="67"/>
-      <c r="D1" s="67"/>
-      <c r="E1" s="68"/>
+      <c r="B1" s="68"/>
+      <c r="C1" s="68"/>
+      <c r="D1" s="68"/>
+      <c r="E1" s="69"/>
     </row>
     <row r="2" spans="1:5">
       <c r="B2" t="s">
@@ -5115,10 +5124,10 @@
       <c r="A16" s="2"/>
     </row>
     <row r="17" spans="1:5">
-      <c r="A17" s="64" t="s">
+      <c r="A17" s="65" t="s">
         <v>193</v>
       </c>
-      <c r="B17" s="64"/>
+      <c r="B17" s="65"/>
       <c r="C17" s="28" t="s">
         <v>202</v>
       </c>
@@ -5260,11 +5269,11 @@
       </c>
     </row>
     <row r="29" spans="1:5">
-      <c r="A29" s="66" t="s">
+      <c r="A29" s="67" t="s">
         <v>75</v>
       </c>
-      <c r="B29" s="67"/>
-      <c r="C29" s="68"/>
+      <c r="B29" s="68"/>
+      <c r="C29" s="69"/>
     </row>
     <row r="30" spans="1:5">
       <c r="B30" s="25" t="s">
@@ -5423,30 +5432,30 @@
       </c>
     </row>
     <row r="3" spans="1:21">
-      <c r="B3" s="65" t="s">
+      <c r="B3" s="66" t="s">
         <v>120</v>
       </c>
-      <c r="C3" s="65"/>
-      <c r="D3" s="65" t="s">
+      <c r="C3" s="66"/>
+      <c r="D3" s="66" t="s">
         <v>121</v>
       </c>
-      <c r="E3" s="65"/>
-      <c r="H3" s="65" t="s">
+      <c r="E3" s="66"/>
+      <c r="H3" s="66" t="s">
         <v>120</v>
       </c>
-      <c r="I3" s="65"/>
-      <c r="J3" s="65" t="s">
+      <c r="I3" s="66"/>
+      <c r="J3" s="66" t="s">
         <v>121</v>
       </c>
-      <c r="K3" s="65"/>
-      <c r="N3" s="65" t="s">
+      <c r="K3" s="66"/>
+      <c r="N3" s="66" t="s">
         <v>120</v>
       </c>
-      <c r="O3" s="65"/>
-      <c r="P3" s="65" t="s">
+      <c r="O3" s="66"/>
+      <c r="P3" s="66" t="s">
         <v>121</v>
       </c>
-      <c r="Q3" s="65"/>
+      <c r="Q3" s="66"/>
     </row>
     <row r="4" spans="1:21">
       <c r="A4" s="13">
@@ -5628,36 +5637,36 @@
       <c r="A7" s="13">
         <v>806</v>
       </c>
-      <c r="B7" s="69" t="s">
+      <c r="B7" s="70" t="s">
         <v>122</v>
       </c>
-      <c r="C7" s="70"/>
-      <c r="D7" s="69" t="s">
+      <c r="C7" s="71"/>
+      <c r="D7" s="70" t="s">
         <v>123</v>
       </c>
-      <c r="E7" s="70"/>
+      <c r="E7" s="71"/>
       <c r="G7" s="13">
         <v>846</v>
       </c>
-      <c r="H7" s="69" t="s">
+      <c r="H7" s="70" t="s">
         <v>122</v>
       </c>
-      <c r="I7" s="70"/>
-      <c r="J7" s="69" t="s">
+      <c r="I7" s="71"/>
+      <c r="J7" s="70" t="s">
         <v>123</v>
       </c>
-      <c r="K7" s="70"/>
+      <c r="K7" s="71"/>
       <c r="M7" s="13">
         <v>886</v>
       </c>
-      <c r="N7" s="69" t="s">
+      <c r="N7" s="70" t="s">
         <v>122</v>
       </c>
-      <c r="O7" s="70"/>
-      <c r="P7" s="69" t="s">
+      <c r="O7" s="71"/>
+      <c r="P7" s="70" t="s">
         <v>123</v>
       </c>
-      <c r="Q7" s="70"/>
+      <c r="Q7" s="71"/>
       <c r="T7">
         <v>3</v>
       </c>
@@ -5797,28 +5806,28 @@
       </c>
       <c r="B11" s="14"/>
       <c r="C11" s="15"/>
-      <c r="D11" s="69" t="s">
+      <c r="D11" s="70" t="s">
         <v>123</v>
       </c>
-      <c r="E11" s="70"/>
+      <c r="E11" s="71"/>
       <c r="G11" s="13" t="s">
         <v>142</v>
       </c>
       <c r="H11" s="14"/>
       <c r="I11" s="15"/>
-      <c r="J11" s="69" t="s">
+      <c r="J11" s="70" t="s">
         <v>123</v>
       </c>
-      <c r="K11" s="70"/>
+      <c r="K11" s="71"/>
       <c r="M11" s="13" t="s">
         <v>245</v>
       </c>
       <c r="N11" s="14"/>
       <c r="O11" s="29"/>
-      <c r="P11" s="69" t="s">
+      <c r="P11" s="70" t="s">
         <v>123</v>
       </c>
-      <c r="Q11" s="70"/>
+      <c r="Q11" s="71"/>
     </row>
     <row r="12" spans="1:21">
       <c r="A12" s="13">
@@ -5938,28 +5947,28 @@
       <c r="A15" s="13">
         <v>816</v>
       </c>
-      <c r="B15" s="69" t="s">
+      <c r="B15" s="70" t="s">
         <v>122</v>
       </c>
-      <c r="C15" s="70"/>
+      <c r="C15" s="71"/>
       <c r="D15" s="16"/>
       <c r="E15" s="17"/>
       <c r="G15" s="13">
         <v>856</v>
       </c>
-      <c r="H15" s="69" t="s">
+      <c r="H15" s="70" t="s">
         <v>122</v>
       </c>
-      <c r="I15" s="70"/>
+      <c r="I15" s="71"/>
       <c r="J15" s="16"/>
       <c r="K15" s="17"/>
       <c r="M15" s="13">
         <v>896</v>
       </c>
-      <c r="N15" s="69" t="s">
+      <c r="N15" s="70" t="s">
         <v>122</v>
       </c>
-      <c r="O15" s="70"/>
+      <c r="O15" s="71"/>
       <c r="P15" s="16"/>
       <c r="Q15" s="17"/>
     </row>
@@ -5967,117 +5976,117 @@
       <c r="A16" s="13">
         <v>818</v>
       </c>
-      <c r="B16" s="65" t="s">
+      <c r="B16" s="66" t="s">
         <v>127</v>
       </c>
-      <c r="C16" s="65"/>
-      <c r="D16" s="65"/>
-      <c r="E16" s="65"/>
+      <c r="C16" s="66"/>
+      <c r="D16" s="66"/>
+      <c r="E16" s="66"/>
       <c r="G16" s="13">
         <v>858</v>
       </c>
-      <c r="H16" s="65" t="s">
+      <c r="H16" s="66" t="s">
         <v>127</v>
       </c>
-      <c r="I16" s="65"/>
-      <c r="J16" s="65"/>
-      <c r="K16" s="65"/>
+      <c r="I16" s="66"/>
+      <c r="J16" s="66"/>
+      <c r="K16" s="66"/>
       <c r="M16" s="13">
         <v>898</v>
       </c>
-      <c r="N16" s="65" t="s">
+      <c r="N16" s="66" t="s">
         <v>127</v>
       </c>
-      <c r="O16" s="65"/>
-      <c r="P16" s="65"/>
-      <c r="Q16" s="65"/>
+      <c r="O16" s="66"/>
+      <c r="P16" s="66"/>
+      <c r="Q16" s="66"/>
     </row>
     <row r="17" spans="1:17">
       <c r="A17" s="13" t="s">
         <v>128</v>
       </c>
-      <c r="B17" s="65" t="s">
+      <c r="B17" s="66" t="s">
         <v>129</v>
       </c>
-      <c r="C17" s="65"/>
-      <c r="D17" s="65"/>
-      <c r="E17" s="65"/>
+      <c r="C17" s="66"/>
+      <c r="D17" s="66"/>
+      <c r="E17" s="66"/>
       <c r="G17" s="13" t="s">
         <v>143</v>
       </c>
-      <c r="H17" s="65" t="s">
+      <c r="H17" s="66" t="s">
         <v>129</v>
       </c>
-      <c r="I17" s="65"/>
-      <c r="J17" s="65"/>
-      <c r="K17" s="65"/>
+      <c r="I17" s="66"/>
+      <c r="J17" s="66"/>
+      <c r="K17" s="66"/>
       <c r="M17" s="13" t="s">
         <v>246</v>
       </c>
-      <c r="N17" s="65" t="s">
+      <c r="N17" s="66" t="s">
         <v>129</v>
       </c>
-      <c r="O17" s="65"/>
-      <c r="P17" s="65"/>
-      <c r="Q17" s="65"/>
+      <c r="O17" s="66"/>
+      <c r="P17" s="66"/>
+      <c r="Q17" s="66"/>
     </row>
     <row r="18" spans="1:17">
       <c r="A18" s="13" t="s">
         <v>130</v>
       </c>
-      <c r="B18" s="65" t="s">
+      <c r="B18" s="66" t="s">
         <v>132</v>
       </c>
-      <c r="C18" s="65"/>
-      <c r="D18" s="65"/>
-      <c r="E18" s="65"/>
+      <c r="C18" s="66"/>
+      <c r="D18" s="66"/>
+      <c r="E18" s="66"/>
       <c r="G18" s="13" t="s">
         <v>144</v>
       </c>
-      <c r="H18" s="65" t="s">
+      <c r="H18" s="66" t="s">
         <v>132</v>
       </c>
-      <c r="I18" s="65"/>
-      <c r="J18" s="65"/>
-      <c r="K18" s="65"/>
+      <c r="I18" s="66"/>
+      <c r="J18" s="66"/>
+      <c r="K18" s="66"/>
       <c r="M18" s="13" t="s">
         <v>247</v>
       </c>
-      <c r="N18" s="65" t="s">
+      <c r="N18" s="66" t="s">
         <v>132</v>
       </c>
-      <c r="O18" s="65"/>
-      <c r="P18" s="65"/>
-      <c r="Q18" s="65"/>
+      <c r="O18" s="66"/>
+      <c r="P18" s="66"/>
+      <c r="Q18" s="66"/>
     </row>
     <row r="19" spans="1:17">
       <c r="A19" s="13" t="s">
         <v>131</v>
       </c>
-      <c r="B19" s="65" t="s">
+      <c r="B19" s="66" t="s">
         <v>132</v>
       </c>
-      <c r="C19" s="65"/>
-      <c r="D19" s="65"/>
-      <c r="E19" s="65"/>
+      <c r="C19" s="66"/>
+      <c r="D19" s="66"/>
+      <c r="E19" s="66"/>
       <c r="G19" s="13" t="s">
         <v>145</v>
       </c>
-      <c r="H19" s="65" t="s">
+      <c r="H19" s="66" t="s">
         <v>132</v>
       </c>
-      <c r="I19" s="65"/>
-      <c r="J19" s="65"/>
-      <c r="K19" s="65"/>
+      <c r="I19" s="66"/>
+      <c r="J19" s="66"/>
+      <c r="K19" s="66"/>
       <c r="M19" s="13" t="s">
         <v>248</v>
       </c>
-      <c r="N19" s="65" t="s">
+      <c r="N19" s="66" t="s">
         <v>132</v>
       </c>
-      <c r="O19" s="65"/>
-      <c r="P19" s="65"/>
-      <c r="Q19" s="65"/>
+      <c r="O19" s="66"/>
+      <c r="P19" s="66"/>
+      <c r="Q19" s="66"/>
     </row>
     <row r="20" spans="1:17">
       <c r="A20" s="13">
@@ -6242,36 +6251,36 @@
       <c r="A23" s="13">
         <v>826</v>
       </c>
-      <c r="B23" s="69" t="s">
+      <c r="B23" s="70" t="s">
         <v>122</v>
       </c>
-      <c r="C23" s="70"/>
-      <c r="D23" s="69" t="s">
+      <c r="C23" s="71"/>
+      <c r="D23" s="70" t="s">
         <v>123</v>
       </c>
-      <c r="E23" s="70"/>
+      <c r="E23" s="71"/>
       <c r="G23" s="13">
         <v>866</v>
       </c>
-      <c r="H23" s="69" t="s">
+      <c r="H23" s="70" t="s">
         <v>122</v>
       </c>
-      <c r="I23" s="70"/>
-      <c r="J23" s="69" t="s">
+      <c r="I23" s="71"/>
+      <c r="J23" s="70" t="s">
         <v>123</v>
       </c>
-      <c r="K23" s="70"/>
+      <c r="K23" s="71"/>
       <c r="M23" s="13" t="s">
         <v>252</v>
       </c>
-      <c r="N23" s="69" t="s">
+      <c r="N23" s="70" t="s">
         <v>122</v>
       </c>
-      <c r="O23" s="70"/>
-      <c r="P23" s="69" t="s">
+      <c r="O23" s="71"/>
+      <c r="P23" s="70" t="s">
         <v>123</v>
       </c>
-      <c r="Q23" s="70"/>
+      <c r="Q23" s="71"/>
     </row>
     <row r="24" spans="1:17">
       <c r="A24" s="13">
@@ -6393,28 +6402,28 @@
       </c>
       <c r="B27" s="14"/>
       <c r="C27" s="15"/>
-      <c r="D27" s="69" t="s">
+      <c r="D27" s="70" t="s">
         <v>123</v>
       </c>
-      <c r="E27" s="70"/>
+      <c r="E27" s="71"/>
       <c r="G27" s="13" t="s">
         <v>148</v>
       </c>
       <c r="H27" s="14"/>
       <c r="I27" s="15"/>
-      <c r="J27" s="69" t="s">
+      <c r="J27" s="70" t="s">
         <v>123</v>
       </c>
-      <c r="K27" s="70"/>
+      <c r="K27" s="71"/>
       <c r="M27" s="13" t="s">
         <v>256</v>
       </c>
       <c r="N27" s="14"/>
       <c r="O27" s="29"/>
-      <c r="P27" s="69" t="s">
+      <c r="P27" s="70" t="s">
         <v>123</v>
       </c>
-      <c r="Q27" s="70"/>
+      <c r="Q27" s="71"/>
     </row>
     <row r="28" spans="1:17">
       <c r="A28" s="13">
@@ -6534,28 +6543,28 @@
       <c r="A31" s="13">
         <v>836</v>
       </c>
-      <c r="B31" s="69" t="s">
+      <c r="B31" s="70" t="s">
         <v>122</v>
       </c>
-      <c r="C31" s="70"/>
+      <c r="C31" s="71"/>
       <c r="D31" s="16"/>
       <c r="E31" s="17"/>
       <c r="G31" s="13">
         <v>876</v>
       </c>
-      <c r="H31" s="69" t="s">
+      <c r="H31" s="70" t="s">
         <v>122</v>
       </c>
-      <c r="I31" s="70"/>
+      <c r="I31" s="71"/>
       <c r="J31" s="16"/>
       <c r="K31" s="17"/>
       <c r="M31" s="13" t="s">
         <v>260</v>
       </c>
-      <c r="N31" s="69" t="s">
+      <c r="N31" s="70" t="s">
         <v>122</v>
       </c>
-      <c r="O31" s="70"/>
+      <c r="O31" s="71"/>
       <c r="P31" s="16"/>
       <c r="Q31" s="17"/>
     </row>
@@ -6563,130 +6572,148 @@
       <c r="A32" s="13">
         <v>838</v>
       </c>
-      <c r="B32" s="65" t="s">
+      <c r="B32" s="66" t="s">
         <v>127</v>
       </c>
-      <c r="C32" s="65"/>
-      <c r="D32" s="65"/>
-      <c r="E32" s="65"/>
+      <c r="C32" s="66"/>
+      <c r="D32" s="66"/>
+      <c r="E32" s="66"/>
       <c r="G32" s="13">
         <v>878</v>
       </c>
-      <c r="H32" s="65" t="s">
+      <c r="H32" s="66" t="s">
         <v>127</v>
       </c>
-      <c r="I32" s="65"/>
-      <c r="J32" s="65"/>
-      <c r="K32" s="65"/>
+      <c r="I32" s="66"/>
+      <c r="J32" s="66"/>
+      <c r="K32" s="66"/>
       <c r="M32" s="13" t="s">
         <v>261</v>
       </c>
-      <c r="N32" s="65" t="s">
+      <c r="N32" s="66" t="s">
         <v>127</v>
       </c>
-      <c r="O32" s="65"/>
-      <c r="P32" s="65"/>
-      <c r="Q32" s="65"/>
+      <c r="O32" s="66"/>
+      <c r="P32" s="66"/>
+      <c r="Q32" s="66"/>
     </row>
     <row r="33" spans="1:17">
       <c r="A33" s="13" t="s">
         <v>136</v>
       </c>
-      <c r="B33" s="65" t="s">
+      <c r="B33" s="66" t="s">
         <v>129</v>
       </c>
-      <c r="C33" s="65"/>
-      <c r="D33" s="65"/>
-      <c r="E33" s="65"/>
+      <c r="C33" s="66"/>
+      <c r="D33" s="66"/>
+      <c r="E33" s="66"/>
       <c r="G33" s="13" t="s">
         <v>149</v>
       </c>
-      <c r="H33" s="65" t="s">
+      <c r="H33" s="66" t="s">
         <v>129</v>
       </c>
-      <c r="I33" s="65"/>
-      <c r="J33" s="65"/>
-      <c r="K33" s="65"/>
+      <c r="I33" s="66"/>
+      <c r="J33" s="66"/>
+      <c r="K33" s="66"/>
       <c r="M33" s="13" t="s">
         <v>262</v>
       </c>
-      <c r="N33" s="65" t="s">
+      <c r="N33" s="66" t="s">
         <v>129</v>
       </c>
-      <c r="O33" s="65"/>
-      <c r="P33" s="65"/>
-      <c r="Q33" s="65"/>
+      <c r="O33" s="66"/>
+      <c r="P33" s="66"/>
+      <c r="Q33" s="66"/>
     </row>
     <row r="34" spans="1:17">
       <c r="A34" s="13" t="s">
         <v>137</v>
       </c>
-      <c r="B34" s="65" t="s">
+      <c r="B34" s="66" t="s">
         <v>132</v>
       </c>
-      <c r="C34" s="65"/>
-      <c r="D34" s="65"/>
-      <c r="E34" s="65"/>
+      <c r="C34" s="66"/>
+      <c r="D34" s="66"/>
+      <c r="E34" s="66"/>
       <c r="G34" s="13" t="s">
         <v>150</v>
       </c>
-      <c r="H34" s="65" t="s">
+      <c r="H34" s="66" t="s">
         <v>132</v>
       </c>
-      <c r="I34" s="65"/>
-      <c r="J34" s="65"/>
-      <c r="K34" s="65"/>
+      <c r="I34" s="66"/>
+      <c r="J34" s="66"/>
+      <c r="K34" s="66"/>
       <c r="M34" s="13" t="s">
         <v>263</v>
       </c>
-      <c r="N34" s="65" t="s">
+      <c r="N34" s="66" t="s">
         <v>132</v>
       </c>
-      <c r="O34" s="65"/>
-      <c r="P34" s="65"/>
-      <c r="Q34" s="65"/>
+      <c r="O34" s="66"/>
+      <c r="P34" s="66"/>
+      <c r="Q34" s="66"/>
     </row>
     <row r="35" spans="1:17">
       <c r="A35" s="13" t="s">
         <v>138</v>
       </c>
-      <c r="B35" s="65" t="s">
+      <c r="B35" s="66" t="s">
         <v>132</v>
       </c>
-      <c r="C35" s="65"/>
-      <c r="D35" s="65"/>
-      <c r="E35" s="65"/>
+      <c r="C35" s="66"/>
+      <c r="D35" s="66"/>
+      <c r="E35" s="66"/>
       <c r="G35" s="13" t="s">
         <v>151</v>
       </c>
-      <c r="H35" s="65" t="s">
+      <c r="H35" s="66" t="s">
         <v>132</v>
       </c>
-      <c r="I35" s="65"/>
-      <c r="J35" s="65"/>
-      <c r="K35" s="65"/>
+      <c r="I35" s="66"/>
+      <c r="J35" s="66"/>
+      <c r="K35" s="66"/>
       <c r="M35" s="13" t="s">
         <v>264</v>
       </c>
-      <c r="N35" s="65" t="s">
+      <c r="N35" s="66" t="s">
         <v>132</v>
       </c>
-      <c r="O35" s="65"/>
-      <c r="P35" s="65"/>
-      <c r="Q35" s="65"/>
+      <c r="O35" s="66"/>
+      <c r="P35" s="66"/>
+      <c r="Q35" s="66"/>
     </row>
   </sheetData>
   <mergeCells count="54">
-    <mergeCell ref="B32:E32"/>
-    <mergeCell ref="B33:E33"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="H32:K32"/>
-    <mergeCell ref="H33:K33"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="J27:K27"/>
-    <mergeCell ref="H31:I31"/>
-    <mergeCell ref="H23:I23"/>
-    <mergeCell ref="J23:K23"/>
+    <mergeCell ref="N33:Q33"/>
+    <mergeCell ref="N34:Q34"/>
+    <mergeCell ref="N35:Q35"/>
+    <mergeCell ref="N23:O23"/>
+    <mergeCell ref="P23:Q23"/>
+    <mergeCell ref="P27:Q27"/>
+    <mergeCell ref="N31:O31"/>
+    <mergeCell ref="N32:Q32"/>
+    <mergeCell ref="N15:O15"/>
+    <mergeCell ref="N16:Q16"/>
+    <mergeCell ref="N17:Q17"/>
+    <mergeCell ref="N18:Q18"/>
+    <mergeCell ref="N19:Q19"/>
+    <mergeCell ref="N3:O3"/>
+    <mergeCell ref="P3:Q3"/>
+    <mergeCell ref="N7:O7"/>
+    <mergeCell ref="P7:Q7"/>
+    <mergeCell ref="P11:Q11"/>
+    <mergeCell ref="B17:E17"/>
+    <mergeCell ref="B18:E18"/>
+    <mergeCell ref="B19:E19"/>
+    <mergeCell ref="B16:E16"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="J11:K11"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="J3:K3"/>
     <mergeCell ref="H34:K34"/>
     <mergeCell ref="H35:K35"/>
     <mergeCell ref="B3:C3"/>
@@ -6703,34 +6730,16 @@
     <mergeCell ref="H19:K19"/>
     <mergeCell ref="D23:E23"/>
     <mergeCell ref="D27:E27"/>
-    <mergeCell ref="J7:K7"/>
-    <mergeCell ref="J11:K11"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="J3:K3"/>
-    <mergeCell ref="B17:E17"/>
-    <mergeCell ref="B18:E18"/>
-    <mergeCell ref="B19:E19"/>
-    <mergeCell ref="B16:E16"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="N3:O3"/>
-    <mergeCell ref="P3:Q3"/>
-    <mergeCell ref="N7:O7"/>
-    <mergeCell ref="P7:Q7"/>
-    <mergeCell ref="P11:Q11"/>
-    <mergeCell ref="N15:O15"/>
-    <mergeCell ref="N16:Q16"/>
-    <mergeCell ref="N17:Q17"/>
-    <mergeCell ref="N18:Q18"/>
-    <mergeCell ref="N19:Q19"/>
-    <mergeCell ref="N33:Q33"/>
-    <mergeCell ref="N34:Q34"/>
-    <mergeCell ref="N35:Q35"/>
-    <mergeCell ref="N23:O23"/>
-    <mergeCell ref="P23:Q23"/>
-    <mergeCell ref="P27:Q27"/>
-    <mergeCell ref="N31:O31"/>
-    <mergeCell ref="N32:Q32"/>
+    <mergeCell ref="B32:E32"/>
+    <mergeCell ref="B33:E33"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="H32:K32"/>
+    <mergeCell ref="H33:K33"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="J27:K27"/>
+    <mergeCell ref="H31:I31"/>
+    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="J23:K23"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6743,10 +6752,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P21"/>
+  <dimension ref="A1:P23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23:N23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6891,17 +6900,17 @@
       <c r="B10" t="s">
         <v>75</v>
       </c>
-      <c r="F10" s="71" t="s">
+      <c r="F10" s="72" t="s">
         <v>326</v>
       </c>
-      <c r="G10" s="71"/>
-      <c r="H10" s="71"/>
-      <c r="I10" s="71"/>
-      <c r="J10" s="71"/>
-      <c r="K10" s="71"/>
-      <c r="L10" s="71"/>
-      <c r="M10" s="71"/>
-      <c r="N10" s="71"/>
+      <c r="G10" s="72"/>
+      <c r="H10" s="72"/>
+      <c r="I10" s="72"/>
+      <c r="J10" s="72"/>
+      <c r="K10" s="72"/>
+      <c r="L10" s="72"/>
+      <c r="M10" s="72"/>
+      <c r="N10" s="72"/>
     </row>
     <row r="11" spans="1:16">
       <c r="C11" s="38" t="s">
@@ -7085,7 +7094,7 @@
       <c r="M16" s="33"/>
       <c r="N16" s="33"/>
     </row>
-    <row r="17" spans="3:14">
+    <row r="17" spans="1:14">
       <c r="C17" s="32" t="s">
         <v>283</v>
       </c>
@@ -7111,7 +7120,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="18" spans="3:14">
+    <row r="18" spans="1:14">
       <c r="G18" s="33">
         <v>5</v>
       </c>
@@ -7133,7 +7142,7 @@
       </c>
       <c r="N18" s="33"/>
     </row>
-    <row r="19" spans="3:14">
+    <row r="19" spans="1:14">
       <c r="G19" s="33">
         <v>6</v>
       </c>
@@ -7153,7 +7162,7 @@
       <c r="M19" s="33"/>
       <c r="N19" s="33"/>
     </row>
-    <row r="20" spans="3:14">
+    <row r="20" spans="1:14">
       <c r="G20" s="33">
         <v>7</v>
       </c>
@@ -7173,7 +7182,7 @@
       <c r="M20" s="33"/>
       <c r="N20" s="33"/>
     </row>
-    <row r="21" spans="3:14">
+    <row r="21" spans="1:14">
       <c r="G21" s="33">
         <v>8</v>
       </c>
@@ -7195,9 +7204,28 @@
         <v>314</v>
       </c>
     </row>
+    <row r="23" spans="1:14" s="63" customFormat="1" ht="30" customHeight="1">
+      <c r="A23" s="77" t="s">
+        <v>478</v>
+      </c>
+      <c r="B23" s="77"/>
+      <c r="C23" s="77"/>
+      <c r="D23" s="77"/>
+      <c r="E23" s="77"/>
+      <c r="F23" s="77"/>
+      <c r="G23" s="77"/>
+      <c r="H23" s="77"/>
+      <c r="I23" s="77"/>
+      <c r="J23" s="77"/>
+      <c r="K23" s="77"/>
+      <c r="L23" s="77"/>
+      <c r="M23" s="77"/>
+      <c r="N23" s="77"/>
+    </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="F10:N10"/>
+    <mergeCell ref="A23:N23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -7222,11 +7250,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="74" t="s">
+      <c r="A1" s="75" t="s">
         <v>358</v>
       </c>
-      <c r="B1" s="74"/>
-      <c r="C1" s="74"/>
+      <c r="B1" s="75"/>
+      <c r="C1" s="75"/>
     </row>
     <row r="3" spans="1:3">
       <c r="B3" s="13" t="s">
@@ -7309,11 +7337,11 @@
       </c>
     </row>
     <row r="14" spans="1:3">
-      <c r="A14" s="73" t="s">
+      <c r="A14" s="74" t="s">
         <v>343</v>
       </c>
-      <c r="B14" s="73"/>
-      <c r="C14" s="73"/>
+      <c r="B14" s="74"/>
+      <c r="C14" s="74"/>
     </row>
     <row r="15" spans="1:3">
       <c r="B15" s="35"/>
@@ -7392,7 +7420,7 @@
       </c>
     </row>
     <row r="25" spans="2:3">
-      <c r="B25" s="72" t="s">
+      <c r="B25" s="73" t="s">
         <v>344</v>
       </c>
       <c r="C25" s="51" t="s">
@@ -7400,31 +7428,31 @@
       </c>
     </row>
     <row r="26" spans="2:3">
-      <c r="B26" s="72"/>
+      <c r="B26" s="73"/>
       <c r="C26" s="52" t="s">
         <v>338</v>
       </c>
     </row>
     <row r="27" spans="2:3">
-      <c r="B27" s="72"/>
+      <c r="B27" s="73"/>
       <c r="C27" s="52" t="s">
         <v>339</v>
       </c>
     </row>
     <row r="28" spans="2:3">
-      <c r="B28" s="72"/>
+      <c r="B28" s="73"/>
       <c r="C28" s="52" t="s">
         <v>340</v>
       </c>
     </row>
     <row r="29" spans="2:3">
-      <c r="B29" s="72"/>
+      <c r="B29" s="73"/>
       <c r="C29" s="52" t="s">
         <v>341</v>
       </c>
     </row>
     <row r="30" spans="2:3">
-      <c r="B30" s="72"/>
+      <c r="B30" s="73"/>
       <c r="C30" s="53" t="s">
         <v>342</v>
       </c>
@@ -7592,11 +7620,11 @@
       </c>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" s="75" t="s">
+      <c r="A10" s="76" t="s">
         <v>228</v>
       </c>
-      <c r="B10" s="75"/>
-      <c r="C10" s="75"/>
+      <c r="B10" s="76"/>
+      <c r="C10" s="76"/>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" t="s">

</xml_diff>

<commit_message>
HCl Build 48, power monitor issues
</commit_message>
<xml_diff>
--- a/syscon_usb/DACS_V1_0_ISE/tools/dacs_memory_map.xlsx
+++ b/syscon_usb/DACS_V1_0_ISE/tools/dacs_memory_map.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="15" windowWidth="19035" windowHeight="12015" activeTab="6"/>
+    <workbookView xWindow="120" yWindow="15" windowWidth="19035" windowHeight="12015" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -91,7 +91,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="973" uniqueCount="479">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="992" uniqueCount="497">
   <si>
     <t>DACS Memory Map</t>
   </si>
@@ -1551,6 +1551,60 @@
   </si>
   <si>
     <t>Each DACS VM interface supports two power monitor boards configured at I2C addresses D0 and D2 respectively. Each board reports a single V/I pair.</t>
+  </si>
+  <si>
+    <t>4C0</t>
+  </si>
+  <si>
+    <t>4C2</t>
+  </si>
+  <si>
+    <t>4C4</t>
+  </si>
+  <si>
+    <t>4C6</t>
+  </si>
+  <si>
+    <t>4C8</t>
+  </si>
+  <si>
+    <t>4CA</t>
+  </si>
+  <si>
+    <t>4CC</t>
+  </si>
+  <si>
+    <t>4CE</t>
+  </si>
+  <si>
+    <t>4D0</t>
+  </si>
+  <si>
+    <t>4D2</t>
+  </si>
+  <si>
+    <t>4D4</t>
+  </si>
+  <si>
+    <t>4D6</t>
+  </si>
+  <si>
+    <t>4D8</t>
+  </si>
+  <si>
+    <t>4DA</t>
+  </si>
+  <si>
+    <t>4DC</t>
+  </si>
+  <si>
+    <t>4DE</t>
+  </si>
+  <si>
+    <t>4E0</t>
+  </si>
+  <si>
+    <t>4E2</t>
   </si>
 </sst>
 </file>
@@ -1735,7 +1789,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
@@ -1887,6 +1941,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1897,8 +1954,8 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2674,8 +2731,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H135"/>
   <sheetViews>
-    <sheetView topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="C68" sqref="C68"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="D56" sqref="D56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3165,7 +3222,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="49" spans="1:3">
+    <row r="49" spans="1:4">
       <c r="A49" s="1" t="s">
         <v>63</v>
       </c>
@@ -3176,7 +3233,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="50" spans="1:3">
+    <row r="50" spans="1:4">
       <c r="A50" s="1" t="s">
         <v>64</v>
       </c>
@@ -3187,7 +3244,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="51" spans="1:3">
+    <row r="51" spans="1:4">
       <c r="A51" s="1" t="s">
         <v>68</v>
       </c>
@@ -3198,7 +3255,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="52" spans="1:3">
+    <row r="52" spans="1:4">
       <c r="A52" s="1" t="s">
         <v>69</v>
       </c>
@@ -3209,7 +3266,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="53" spans="1:3">
+    <row r="53" spans="1:4">
       <c r="A53" s="1" t="s">
         <v>70</v>
       </c>
@@ -3220,7 +3277,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="54" spans="1:3">
+    <row r="54" spans="1:4">
       <c r="A54" s="1" t="s">
         <v>71</v>
       </c>
@@ -3231,17 +3288,20 @@
         <v>58</v>
       </c>
     </row>
-    <row r="55" spans="1:3">
+    <row r="55" spans="1:4">
       <c r="A55" s="1"/>
     </row>
-    <row r="56" spans="1:3">
+    <row r="56" spans="1:4">
       <c r="A56" s="19" t="s">
         <v>440</v>
       </c>
       <c r="B56" s="20"/>
       <c r="C56" s="19"/>
-    </row>
-    <row r="57" spans="1:3">
+      <c r="D56" s="4" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4">
       <c r="A57" s="1" t="s">
         <v>441</v>
       </c>
@@ -3251,8 +3311,11 @@
       <c r="C57" t="s">
         <v>442</v>
       </c>
-    </row>
-    <row r="58" spans="1:3">
+      <c r="D57" s="23" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4">
       <c r="A58" s="1" t="s">
         <v>443</v>
       </c>
@@ -3262,8 +3325,11 @@
       <c r="C58" t="s">
         <v>444</v>
       </c>
-    </row>
-    <row r="59" spans="1:3">
+      <c r="D58" s="4" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4">
       <c r="A59" s="1" t="s">
         <v>445</v>
       </c>
@@ -3273,8 +3339,11 @@
       <c r="C59" t="s">
         <v>446</v>
       </c>
-    </row>
-    <row r="60" spans="1:3">
+      <c r="D59" s="4" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4">
       <c r="A60" s="1" t="s">
         <v>447</v>
       </c>
@@ -3284,8 +3353,11 @@
       <c r="C60" t="s">
         <v>459</v>
       </c>
-    </row>
-    <row r="61" spans="1:3">
+      <c r="D60" s="4" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4">
       <c r="A61" s="1" t="s">
         <v>448</v>
       </c>
@@ -3295,8 +3367,11 @@
       <c r="C61" t="s">
         <v>460</v>
       </c>
-    </row>
-    <row r="62" spans="1:3">
+      <c r="D61" s="4" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4">
       <c r="A62" s="1" t="s">
         <v>449</v>
       </c>
@@ -3306,8 +3381,11 @@
       <c r="C62" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="63" spans="1:3">
+      <c r="D62" s="4" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4">
       <c r="A63" s="1" t="s">
         <v>450</v>
       </c>
@@ -3317,8 +3395,11 @@
       <c r="C63" t="s">
         <v>462</v>
       </c>
-    </row>
-    <row r="64" spans="1:3">
+      <c r="D63" s="4" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4">
       <c r="A64" s="1" t="s">
         <v>451</v>
       </c>
@@ -3327,6 +3408,9 @@
       </c>
       <c r="C64" t="s">
         <v>463</v>
+      </c>
+      <c r="D64" s="4" t="s">
+        <v>486</v>
       </c>
     </row>
     <row r="65" spans="1:8">
@@ -3339,6 +3423,9 @@
       <c r="C65" t="s">
         <v>464</v>
       </c>
+      <c r="D65" s="4" t="s">
+        <v>487</v>
+      </c>
     </row>
     <row r="66" spans="1:8">
       <c r="A66" s="1" t="s">
@@ -3350,6 +3437,9 @@
       <c r="C66" t="s">
         <v>465</v>
       </c>
+      <c r="D66" s="4" t="s">
+        <v>488</v>
+      </c>
     </row>
     <row r="67" spans="1:8">
       <c r="A67" s="1" t="s">
@@ -3361,6 +3451,9 @@
       <c r="C67" t="s">
         <v>466</v>
       </c>
+      <c r="D67" s="4" t="s">
+        <v>489</v>
+      </c>
     </row>
     <row r="68" spans="1:8">
       <c r="A68" s="1" t="s">
@@ -3372,6 +3465,9 @@
       <c r="C68" t="s">
         <v>467</v>
       </c>
+      <c r="D68" s="4" t="s">
+        <v>490</v>
+      </c>
     </row>
     <row r="69" spans="1:8">
       <c r="A69" s="1" t="s">
@@ -3383,6 +3479,9 @@
       <c r="C69" t="s">
         <v>468</v>
       </c>
+      <c r="D69" s="4" t="s">
+        <v>491</v>
+      </c>
     </row>
     <row r="70" spans="1:8">
       <c r="A70" s="1" t="s">
@@ -3394,6 +3493,9 @@
       <c r="C70" t="s">
         <v>469</v>
       </c>
+      <c r="D70" s="4" t="s">
+        <v>492</v>
+      </c>
     </row>
     <row r="71" spans="1:8">
       <c r="A71" s="1" t="s">
@@ -3405,6 +3507,9 @@
       <c r="C71" t="s">
         <v>470</v>
       </c>
+      <c r="D71" s="23" t="s">
+        <v>493</v>
+      </c>
     </row>
     <row r="72" spans="1:8">
       <c r="A72" s="1" t="s">
@@ -3416,6 +3521,9 @@
       <c r="C72" t="s">
         <v>474</v>
       </c>
+      <c r="D72" s="23" t="s">
+        <v>494</v>
+      </c>
     </row>
     <row r="73" spans="1:8">
       <c r="A73" s="1" t="s">
@@ -3427,6 +3535,9 @@
       <c r="C73" t="s">
         <v>475</v>
       </c>
+      <c r="D73" s="78" t="s">
+        <v>495</v>
+      </c>
     </row>
     <row r="74" spans="1:8">
       <c r="A74" s="1" t="s">
@@ -3437,6 +3548,9 @@
       </c>
       <c r="C74" t="s">
         <v>476</v>
+      </c>
+      <c r="D74" s="78" t="s">
+        <v>496</v>
       </c>
     </row>
     <row r="76" spans="1:8">
@@ -6686,34 +6800,16 @@
     </row>
   </sheetData>
   <mergeCells count="54">
-    <mergeCell ref="N33:Q33"/>
-    <mergeCell ref="N34:Q34"/>
-    <mergeCell ref="N35:Q35"/>
-    <mergeCell ref="N23:O23"/>
-    <mergeCell ref="P23:Q23"/>
-    <mergeCell ref="P27:Q27"/>
-    <mergeCell ref="N31:O31"/>
-    <mergeCell ref="N32:Q32"/>
-    <mergeCell ref="N15:O15"/>
-    <mergeCell ref="N16:Q16"/>
-    <mergeCell ref="N17:Q17"/>
-    <mergeCell ref="N18:Q18"/>
-    <mergeCell ref="N19:Q19"/>
-    <mergeCell ref="N3:O3"/>
-    <mergeCell ref="P3:Q3"/>
-    <mergeCell ref="N7:O7"/>
-    <mergeCell ref="P7:Q7"/>
-    <mergeCell ref="P11:Q11"/>
-    <mergeCell ref="B17:E17"/>
-    <mergeCell ref="B18:E18"/>
-    <mergeCell ref="B19:E19"/>
-    <mergeCell ref="B16:E16"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="J7:K7"/>
-    <mergeCell ref="J11:K11"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="B32:E32"/>
+    <mergeCell ref="B33:E33"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="H32:K32"/>
+    <mergeCell ref="H33:K33"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="J27:K27"/>
+    <mergeCell ref="H31:I31"/>
+    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="J23:K23"/>
     <mergeCell ref="H34:K34"/>
     <mergeCell ref="H35:K35"/>
     <mergeCell ref="B3:C3"/>
@@ -6730,16 +6826,34 @@
     <mergeCell ref="H19:K19"/>
     <mergeCell ref="D23:E23"/>
     <mergeCell ref="D27:E27"/>
-    <mergeCell ref="B32:E32"/>
-    <mergeCell ref="B33:E33"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="H32:K32"/>
-    <mergeCell ref="H33:K33"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="J27:K27"/>
-    <mergeCell ref="H31:I31"/>
-    <mergeCell ref="H23:I23"/>
-    <mergeCell ref="J23:K23"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="J11:K11"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="B17:E17"/>
+    <mergeCell ref="B18:E18"/>
+    <mergeCell ref="B19:E19"/>
+    <mergeCell ref="B16:E16"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="N3:O3"/>
+    <mergeCell ref="P3:Q3"/>
+    <mergeCell ref="N7:O7"/>
+    <mergeCell ref="P7:Q7"/>
+    <mergeCell ref="P11:Q11"/>
+    <mergeCell ref="N15:O15"/>
+    <mergeCell ref="N16:Q16"/>
+    <mergeCell ref="N17:Q17"/>
+    <mergeCell ref="N18:Q18"/>
+    <mergeCell ref="N19:Q19"/>
+    <mergeCell ref="N33:Q33"/>
+    <mergeCell ref="N34:Q34"/>
+    <mergeCell ref="N35:Q35"/>
+    <mergeCell ref="N23:O23"/>
+    <mergeCell ref="P23:Q23"/>
+    <mergeCell ref="P27:Q27"/>
+    <mergeCell ref="N31:O31"/>
+    <mergeCell ref="N32:Q32"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6754,7 +6868,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:P23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A23" sqref="A23:N23"/>
     </sheetView>
   </sheetViews>
@@ -7205,22 +7319,22 @@
       </c>
     </row>
     <row r="23" spans="1:14" s="63" customFormat="1" ht="30" customHeight="1">
-      <c r="A23" s="77" t="s">
+      <c r="A23" s="73" t="s">
         <v>478</v>
       </c>
-      <c r="B23" s="77"/>
-      <c r="C23" s="77"/>
-      <c r="D23" s="77"/>
-      <c r="E23" s="77"/>
-      <c r="F23" s="77"/>
-      <c r="G23" s="77"/>
-      <c r="H23" s="77"/>
-      <c r="I23" s="77"/>
-      <c r="J23" s="77"/>
-      <c r="K23" s="77"/>
-      <c r="L23" s="77"/>
-      <c r="M23" s="77"/>
-      <c r="N23" s="77"/>
+      <c r="B23" s="73"/>
+      <c r="C23" s="73"/>
+      <c r="D23" s="73"/>
+      <c r="E23" s="73"/>
+      <c r="F23" s="73"/>
+      <c r="G23" s="73"/>
+      <c r="H23" s="73"/>
+      <c r="I23" s="73"/>
+      <c r="J23" s="73"/>
+      <c r="K23" s="73"/>
+      <c r="L23" s="73"/>
+      <c r="M23" s="73"/>
+      <c r="N23" s="73"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -7250,11 +7364,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="75" t="s">
+      <c r="A1" s="76" t="s">
         <v>358</v>
       </c>
-      <c r="B1" s="75"/>
-      <c r="C1" s="75"/>
+      <c r="B1" s="76"/>
+      <c r="C1" s="76"/>
     </row>
     <row r="3" spans="1:3">
       <c r="B3" s="13" t="s">
@@ -7337,11 +7451,11 @@
       </c>
     </row>
     <row r="14" spans="1:3">
-      <c r="A14" s="74" t="s">
+      <c r="A14" s="75" t="s">
         <v>343</v>
       </c>
-      <c r="B14" s="74"/>
-      <c r="C14" s="74"/>
+      <c r="B14" s="75"/>
+      <c r="C14" s="75"/>
     </row>
     <row r="15" spans="1:3">
       <c r="B15" s="35"/>
@@ -7420,7 +7534,7 @@
       </c>
     </row>
     <row r="25" spans="2:3">
-      <c r="B25" s="73" t="s">
+      <c r="B25" s="74" t="s">
         <v>344</v>
       </c>
       <c r="C25" s="51" t="s">
@@ -7428,31 +7542,31 @@
       </c>
     </row>
     <row r="26" spans="2:3">
-      <c r="B26" s="73"/>
+      <c r="B26" s="74"/>
       <c r="C26" s="52" t="s">
         <v>338</v>
       </c>
     </row>
     <row r="27" spans="2:3">
-      <c r="B27" s="73"/>
+      <c r="B27" s="74"/>
       <c r="C27" s="52" t="s">
         <v>339</v>
       </c>
     </row>
     <row r="28" spans="2:3">
-      <c r="B28" s="73"/>
+      <c r="B28" s="74"/>
       <c r="C28" s="52" t="s">
         <v>340</v>
       </c>
     </row>
     <row r="29" spans="2:3">
-      <c r="B29" s="73"/>
+      <c r="B29" s="74"/>
       <c r="C29" s="52" t="s">
         <v>341</v>
       </c>
     </row>
     <row r="30" spans="2:3">
-      <c r="B30" s="73"/>
+      <c r="B30" s="74"/>
       <c r="C30" s="53" t="s">
         <v>342</v>
       </c>
@@ -7620,11 +7734,11 @@
       </c>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" s="76" t="s">
+      <c r="A10" s="77" t="s">
         <v>228</v>
       </c>
-      <c r="B10" s="76"/>
-      <c r="C10" s="76"/>
+      <c r="B10" s="77"/>
+      <c r="C10" s="77"/>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" t="s">

</xml_diff>

<commit_message>
PDACS_HTW editted, checked, ready for Xilinx
</commit_message>
<xml_diff>
--- a/syscon_usb/DACS_V1_0_ISE/tools/dacs_memory_map.xlsx
+++ b/syscon_usb/DACS_V1_0_ISE/tools/dacs_memory_map.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nort\Documents\Documents\SW\arp-fpga\syscon_usb\DACS_V1_0_ISE\tools\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D13C071-D9F3-4900-AA97-200DD5AEEDEF}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="15" windowWidth="19035" windowHeight="12015" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -18,17 +24,25 @@
     <sheet name="QCLICTRL" sheetId="10" r:id="rId9"/>
     <sheet name="LK204" sheetId="12" r:id="rId10"/>
   </sheets>
-  <calcPr calcId="125725" calcMode="manual"/>
+  <calcPr calcId="191029" calcMode="manual"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Norton Allen</author>
   </authors>
   <commentList>
-    <comment ref="B13" authorId="0">
+    <comment ref="B13" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -57,12 +71,12 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Norton Allen</author>
   </authors>
   <commentList>
-    <comment ref="C31" authorId="0">
+    <comment ref="C31" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0700-000001000000}">
       <text>
         <r>
           <rPr>
@@ -1433,9 +1447,6 @@
     <t>04A2</t>
   </si>
   <si>
-    <t>TS</t>
-  </si>
-  <si>
     <t>Temp Sensor</t>
   </si>
   <si>
@@ -1605,13 +1616,16 @@
   </si>
   <si>
     <t>4E2</t>
+  </si>
+  <si>
+    <t>TempSensor</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1914,6 +1928,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1954,15 +1971,20 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -2009,7 +2031,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2041,9 +2063,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2075,6 +2115,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2250,24 +2308,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="3" max="3" width="12.5703125" customWidth="1"/>
     <col min="4" max="4" width="14.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>171</v>
       </c>
@@ -2281,7 +2340,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>174</v>
       </c>
@@ -2293,7 +2352,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>361</v>
       </c>
@@ -2305,7 +2364,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>178</v>
       </c>
@@ -2316,7 +2375,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="46" t="s">
         <v>15</v>
       </c>
@@ -2330,7 +2389,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>316</v>
       </c>
@@ -2341,7 +2400,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>3</v>
       </c>
@@ -2352,7 +2411,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>437</v>
       </c>
@@ -2360,10 +2419,10 @@
         <v>438</v>
       </c>
       <c r="C9" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>6</v>
       </c>
@@ -2374,7 +2433,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>8</v>
       </c>
@@ -2385,7 +2444,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -2396,7 +2455,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>1</v>
       </c>
@@ -2407,7 +2466,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="22" t="s">
         <v>432</v>
       </c>
@@ -2418,7 +2477,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>226</v>
       </c>
@@ -2429,7 +2488,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>372</v>
       </c>
@@ -2451,19 +2510,19 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:E27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
         <v>374</v>
       </c>
@@ -2471,7 +2530,7 @@
       <c r="C1" s="19"/>
       <c r="D1" s="4"/>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="58" t="s">
         <v>372</v>
       </c>
@@ -2483,7 +2542,7 @@
       </c>
       <c r="D2" s="4"/>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>373</v>
       </c>
@@ -2497,7 +2556,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="4"/>
       <c r="D4" s="4" t="s">
@@ -2507,7 +2566,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="4"/>
       <c r="D5" s="4">
@@ -2517,12 +2576,12 @@
         <v>429</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="4"/>
       <c r="D6" s="4"/>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>373</v>
       </c>
@@ -2534,7 +2593,7 @@
       </c>
       <c r="D7" s="4"/>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>379</v>
       </c>
@@ -2548,7 +2607,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="4"/>
       <c r="D9" s="4">
@@ -2558,7 +2617,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="4"/>
       <c r="D10" s="4">
@@ -2568,7 +2627,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="4"/>
       <c r="D11" s="4">
@@ -2578,7 +2637,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="4"/>
       <c r="D12" s="4" t="s">
@@ -2588,12 +2647,12 @@
         <v>421</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="4"/>
       <c r="D13" s="4"/>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>379</v>
       </c>
@@ -2605,7 +2664,7 @@
       </c>
       <c r="D14" s="4"/>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B15" s="4"/>
       <c r="D15" s="4">
         <v>0</v>
@@ -2614,7 +2673,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B16" s="4"/>
       <c r="D16" s="4">
         <v>1</v>
@@ -2623,7 +2682,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="17" spans="2:5">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" s="4"/>
       <c r="D17" s="4">
         <v>2</v>
@@ -2632,7 +2691,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="18" spans="2:5">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18" s="4"/>
       <c r="D18" s="4">
         <v>3</v>
@@ -2641,7 +2700,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="19" spans="2:5">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19" s="4"/>
       <c r="D19" s="4">
         <v>4</v>
@@ -2650,7 +2709,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="20" spans="2:5">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20" s="4"/>
       <c r="D20" s="4">
         <v>5</v>
@@ -2659,7 +2718,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="21" spans="2:5">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21" s="4"/>
       <c r="D21" s="4">
         <v>6</v>
@@ -2668,7 +2727,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="22" spans="2:5">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B22" s="4"/>
       <c r="D22" s="4">
         <v>7</v>
@@ -2677,7 +2736,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="23" spans="2:5">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23" s="4"/>
       <c r="D23" s="59" t="s">
         <v>389</v>
@@ -2686,7 +2745,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="24" spans="2:5">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B24" s="4"/>
       <c r="D24" s="4">
         <v>8</v>
@@ -2695,7 +2754,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="25" spans="2:5">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B25" s="4"/>
       <c r="D25" s="4">
         <v>9</v>
@@ -2704,7 +2763,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="26" spans="2:5">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B26" s="4"/>
       <c r="D26" s="4">
         <v>12</v>
@@ -2713,7 +2772,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="27" spans="2:5">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B27" s="4"/>
       <c r="D27" s="4">
         <v>13</v>
@@ -2728,14 +2787,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H135"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
       <selection activeCell="D56" sqref="D56"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="6.5703125" style="4" customWidth="1"/>
     <col min="3" max="3" width="24.42578125" customWidth="1"/>
@@ -2744,14 +2803,14 @@
     <col min="6" max="6" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
         <v>16</v>
       </c>
       <c r="B1" s="20"/>
       <c r="C1" s="19"/>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>15</v>
       </c>
@@ -2762,7 +2821,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>19</v>
       </c>
@@ -2773,7 +2832,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>21</v>
       </c>
@@ -2784,7 +2843,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>23</v>
       </c>
@@ -2795,7 +2854,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>25</v>
       </c>
@@ -2806,7 +2865,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>27</v>
       </c>
@@ -2817,7 +2876,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>28</v>
       </c>
@@ -2828,7 +2887,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>29</v>
       </c>
@@ -2839,7 +2898,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>34</v>
       </c>
@@ -2850,7 +2909,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>35</v>
       </c>
@@ -2861,7 +2920,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>36</v>
       </c>
@@ -2872,7 +2931,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>37</v>
       </c>
@@ -2883,7 +2942,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>38</v>
       </c>
@@ -2894,10 +2953,10 @@
         <v>156</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>157</v>
       </c>
@@ -2908,7 +2967,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>158</v>
       </c>
@@ -2919,7 +2978,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>159</v>
       </c>
@@ -2930,7 +2989,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>160</v>
       </c>
@@ -2941,7 +3000,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>161</v>
       </c>
@@ -2952,7 +3011,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>162</v>
       </c>
@@ -2963,7 +3022,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>163</v>
       </c>
@@ -2974,7 +3033,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>164</v>
       </c>
@@ -2985,7 +3044,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>165</v>
       </c>
@@ -2996,7 +3055,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>166</v>
       </c>
@@ -3007,7 +3066,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>167</v>
       </c>
@@ -3018,7 +3077,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="28" spans="1:3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>168</v>
       </c>
@@ -3029,7 +3088,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="29" spans="1:3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>169</v>
       </c>
@@ -3040,17 +3099,17 @@
         <v>156</v>
       </c>
     </row>
-    <row r="30" spans="1:3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>
     </row>
-    <row r="31" spans="1:3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="21" t="s">
         <v>277</v>
       </c>
       <c r="B31" s="20"/>
       <c r="C31" s="19"/>
     </row>
-    <row r="32" spans="1:3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>316</v>
       </c>
@@ -3061,7 +3120,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="33" spans="1:4">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>319</v>
       </c>
@@ -3072,7 +3131,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="34" spans="1:4">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>321</v>
       </c>
@@ -3083,7 +3142,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="35" spans="1:4">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>323</v>
       </c>
@@ -3094,19 +3153,19 @@
         <v>324</v>
       </c>
     </row>
-    <row r="37" spans="1:4">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="21" t="s">
         <v>5</v>
       </c>
       <c r="B37" s="20"/>
       <c r="C37" s="19"/>
     </row>
-    <row r="38" spans="1:4">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D38" s="4" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="39" spans="1:4">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>39</v>
       </c>
@@ -3120,7 +3179,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="40" spans="1:4">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>42</v>
       </c>
@@ -3131,7 +3190,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="41" spans="1:4">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>44</v>
       </c>
@@ -3142,7 +3201,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="42" spans="1:4">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>59</v>
       </c>
@@ -3153,7 +3212,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="43" spans="1:4">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>60</v>
       </c>
@@ -3164,7 +3223,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="44" spans="1:4">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>65</v>
       </c>
@@ -3175,7 +3234,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="45" spans="1:4">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>66</v>
       </c>
@@ -3186,7 +3245,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="46" spans="1:4">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>67</v>
       </c>
@@ -3197,7 +3256,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="47" spans="1:4">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>61</v>
       </c>
@@ -3211,7 +3270,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="48" spans="1:4">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>62</v>
       </c>
@@ -3222,7 +3281,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="49" spans="1:4">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>63</v>
       </c>
@@ -3233,7 +3292,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="50" spans="1:4">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>64</v>
       </c>
@@ -3244,7 +3303,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="51" spans="1:4">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>68</v>
       </c>
@@ -3255,7 +3314,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="52" spans="1:4">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>69</v>
       </c>
@@ -3266,7 +3325,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="53" spans="1:4">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>70</v>
       </c>
@@ -3277,7 +3336,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="54" spans="1:4">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>71</v>
       </c>
@@ -3288,288 +3347,288 @@
         <v>58</v>
       </c>
     </row>
-    <row r="55" spans="1:4">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="1"/>
     </row>
-    <row r="56" spans="1:4">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="19" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="B56" s="20"/>
       <c r="C56" s="19"/>
       <c r="D56" s="4" t="s">
-        <v>477</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
+        <v>440</v>
+      </c>
+      <c r="B57" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C57" t="s">
         <v>441</v>
       </c>
-      <c r="B57" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C57" t="s">
+      <c r="D57" s="23" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
         <v>442</v>
       </c>
-      <c r="D57" s="23" t="s">
+      <c r="B58" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C58" t="s">
+        <v>443</v>
+      </c>
+      <c r="D58" s="4" t="s">
         <v>479</v>
       </c>
     </row>
-    <row r="58" spans="1:4">
-      <c r="A58" s="1" t="s">
-        <v>443</v>
-      </c>
-      <c r="B58" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C58" t="s">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
         <v>444</v>
       </c>
-      <c r="D58" s="4" t="s">
+      <c r="B59" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C59" t="s">
+        <v>445</v>
+      </c>
+      <c r="D59" s="4" t="s">
         <v>480</v>
       </c>
     </row>
-    <row r="59" spans="1:4">
-      <c r="A59" s="1" t="s">
-        <v>445</v>
-      </c>
-      <c r="B59" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C59" t="s">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
         <v>446</v>
       </c>
-      <c r="D59" s="4" t="s">
+      <c r="B60" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C60" t="s">
+        <v>458</v>
+      </c>
+      <c r="D60" s="4" t="s">
         <v>481</v>
       </c>
     </row>
-    <row r="60" spans="1:4">
-      <c r="A60" s="1" t="s">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
         <v>447</v>
       </c>
-      <c r="B60" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C60" t="s">
+      <c r="B61" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C61" t="s">
         <v>459</v>
       </c>
-      <c r="D60" s="4" t="s">
+      <c r="D61" s="4" t="s">
         <v>482</v>
       </c>
     </row>
-    <row r="61" spans="1:4">
-      <c r="A61" s="1" t="s">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" s="1" t="s">
         <v>448</v>
       </c>
-      <c r="B61" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C61" t="s">
+      <c r="B62" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C62" t="s">
         <v>460</v>
       </c>
-      <c r="D61" s="4" t="s">
+      <c r="D62" s="4" t="s">
         <v>483</v>
       </c>
     </row>
-    <row r="62" spans="1:4">
-      <c r="A62" s="1" t="s">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" s="1" t="s">
         <v>449</v>
       </c>
-      <c r="B62" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C62" t="s">
+      <c r="B63" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C63" t="s">
         <v>461</v>
       </c>
-      <c r="D62" s="4" t="s">
+      <c r="D63" s="4" t="s">
         <v>484</v>
       </c>
     </row>
-    <row r="63" spans="1:4">
-      <c r="A63" s="1" t="s">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" s="1" t="s">
         <v>450</v>
       </c>
-      <c r="B63" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C63" t="s">
+      <c r="B64" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C64" t="s">
         <v>462</v>
       </c>
-      <c r="D63" s="4" t="s">
+      <c r="D64" s="4" t="s">
         <v>485</v>
       </c>
     </row>
-    <row r="64" spans="1:4">
-      <c r="A64" s="1" t="s">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A65" s="1" t="s">
         <v>451</v>
       </c>
-      <c r="B64" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C64" t="s">
+      <c r="B65" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C65" t="s">
         <v>463</v>
       </c>
-      <c r="D64" s="4" t="s">
+      <c r="D65" s="4" t="s">
         <v>486</v>
       </c>
     </row>
-    <row r="65" spans="1:8">
-      <c r="A65" s="1" t="s">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A66" s="1" t="s">
         <v>452</v>
       </c>
-      <c r="B65" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C65" t="s">
+      <c r="B66" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C66" t="s">
         <v>464</v>
       </c>
-      <c r="D65" s="4" t="s">
+      <c r="D66" s="4" t="s">
         <v>487</v>
       </c>
     </row>
-    <row r="66" spans="1:8">
-      <c r="A66" s="1" t="s">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A67" s="1" t="s">
         <v>453</v>
       </c>
-      <c r="B66" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C66" t="s">
+      <c r="B67" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C67" t="s">
         <v>465</v>
       </c>
-      <c r="D66" s="4" t="s">
+      <c r="D67" s="4" t="s">
         <v>488</v>
       </c>
     </row>
-    <row r="67" spans="1:8">
-      <c r="A67" s="1" t="s">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A68" s="1" t="s">
         <v>454</v>
       </c>
-      <c r="B67" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C67" t="s">
+      <c r="B68" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C68" t="s">
         <v>466</v>
       </c>
-      <c r="D67" s="4" t="s">
+      <c r="D68" s="4" t="s">
         <v>489</v>
       </c>
     </row>
-    <row r="68" spans="1:8">
-      <c r="A68" s="1" t="s">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A69" s="1" t="s">
         <v>455</v>
       </c>
-      <c r="B68" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C68" t="s">
+      <c r="B69" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C69" t="s">
         <v>467</v>
       </c>
-      <c r="D68" s="4" t="s">
+      <c r="D69" s="4" t="s">
         <v>490</v>
       </c>
     </row>
-    <row r="69" spans="1:8">
-      <c r="A69" s="1" t="s">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A70" s="1" t="s">
         <v>456</v>
       </c>
-      <c r="B69" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C69" t="s">
+      <c r="B70" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C70" t="s">
         <v>468</v>
       </c>
-      <c r="D69" s="4" t="s">
+      <c r="D70" s="4" t="s">
         <v>491</v>
       </c>
     </row>
-    <row r="70" spans="1:8">
-      <c r="A70" s="1" t="s">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A71" s="1" t="s">
         <v>457</v>
       </c>
-      <c r="B70" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C70" t="s">
+      <c r="B71" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C71" t="s">
         <v>469</v>
       </c>
-      <c r="D70" s="4" t="s">
+      <c r="D71" s="23" t="s">
         <v>492</v>
       </c>
     </row>
-    <row r="71" spans="1:8">
-      <c r="A71" s="1" t="s">
-        <v>458</v>
-      </c>
-      <c r="B71" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C71" t="s">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A72" s="1" t="s">
         <v>470</v>
       </c>
-      <c r="D71" s="23" t="s">
+      <c r="B72" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C72" t="s">
+        <v>473</v>
+      </c>
+      <c r="D72" s="23" t="s">
         <v>493</v>
       </c>
     </row>
-    <row r="72" spans="1:8">
-      <c r="A72" s="1" t="s">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A73" s="1" t="s">
         <v>471</v>
       </c>
-      <c r="B72" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C72" t="s">
+      <c r="B73" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C73" t="s">
         <v>474</v>
       </c>
-      <c r="D72" s="23" t="s">
+      <c r="D73" s="64" t="s">
         <v>494</v>
       </c>
     </row>
-    <row r="73" spans="1:8">
-      <c r="A73" s="1" t="s">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A74" s="1" t="s">
         <v>472</v>
       </c>
-      <c r="B73" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C73" t="s">
+      <c r="B74" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C74" t="s">
         <v>475</v>
       </c>
-      <c r="D73" s="78" t="s">
+      <c r="D74" s="64" t="s">
         <v>495</v>
       </c>
     </row>
-    <row r="74" spans="1:8">
-      <c r="A74" s="1" t="s">
-        <v>473</v>
-      </c>
-      <c r="B74" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C74" t="s">
-        <v>476</v>
-      </c>
-      <c r="D74" s="78" t="s">
-        <v>496</v>
-      </c>
-    </row>
-    <row r="76" spans="1:8">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="19" t="s">
         <v>14</v>
       </c>
       <c r="B76" s="20"/>
       <c r="C76" s="19"/>
     </row>
-    <row r="77" spans="1:8">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D77" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="E77" s="64" t="s">
+      <c r="E77" s="65" t="s">
         <v>85</v>
       </c>
-      <c r="F77" s="64"/>
-    </row>
-    <row r="78" spans="1:8">
+      <c r="F77" s="65"/>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="3">
         <v>600</v>
       </c>
@@ -3577,7 +3636,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="79" spans="1:8">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" s="3">
         <v>602</v>
       </c>
@@ -3587,7 +3646,7 @@
       <c r="F79" s="8"/>
       <c r="G79" s="8"/>
     </row>
-    <row r="80" spans="1:8">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" s="6">
         <v>610</v>
       </c>
@@ -3606,7 +3665,7 @@
       <c r="G80" s="8"/>
       <c r="H80" s="9"/>
     </row>
-    <row r="81" spans="1:6">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" s="6">
         <v>612</v>
       </c>
@@ -3623,7 +3682,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="82" spans="1:6">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" s="6">
         <v>614</v>
       </c>
@@ -3640,7 +3699,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="83" spans="1:6">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" s="6">
         <v>616</v>
       </c>
@@ -3657,7 +3716,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="84" spans="1:6">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" s="6">
         <v>618</v>
       </c>
@@ -3674,7 +3733,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="85" spans="1:6">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" s="6" t="s">
         <v>72</v>
       </c>
@@ -3691,7 +3750,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="86" spans="1:6">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" s="6" t="s">
         <v>73</v>
       </c>
@@ -3708,7 +3767,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="87" spans="1:6">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" s="6" t="s">
         <v>74</v>
       </c>
@@ -3725,7 +3784,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="89" spans="1:6">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" s="3" t="s">
         <v>97</v>
       </c>
@@ -3733,7 +3792,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="90" spans="1:6">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" s="3" t="s">
         <v>98</v>
       </c>
@@ -3741,7 +3800,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="91" spans="1:6">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" s="6">
         <v>630</v>
       </c>
@@ -3758,7 +3817,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="92" spans="1:6">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" s="6">
         <v>632</v>
       </c>
@@ -3775,7 +3834,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="93" spans="1:6">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" s="6">
         <v>634</v>
       </c>
@@ -3792,7 +3851,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="94" spans="1:6">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" s="6">
         <v>636</v>
       </c>
@@ -3809,7 +3868,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="95" spans="1:6">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" s="6">
         <v>638</v>
       </c>
@@ -3826,7 +3885,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="96" spans="1:6">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" s="6" t="s">
         <v>99</v>
       </c>
@@ -3843,7 +3902,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="97" spans="1:8">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97" s="6" t="s">
         <v>100</v>
       </c>
@@ -3860,7 +3919,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="98" spans="1:8">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98" s="6" t="s">
         <v>101</v>
       </c>
@@ -3877,7 +3936,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="100" spans="1:8">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100" s="3">
         <v>640</v>
       </c>
@@ -3885,7 +3944,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="101" spans="1:8">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A101" s="3">
         <v>642</v>
       </c>
@@ -3893,7 +3952,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="102" spans="1:8">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A102" s="6">
         <v>650</v>
       </c>
@@ -3910,7 +3969,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="103" spans="1:8">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A103" s="6">
         <v>652</v>
       </c>
@@ -3927,7 +3986,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="104" spans="1:8">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A104" s="6">
         <v>654</v>
       </c>
@@ -3945,7 +4004,7 @@
       </c>
       <c r="H104" s="9"/>
     </row>
-    <row r="105" spans="1:8">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A105" s="6">
         <v>656</v>
       </c>
@@ -3963,7 +4022,7 @@
       </c>
       <c r="H105" s="9"/>
     </row>
-    <row r="106" spans="1:8">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A106" s="6">
         <v>658</v>
       </c>
@@ -3981,7 +4040,7 @@
       </c>
       <c r="H106" s="9"/>
     </row>
-    <row r="107" spans="1:8">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A107" s="6" t="s">
         <v>102</v>
       </c>
@@ -3999,7 +4058,7 @@
       </c>
       <c r="H107" s="9"/>
     </row>
-    <row r="108" spans="1:8">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A108" s="6" t="s">
         <v>103</v>
       </c>
@@ -4013,7 +4072,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="109" spans="1:8">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A109" s="6" t="s">
         <v>104</v>
       </c>
@@ -4027,14 +4086,14 @@
         <v>117</v>
       </c>
     </row>
-    <row r="111" spans="1:8">
+    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A111" s="30" t="s">
         <v>434</v>
       </c>
       <c r="B111" s="20"/>
       <c r="C111" s="19"/>
     </row>
-    <row r="112" spans="1:8">
+    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A112" s="62" t="s">
         <v>432</v>
       </c>
@@ -4045,7 +4104,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="113" spans="1:6">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A113" s="62" t="s">
         <v>433</v>
       </c>
@@ -4056,7 +4115,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="115" spans="1:6">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A115" s="30" t="s">
         <v>118</v>
       </c>
@@ -4065,7 +4124,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="117" spans="1:6">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A117" s="19" t="s">
         <v>227</v>
       </c>
@@ -4077,7 +4136,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="118" spans="1:6">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
         <v>226</v>
       </c>
@@ -4094,7 +4153,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="119" spans="1:6">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
         <v>229</v>
       </c>
@@ -4111,7 +4170,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="120" spans="1:6">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
         <v>231</v>
       </c>
@@ -4128,7 +4187,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="121" spans="1:6">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
         <v>233</v>
       </c>
@@ -4139,7 +4198,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="122" spans="1:6">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
         <v>236</v>
       </c>
@@ -4150,7 +4209,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="123" spans="1:6">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
         <v>238</v>
       </c>
@@ -4161,7 +4220,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="124" spans="1:6">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
         <v>239</v>
       </c>
@@ -4172,7 +4231,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="126" spans="1:6">
+    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A126" s="19" t="s">
         <v>374</v>
       </c>
@@ -4181,7 +4240,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="127" spans="1:6">
+    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A127" s="58" t="s">
         <v>372</v>
       </c>
@@ -4192,7 +4251,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="128" spans="1:6">
+    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
         <v>373</v>
       </c>
@@ -4203,7 +4262,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="129" spans="1:4">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
         <v>373</v>
       </c>
@@ -4214,7 +4273,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="130" spans="1:4">
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
         <v>379</v>
       </c>
@@ -4225,7 +4284,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="131" spans="1:4">
+    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" s="1" t="s">
         <v>379</v>
       </c>
@@ -4236,7 +4295,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="135" spans="1:4">
+    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D135" s="59"/>
     </row>
   </sheetData>
@@ -4252,14 +4311,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:U22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="18" width="3" style="4" customWidth="1"/>
     <col min="19" max="19" width="2.140625" customWidth="1"/>
@@ -4267,32 +4326,32 @@
     <col min="21" max="21" width="49" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21">
-      <c r="A1" s="65" t="s">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A1" s="66" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="65"/>
-      <c r="C1" s="65"/>
-      <c r="D1" s="65"/>
-      <c r="E1" s="65"/>
-      <c r="F1" s="65"/>
-      <c r="G1" s="65"/>
-      <c r="H1" s="65"/>
-      <c r="I1" s="65"/>
-      <c r="J1" s="65"/>
-      <c r="K1" s="65"/>
-      <c r="L1" s="65"/>
-      <c r="M1" s="65"/>
-      <c r="N1" s="65"/>
-      <c r="O1" s="65"/>
-      <c r="P1" s="65"/>
-      <c r="Q1" s="65"/>
-      <c r="R1" s="65"/>
-      <c r="S1" s="65"/>
-      <c r="T1" s="65"/>
-      <c r="U1" s="65"/>
-    </row>
-    <row r="3" spans="1:21">
+      <c r="B1" s="66"/>
+      <c r="C1" s="66"/>
+      <c r="D1" s="66"/>
+      <c r="E1" s="66"/>
+      <c r="F1" s="66"/>
+      <c r="G1" s="66"/>
+      <c r="H1" s="66"/>
+      <c r="I1" s="66"/>
+      <c r="J1" s="66"/>
+      <c r="K1" s="66"/>
+      <c r="L1" s="66"/>
+      <c r="M1" s="66"/>
+      <c r="N1" s="66"/>
+      <c r="O1" s="66"/>
+      <c r="P1" s="66"/>
+      <c r="Q1" s="66"/>
+      <c r="R1" s="66"/>
+      <c r="S1" s="66"/>
+      <c r="T1" s="66"/>
+      <c r="U1" s="66"/>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>282</v>
       </c>
@@ -4345,7 +4404,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:21">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="C4" s="35"/>
       <c r="D4" s="35"/>
       <c r="E4" s="35"/>
@@ -4363,12 +4422,12 @@
       <c r="Q4" s="35"/>
       <c r="R4" s="35"/>
     </row>
-    <row r="5" spans="1:21">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>418</v>
       </c>
     </row>
-    <row r="6" spans="1:21">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="C6" s="60">
         <v>0</v>
       </c>
@@ -4393,19 +4452,19 @@
       <c r="J6" s="60">
         <v>0</v>
       </c>
-      <c r="K6" s="66" t="s">
+      <c r="K6" s="67" t="s">
         <v>393</v>
       </c>
-      <c r="L6" s="66"/>
-      <c r="M6" s="66"/>
+      <c r="L6" s="67"/>
+      <c r="M6" s="67"/>
       <c r="N6" s="60" t="s">
         <v>394</v>
       </c>
-      <c r="O6" s="66" t="s">
+      <c r="O6" s="67" t="s">
         <v>395</v>
       </c>
-      <c r="P6" s="66"/>
-      <c r="Q6" s="66"/>
+      <c r="P6" s="67"/>
+      <c r="Q6" s="67"/>
       <c r="R6" s="60">
         <v>0</v>
       </c>
@@ -4416,7 +4475,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="7" spans="1:21">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="T7" t="s">
         <v>398</v>
       </c>
@@ -4424,7 +4483,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="8" spans="1:21">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="C8" s="60">
         <v>0</v>
       </c>
@@ -4449,19 +4508,19 @@
       <c r="J8" s="60">
         <v>1</v>
       </c>
-      <c r="K8" s="66" t="s">
+      <c r="K8" s="67" t="s">
         <v>400</v>
       </c>
-      <c r="L8" s="66"/>
-      <c r="M8" s="66"/>
+      <c r="L8" s="67"/>
+      <c r="M8" s="67"/>
       <c r="N8" s="60" t="s">
         <v>394</v>
       </c>
-      <c r="O8" s="66" t="s">
+      <c r="O8" s="67" t="s">
         <v>401</v>
       </c>
-      <c r="P8" s="66"/>
-      <c r="Q8" s="66"/>
+      <c r="P8" s="67"/>
+      <c r="Q8" s="67"/>
       <c r="R8" s="60">
         <v>0</v>
       </c>
@@ -4472,7 +4531,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="9" spans="1:21">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="T9" t="s">
         <v>398</v>
       </c>
@@ -4480,7 +4539,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="10" spans="1:21">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="C10" s="60">
         <v>0</v>
       </c>
@@ -4536,36 +4595,36 @@
         <v>403</v>
       </c>
     </row>
-    <row r="14" spans="1:21">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>404</v>
       </c>
     </row>
-    <row r="16" spans="1:21">
-      <c r="C16" s="66" t="s">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="C16" s="67" t="s">
         <v>406</v>
       </c>
-      <c r="D16" s="66"/>
-      <c r="E16" s="66"/>
-      <c r="F16" s="66"/>
-      <c r="G16" s="66"/>
-      <c r="H16" s="66"/>
-      <c r="I16" s="66"/>
+      <c r="D16" s="67"/>
+      <c r="E16" s="67"/>
+      <c r="F16" s="67"/>
+      <c r="G16" s="67"/>
+      <c r="H16" s="67"/>
+      <c r="I16" s="67"/>
       <c r="J16" s="60" t="s">
         <v>407</v>
       </c>
-      <c r="K16" s="66" t="s">
+      <c r="K16" s="67" t="s">
         <v>400</v>
       </c>
-      <c r="L16" s="66"/>
-      <c r="M16" s="66"/>
-      <c r="N16" s="66" t="s">
+      <c r="L16" s="67"/>
+      <c r="M16" s="67"/>
+      <c r="N16" s="67" t="s">
         <v>405</v>
       </c>
-      <c r="O16" s="66"/>
-      <c r="P16" s="66"/>
-      <c r="Q16" s="66"/>
-      <c r="R16" s="66"/>
+      <c r="O16" s="67"/>
+      <c r="P16" s="67"/>
+      <c r="Q16" s="67"/>
+      <c r="R16" s="67"/>
       <c r="T16" t="s">
         <v>409</v>
       </c>
@@ -4573,7 +4632,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="17" spans="2:21">
+    <row r="17" spans="2:21" x14ac:dyDescent="0.25">
       <c r="T17" t="s">
         <v>411</v>
       </c>
@@ -4581,7 +4640,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="18" spans="2:21">
+    <row r="18" spans="2:21" x14ac:dyDescent="0.25">
       <c r="T18" t="s">
         <v>413</v>
       </c>
@@ -4589,38 +4648,38 @@
         <v>414</v>
       </c>
     </row>
-    <row r="21" spans="2:21">
+    <row r="21" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>343</v>
       </c>
     </row>
-    <row r="22" spans="2:21">
-      <c r="C22" s="66" t="s">
+    <row r="22" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="C22" s="67" t="s">
         <v>406</v>
       </c>
-      <c r="D22" s="66"/>
-      <c r="E22" s="66"/>
-      <c r="F22" s="66"/>
-      <c r="G22" s="66" t="s">
+      <c r="D22" s="67"/>
+      <c r="E22" s="67"/>
+      <c r="F22" s="67"/>
+      <c r="G22" s="67" t="s">
         <v>415</v>
       </c>
-      <c r="H22" s="66"/>
-      <c r="I22" s="66"/>
-      <c r="J22" s="66"/>
+      <c r="H22" s="67"/>
+      <c r="I22" s="67"/>
+      <c r="J22" s="67"/>
       <c r="K22" s="60">
         <v>0</v>
       </c>
-      <c r="L22" s="66" t="s">
+      <c r="L22" s="67" t="s">
         <v>416</v>
       </c>
-      <c r="M22" s="66"/>
-      <c r="N22" s="66" t="s">
+      <c r="M22" s="67"/>
+      <c r="N22" s="67" t="s">
         <v>417</v>
       </c>
-      <c r="O22" s="66"/>
-      <c r="P22" s="66"/>
-      <c r="Q22" s="66"/>
-      <c r="R22" s="66"/>
+      <c r="O22" s="67"/>
+      <c r="P22" s="67"/>
+      <c r="Q22" s="67"/>
+      <c r="R22" s="67"/>
     </row>
   </sheetData>
   <mergeCells count="12">
@@ -4643,14 +4702,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="6.5703125" style="4" customWidth="1"/>
     <col min="3" max="3" width="26.28515625" customWidth="1"/>
@@ -4659,16 +4718,16 @@
     <col min="6" max="6" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" s="65" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="66" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="65"/>
-      <c r="C1" s="65"/>
-      <c r="D1" s="65"/>
-      <c r="E1" s="65"/>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="B1" s="66"/>
+      <c r="C1" s="66"/>
+      <c r="D1" s="66"/>
+      <c r="E1" s="66"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>192</v>
       </c>
@@ -4676,7 +4735,7 @@
       <c r="D2"/>
       <c r="E2" s="4"/>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>179</v>
       </c>
@@ -4688,7 +4747,7 @@
       </c>
       <c r="E3" s="4"/>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>191</v>
       </c>
@@ -4700,7 +4759,7 @@
       </c>
       <c r="E4" s="4"/>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>180</v>
       </c>
@@ -4712,7 +4771,7 @@
       </c>
       <c r="E5" s="4"/>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>181</v>
       </c>
@@ -4724,7 +4783,7 @@
       </c>
       <c r="E6" s="4"/>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
         <v>182</v>
       </c>
@@ -4736,7 +4795,7 @@
       </c>
       <c r="E7" s="4"/>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
         <v>183</v>
       </c>
@@ -4748,7 +4807,7 @@
       </c>
       <c r="E8" s="4"/>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
         <v>184</v>
       </c>
@@ -4760,7 +4819,7 @@
       </c>
       <c r="E9" s="4"/>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B10" s="3" t="s">
         <v>185</v>
       </c>
@@ -4772,7 +4831,7 @@
       </c>
       <c r="E10" s="4"/>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
         <v>186</v>
       </c>
@@ -4784,7 +4843,7 @@
       </c>
       <c r="E11" s="4"/>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
         <v>187</v>
       </c>
@@ -4796,7 +4855,7 @@
       </c>
       <c r="E12" s="4"/>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
         <v>188</v>
       </c>
@@ -4808,7 +4867,7 @@
       </c>
       <c r="E13" s="4"/>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
         <v>189</v>
       </c>
@@ -4820,7 +4879,7 @@
       </c>
       <c r="E14" s="4"/>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B15" s="2" t="s">
         <v>190</v>
       </c>
@@ -4832,10 +4891,10 @@
       </c>
       <c r="E15" s="4"/>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="27" t="s">
         <v>193</v>
       </c>
@@ -4850,7 +4909,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B18" s="23" t="s">
         <v>178</v>
       </c>
@@ -4858,42 +4917,42 @@
         <v>175</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B19" s="23" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B20" s="23" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B21" s="23" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B22" s="23" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B23" s="23" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B24" s="23" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B25" s="23" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B26" s="23" t="s">
         <v>15</v>
       </c>
@@ -4904,7 +4963,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B27" s="23" t="s">
         <v>157</v>
       </c>
@@ -4915,7 +4974,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B28" s="23" t="s">
         <v>205</v>
       </c>
@@ -4923,14 +4982,14 @@
         <v>208</v>
       </c>
     </row>
-    <row r="30" spans="1:5">
-      <c r="A30" s="67" t="s">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="68" t="s">
         <v>75</v>
       </c>
-      <c r="B30" s="68"/>
-      <c r="C30" s="69"/>
-    </row>
-    <row r="31" spans="1:5">
+      <c r="B30" s="69"/>
+      <c r="C30" s="70"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B31" s="25" t="s">
         <v>223</v>
       </c>
@@ -4938,7 +4997,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B32" s="24">
         <v>0</v>
       </c>
@@ -4946,7 +5005,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="33" spans="2:3">
+    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B33" s="24">
         <v>1</v>
       </c>
@@ -4954,7 +5013,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="34" spans="2:3">
+    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B34" s="24">
         <v>2</v>
       </c>
@@ -4962,7 +5021,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="35" spans="2:3">
+    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B35" s="24">
         <v>3</v>
       </c>
@@ -4970,7 +5029,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="36" spans="2:3">
+    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B36" s="24">
         <v>4</v>
       </c>
@@ -4978,7 +5037,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="37" spans="2:3">
+    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B37" s="24">
         <v>5</v>
       </c>
@@ -4986,7 +5045,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="38" spans="2:3">
+    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B38" s="24">
         <v>6</v>
       </c>
@@ -4994,7 +5053,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="39" spans="2:3">
+    <row r="39" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B39" s="24">
         <v>7</v>
       </c>
@@ -5002,7 +5061,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="40" spans="2:3">
+    <row r="40" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B40" s="24">
         <v>8</v>
       </c>
@@ -5010,7 +5069,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="41" spans="2:3">
+    <row r="41" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B41" s="24">
         <v>9</v>
       </c>
@@ -5018,7 +5077,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="42" spans="2:3">
+    <row r="42" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B42" s="24">
         <v>10</v>
       </c>
@@ -5026,7 +5085,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="43" spans="2:3">
+    <row r="43" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B43" s="24">
         <v>11</v>
       </c>
@@ -5045,14 +5104,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:E43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="6.5703125" style="4" customWidth="1"/>
     <col min="3" max="3" width="26.85546875" customWidth="1"/>
@@ -5061,16 +5120,16 @@
     <col min="6" max="6" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" s="67" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="68" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="68"/>
-      <c r="C1" s="68"/>
-      <c r="D1" s="68"/>
-      <c r="E1" s="69"/>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="B1" s="69"/>
+      <c r="C1" s="69"/>
+      <c r="D1" s="69"/>
+      <c r="E1" s="70"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>192</v>
       </c>
@@ -5078,7 +5137,7 @@
       <c r="D2"/>
       <c r="E2" s="4"/>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>179</v>
       </c>
@@ -5090,7 +5149,7 @@
       </c>
       <c r="E3" s="4"/>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>191</v>
       </c>
@@ -5102,7 +5161,7 @@
       </c>
       <c r="E4" s="4"/>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>180</v>
       </c>
@@ -5114,7 +5173,7 @@
       </c>
       <c r="E5" s="4"/>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>181</v>
       </c>
@@ -5126,7 +5185,7 @@
       </c>
       <c r="E6" s="4"/>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
         <v>182</v>
       </c>
@@ -5138,7 +5197,7 @@
       </c>
       <c r="E7" s="4"/>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
         <v>183</v>
       </c>
@@ -5150,7 +5209,7 @@
       </c>
       <c r="E8" s="4"/>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
         <v>184</v>
       </c>
@@ -5162,7 +5221,7 @@
       </c>
       <c r="E9" s="4"/>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B10" s="3" t="s">
         <v>185</v>
       </c>
@@ -5174,7 +5233,7 @@
       </c>
       <c r="E10" s="4"/>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
         <v>186</v>
       </c>
@@ -5186,7 +5245,7 @@
       </c>
       <c r="E11" s="4"/>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
         <v>187</v>
       </c>
@@ -5198,7 +5257,7 @@
       </c>
       <c r="E12" s="4"/>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
         <v>188</v>
       </c>
@@ -5210,7 +5269,7 @@
       </c>
       <c r="E13" s="4"/>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
         <v>189</v>
       </c>
@@ -5222,7 +5281,7 @@
       </c>
       <c r="E14" s="4"/>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B15" s="2" t="s">
         <v>190</v>
       </c>
@@ -5234,14 +5293,14 @@
       </c>
       <c r="E15" s="4"/>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
     </row>
-    <row r="17" spans="1:5">
-      <c r="A17" s="65" t="s">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="66" t="s">
         <v>193</v>
       </c>
-      <c r="B17" s="65"/>
+      <c r="B17" s="66"/>
       <c r="C17" s="28" t="s">
         <v>202</v>
       </c>
@@ -5249,10 +5308,10 @@
         <v>206</v>
       </c>
       <c r="E17" s="28" t="s">
-        <v>477</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>0</v>
       </c>
@@ -5269,7 +5328,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19">
         <f>A18+1</f>
         <v>1</v>
@@ -5287,7 +5346,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20">
         <f t="shared" ref="A20:A26" si="0">A19+1</f>
         <v>2</v>
@@ -5305,7 +5364,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -5317,7 +5376,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -5329,7 +5388,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -5341,7 +5400,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -5353,7 +5412,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -5365,7 +5424,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -5377,19 +5436,19 @@
         <v>272</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B27" s="23" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="29" spans="1:5">
-      <c r="A29" s="67" t="s">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="68" t="s">
         <v>75</v>
       </c>
-      <c r="B29" s="68"/>
-      <c r="C29" s="69"/>
-    </row>
-    <row r="30" spans="1:5">
+      <c r="B29" s="69"/>
+      <c r="C29" s="70"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B30" s="25" t="s">
         <v>223</v>
       </c>
@@ -5397,7 +5456,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="31" spans="1:5">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B31" s="24">
         <v>0</v>
       </c>
@@ -5405,7 +5464,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B32" s="24">
         <v>1</v>
       </c>
@@ -5413,7 +5472,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="33" spans="2:3">
+    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B33" s="24">
         <v>2</v>
       </c>
@@ -5421,7 +5480,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="34" spans="2:3">
+    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B34" s="24">
         <v>3</v>
       </c>
@@ -5429,7 +5488,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="35" spans="2:3">
+    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B35" s="24">
         <v>4</v>
       </c>
@@ -5437,7 +5496,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="36" spans="2:3">
+    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B36" s="24">
         <v>5</v>
       </c>
@@ -5445,7 +5504,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="37" spans="2:3">
+    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B37" s="24">
         <v>6</v>
       </c>
@@ -5453,7 +5512,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="38" spans="2:3">
+    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B38" s="24">
         <v>7</v>
       </c>
@@ -5461,7 +5520,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="39" spans="2:3">
+    <row r="39" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B39" s="24">
         <v>8</v>
       </c>
@@ -5469,7 +5528,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="40" spans="2:3">
+    <row r="40" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B40" s="24">
         <v>9</v>
       </c>
@@ -5477,7 +5536,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="41" spans="2:3">
+    <row r="41" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B41" s="24">
         <v>10</v>
       </c>
@@ -5485,7 +5544,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="42" spans="2:3">
+    <row r="42" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B42" s="24">
         <v>11</v>
       </c>
@@ -5493,7 +5552,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="43" spans="2:3">
+    <row r="43" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B43" s="24">
         <v>12</v>
       </c>
@@ -5516,14 +5575,14 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:U35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="T4" sqref="T4:U9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5.5703125" customWidth="1"/>
@@ -5540,38 +5599,38 @@
     <col min="17" max="17" width="4.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="23.25">
+    <row r="1" spans="1:21" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="18" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="3" spans="1:21">
-      <c r="B3" s="66" t="s">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B3" s="67" t="s">
         <v>120</v>
       </c>
-      <c r="C3" s="66"/>
-      <c r="D3" s="66" t="s">
+      <c r="C3" s="67"/>
+      <c r="D3" s="67" t="s">
         <v>121</v>
       </c>
-      <c r="E3" s="66"/>
-      <c r="H3" s="66" t="s">
+      <c r="E3" s="67"/>
+      <c r="H3" s="67" t="s">
         <v>120</v>
       </c>
-      <c r="I3" s="66"/>
-      <c r="J3" s="66" t="s">
+      <c r="I3" s="67"/>
+      <c r="J3" s="67" t="s">
         <v>121</v>
       </c>
-      <c r="K3" s="66"/>
-      <c r="N3" s="66" t="s">
+      <c r="K3" s="67"/>
+      <c r="N3" s="67" t="s">
         <v>120</v>
       </c>
-      <c r="O3" s="66"/>
-      <c r="P3" s="66" t="s">
+      <c r="O3" s="67"/>
+      <c r="P3" s="67" t="s">
         <v>121</v>
       </c>
-      <c r="Q3" s="66"/>
-    </row>
-    <row r="4" spans="1:21">
+      <c r="Q3" s="67"/>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" s="13">
         <v>800</v>
       </c>
@@ -5629,7 +5688,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:21">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" s="13">
         <v>802</v>
       </c>
@@ -5688,7 +5747,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:21">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" s="13">
         <v>804</v>
       </c>
@@ -5747,40 +5806,40 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:21">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" s="13">
         <v>806</v>
       </c>
-      <c r="B7" s="70" t="s">
+      <c r="B7" s="71" t="s">
         <v>122</v>
       </c>
-      <c r="C7" s="71"/>
-      <c r="D7" s="70" t="s">
+      <c r="C7" s="72"/>
+      <c r="D7" s="71" t="s">
         <v>123</v>
       </c>
-      <c r="E7" s="71"/>
+      <c r="E7" s="72"/>
       <c r="G7" s="13">
         <v>846</v>
       </c>
-      <c r="H7" s="70" t="s">
+      <c r="H7" s="71" t="s">
         <v>122</v>
       </c>
-      <c r="I7" s="71"/>
-      <c r="J7" s="70" t="s">
+      <c r="I7" s="72"/>
+      <c r="J7" s="71" t="s">
         <v>123</v>
       </c>
-      <c r="K7" s="71"/>
+      <c r="K7" s="72"/>
       <c r="M7" s="13">
         <v>886</v>
       </c>
-      <c r="N7" s="70" t="s">
+      <c r="N7" s="71" t="s">
         <v>122</v>
       </c>
-      <c r="O7" s="71"/>
-      <c r="P7" s="70" t="s">
+      <c r="O7" s="72"/>
+      <c r="P7" s="71" t="s">
         <v>123</v>
       </c>
-      <c r="Q7" s="71"/>
+      <c r="Q7" s="72"/>
       <c r="T7">
         <v>3</v>
       </c>
@@ -5788,7 +5847,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:21">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" s="13">
         <v>808</v>
       </c>
@@ -5832,7 +5891,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:21">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>124</v>
       </c>
@@ -5876,7 +5935,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:21">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
         <v>125</v>
       </c>
@@ -5914,36 +5973,36 @@
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:21">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
         <v>126</v>
       </c>
       <c r="B11" s="14"/>
       <c r="C11" s="15"/>
-      <c r="D11" s="70" t="s">
+      <c r="D11" s="71" t="s">
         <v>123</v>
       </c>
-      <c r="E11" s="71"/>
+      <c r="E11" s="72"/>
       <c r="G11" s="13" t="s">
         <v>142</v>
       </c>
       <c r="H11" s="14"/>
       <c r="I11" s="15"/>
-      <c r="J11" s="70" t="s">
+      <c r="J11" s="71" t="s">
         <v>123</v>
       </c>
-      <c r="K11" s="71"/>
+      <c r="K11" s="72"/>
       <c r="M11" s="13" t="s">
         <v>245</v>
       </c>
       <c r="N11" s="14"/>
       <c r="O11" s="29"/>
-      <c r="P11" s="70" t="s">
+      <c r="P11" s="71" t="s">
         <v>123</v>
       </c>
-      <c r="Q11" s="71"/>
-    </row>
-    <row r="12" spans="1:21">
+      <c r="Q11" s="72"/>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" s="13">
         <v>810</v>
       </c>
@@ -5981,7 +6040,7 @@
       <c r="P12" s="14"/>
       <c r="Q12" s="29"/>
     </row>
-    <row r="13" spans="1:21">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" s="13">
         <v>812</v>
       </c>
@@ -6019,7 +6078,7 @@
       <c r="P13" s="14"/>
       <c r="Q13" s="29"/>
     </row>
-    <row r="14" spans="1:21">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" s="13">
         <v>814</v>
       </c>
@@ -6057,152 +6116,152 @@
       <c r="P14" s="14"/>
       <c r="Q14" s="29"/>
     </row>
-    <row r="15" spans="1:21">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" s="13">
         <v>816</v>
       </c>
-      <c r="B15" s="70" t="s">
+      <c r="B15" s="71" t="s">
         <v>122</v>
       </c>
-      <c r="C15" s="71"/>
+      <c r="C15" s="72"/>
       <c r="D15" s="16"/>
       <c r="E15" s="17"/>
       <c r="G15" s="13">
         <v>856</v>
       </c>
-      <c r="H15" s="70" t="s">
+      <c r="H15" s="71" t="s">
         <v>122</v>
       </c>
-      <c r="I15" s="71"/>
+      <c r="I15" s="72"/>
       <c r="J15" s="16"/>
       <c r="K15" s="17"/>
       <c r="M15" s="13">
         <v>896</v>
       </c>
-      <c r="N15" s="70" t="s">
+      <c r="N15" s="71" t="s">
         <v>122</v>
       </c>
-      <c r="O15" s="71"/>
+      <c r="O15" s="72"/>
       <c r="P15" s="16"/>
       <c r="Q15" s="17"/>
     </row>
-    <row r="16" spans="1:21">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" s="13">
         <v>818</v>
       </c>
-      <c r="B16" s="66" t="s">
+      <c r="B16" s="67" t="s">
         <v>127</v>
       </c>
-      <c r="C16" s="66"/>
-      <c r="D16" s="66"/>
-      <c r="E16" s="66"/>
+      <c r="C16" s="67"/>
+      <c r="D16" s="67"/>
+      <c r="E16" s="67"/>
       <c r="G16" s="13">
         <v>858</v>
       </c>
-      <c r="H16" s="66" t="s">
+      <c r="H16" s="67" t="s">
         <v>127</v>
       </c>
-      <c r="I16" s="66"/>
-      <c r="J16" s="66"/>
-      <c r="K16" s="66"/>
+      <c r="I16" s="67"/>
+      <c r="J16" s="67"/>
+      <c r="K16" s="67"/>
       <c r="M16" s="13">
         <v>898</v>
       </c>
-      <c r="N16" s="66" t="s">
+      <c r="N16" s="67" t="s">
         <v>127</v>
       </c>
-      <c r="O16" s="66"/>
-      <c r="P16" s="66"/>
-      <c r="Q16" s="66"/>
-    </row>
-    <row r="17" spans="1:17">
+      <c r="O16" s="67"/>
+      <c r="P16" s="67"/>
+      <c r="Q16" s="67"/>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="13" t="s">
         <v>128</v>
       </c>
-      <c r="B17" s="66" t="s">
+      <c r="B17" s="67" t="s">
         <v>129</v>
       </c>
-      <c r="C17" s="66"/>
-      <c r="D17" s="66"/>
-      <c r="E17" s="66"/>
+      <c r="C17" s="67"/>
+      <c r="D17" s="67"/>
+      <c r="E17" s="67"/>
       <c r="G17" s="13" t="s">
         <v>143</v>
       </c>
-      <c r="H17" s="66" t="s">
+      <c r="H17" s="67" t="s">
         <v>129</v>
       </c>
-      <c r="I17" s="66"/>
-      <c r="J17" s="66"/>
-      <c r="K17" s="66"/>
+      <c r="I17" s="67"/>
+      <c r="J17" s="67"/>
+      <c r="K17" s="67"/>
       <c r="M17" s="13" t="s">
         <v>246</v>
       </c>
-      <c r="N17" s="66" t="s">
+      <c r="N17" s="67" t="s">
         <v>129</v>
       </c>
-      <c r="O17" s="66"/>
-      <c r="P17" s="66"/>
-      <c r="Q17" s="66"/>
-    </row>
-    <row r="18" spans="1:17">
+      <c r="O17" s="67"/>
+      <c r="P17" s="67"/>
+      <c r="Q17" s="67"/>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="13" t="s">
         <v>130</v>
       </c>
-      <c r="B18" s="66" t="s">
+      <c r="B18" s="67" t="s">
         <v>132</v>
       </c>
-      <c r="C18" s="66"/>
-      <c r="D18" s="66"/>
-      <c r="E18" s="66"/>
+      <c r="C18" s="67"/>
+      <c r="D18" s="67"/>
+      <c r="E18" s="67"/>
       <c r="G18" s="13" t="s">
         <v>144</v>
       </c>
-      <c r="H18" s="66" t="s">
+      <c r="H18" s="67" t="s">
         <v>132</v>
       </c>
-      <c r="I18" s="66"/>
-      <c r="J18" s="66"/>
-      <c r="K18" s="66"/>
+      <c r="I18" s="67"/>
+      <c r="J18" s="67"/>
+      <c r="K18" s="67"/>
       <c r="M18" s="13" t="s">
         <v>247</v>
       </c>
-      <c r="N18" s="66" t="s">
+      <c r="N18" s="67" t="s">
         <v>132</v>
       </c>
-      <c r="O18" s="66"/>
-      <c r="P18" s="66"/>
-      <c r="Q18" s="66"/>
-    </row>
-    <row r="19" spans="1:17">
+      <c r="O18" s="67"/>
+      <c r="P18" s="67"/>
+      <c r="Q18" s="67"/>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" s="13" t="s">
         <v>131</v>
       </c>
-      <c r="B19" s="66" t="s">
+      <c r="B19" s="67" t="s">
         <v>132</v>
       </c>
-      <c r="C19" s="66"/>
-      <c r="D19" s="66"/>
-      <c r="E19" s="66"/>
+      <c r="C19" s="67"/>
+      <c r="D19" s="67"/>
+      <c r="E19" s="67"/>
       <c r="G19" s="13" t="s">
         <v>145</v>
       </c>
-      <c r="H19" s="66" t="s">
+      <c r="H19" s="67" t="s">
         <v>132</v>
       </c>
-      <c r="I19" s="66"/>
-      <c r="J19" s="66"/>
-      <c r="K19" s="66"/>
+      <c r="I19" s="67"/>
+      <c r="J19" s="67"/>
+      <c r="K19" s="67"/>
       <c r="M19" s="13" t="s">
         <v>248</v>
       </c>
-      <c r="N19" s="66" t="s">
+      <c r="N19" s="67" t="s">
         <v>132</v>
       </c>
-      <c r="O19" s="66"/>
-      <c r="P19" s="66"/>
-      <c r="Q19" s="66"/>
-    </row>
-    <row r="20" spans="1:17">
+      <c r="O19" s="67"/>
+      <c r="P19" s="67"/>
+      <c r="Q19" s="67"/>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" s="13">
         <v>820</v>
       </c>
@@ -6255,7 +6314,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="21" spans="1:17">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" s="13">
         <v>822</v>
       </c>
@@ -6308,7 +6367,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="22" spans="1:17">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" s="13">
         <v>824</v>
       </c>
@@ -6361,42 +6420,42 @@
         <v>34</v>
       </c>
     </row>
-    <row r="23" spans="1:17">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" s="13">
         <v>826</v>
       </c>
-      <c r="B23" s="70" t="s">
+      <c r="B23" s="71" t="s">
         <v>122</v>
       </c>
-      <c r="C23" s="71"/>
-      <c r="D23" s="70" t="s">
+      <c r="C23" s="72"/>
+      <c r="D23" s="71" t="s">
         <v>123</v>
       </c>
-      <c r="E23" s="71"/>
+      <c r="E23" s="72"/>
       <c r="G23" s="13">
         <v>866</v>
       </c>
-      <c r="H23" s="70" t="s">
+      <c r="H23" s="71" t="s">
         <v>122</v>
       </c>
-      <c r="I23" s="71"/>
-      <c r="J23" s="70" t="s">
+      <c r="I23" s="72"/>
+      <c r="J23" s="71" t="s">
         <v>123</v>
       </c>
-      <c r="K23" s="71"/>
+      <c r="K23" s="72"/>
       <c r="M23" s="13" t="s">
         <v>252</v>
       </c>
-      <c r="N23" s="70" t="s">
+      <c r="N23" s="71" t="s">
         <v>122</v>
       </c>
-      <c r="O23" s="71"/>
-      <c r="P23" s="70" t="s">
+      <c r="O23" s="72"/>
+      <c r="P23" s="71" t="s">
         <v>123</v>
       </c>
-      <c r="Q23" s="71"/>
-    </row>
-    <row r="24" spans="1:17">
+      <c r="Q23" s="72"/>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" s="13">
         <v>828</v>
       </c>
@@ -6434,7 +6493,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="25" spans="1:17">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" s="13" t="s">
         <v>133</v>
       </c>
@@ -6472,7 +6531,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="26" spans="1:17">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" s="13" t="s">
         <v>134</v>
       </c>
@@ -6510,36 +6569,36 @@
         <v>34</v>
       </c>
     </row>
-    <row r="27" spans="1:17">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" s="13" t="s">
         <v>135</v>
       </c>
       <c r="B27" s="14"/>
       <c r="C27" s="15"/>
-      <c r="D27" s="70" t="s">
+      <c r="D27" s="71" t="s">
         <v>123</v>
       </c>
-      <c r="E27" s="71"/>
+      <c r="E27" s="72"/>
       <c r="G27" s="13" t="s">
         <v>148</v>
       </c>
       <c r="H27" s="14"/>
       <c r="I27" s="15"/>
-      <c r="J27" s="70" t="s">
+      <c r="J27" s="71" t="s">
         <v>123</v>
       </c>
-      <c r="K27" s="71"/>
+      <c r="K27" s="72"/>
       <c r="M27" s="13" t="s">
         <v>256</v>
       </c>
       <c r="N27" s="14"/>
       <c r="O27" s="29"/>
-      <c r="P27" s="70" t="s">
+      <c r="P27" s="71" t="s">
         <v>123</v>
       </c>
-      <c r="Q27" s="71"/>
-    </row>
-    <row r="28" spans="1:17">
+      <c r="Q27" s="72"/>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" s="13">
         <v>830</v>
       </c>
@@ -6577,7 +6636,7 @@
       <c r="P28" s="14"/>
       <c r="Q28" s="29"/>
     </row>
-    <row r="29" spans="1:17">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29" s="13">
         <v>832</v>
       </c>
@@ -6615,7 +6674,7 @@
       <c r="P29" s="14"/>
       <c r="Q29" s="29"/>
     </row>
-    <row r="30" spans="1:17">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30" s="13">
         <v>834</v>
       </c>
@@ -6653,163 +6712,181 @@
       <c r="P30" s="14"/>
       <c r="Q30" s="29"/>
     </row>
-    <row r="31" spans="1:17">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31" s="13">
         <v>836</v>
       </c>
-      <c r="B31" s="70" t="s">
+      <c r="B31" s="71" t="s">
         <v>122</v>
       </c>
-      <c r="C31" s="71"/>
+      <c r="C31" s="72"/>
       <c r="D31" s="16"/>
       <c r="E31" s="17"/>
       <c r="G31" s="13">
         <v>876</v>
       </c>
-      <c r="H31" s="70" t="s">
+      <c r="H31" s="71" t="s">
         <v>122</v>
       </c>
-      <c r="I31" s="71"/>
+      <c r="I31" s="72"/>
       <c r="J31" s="16"/>
       <c r="K31" s="17"/>
       <c r="M31" s="13" t="s">
         <v>260</v>
       </c>
-      <c r="N31" s="70" t="s">
+      <c r="N31" s="71" t="s">
         <v>122</v>
       </c>
-      <c r="O31" s="71"/>
+      <c r="O31" s="72"/>
       <c r="P31" s="16"/>
       <c r="Q31" s="17"/>
     </row>
-    <row r="32" spans="1:17">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A32" s="13">
         <v>838</v>
       </c>
-      <c r="B32" s="66" t="s">
+      <c r="B32" s="67" t="s">
         <v>127</v>
       </c>
-      <c r="C32" s="66"/>
-      <c r="D32" s="66"/>
-      <c r="E32" s="66"/>
+      <c r="C32" s="67"/>
+      <c r="D32" s="67"/>
+      <c r="E32" s="67"/>
       <c r="G32" s="13">
         <v>878</v>
       </c>
-      <c r="H32" s="66" t="s">
+      <c r="H32" s="67" t="s">
         <v>127</v>
       </c>
-      <c r="I32" s="66"/>
-      <c r="J32" s="66"/>
-      <c r="K32" s="66"/>
+      <c r="I32" s="67"/>
+      <c r="J32" s="67"/>
+      <c r="K32" s="67"/>
       <c r="M32" s="13" t="s">
         <v>261</v>
       </c>
-      <c r="N32" s="66" t="s">
+      <c r="N32" s="67" t="s">
         <v>127</v>
       </c>
-      <c r="O32" s="66"/>
-      <c r="P32" s="66"/>
-      <c r="Q32" s="66"/>
-    </row>
-    <row r="33" spans="1:17">
+      <c r="O32" s="67"/>
+      <c r="P32" s="67"/>
+      <c r="Q32" s="67"/>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A33" s="13" t="s">
         <v>136</v>
       </c>
-      <c r="B33" s="66" t="s">
+      <c r="B33" s="67" t="s">
         <v>129</v>
       </c>
-      <c r="C33" s="66"/>
-      <c r="D33" s="66"/>
-      <c r="E33" s="66"/>
+      <c r="C33" s="67"/>
+      <c r="D33" s="67"/>
+      <c r="E33" s="67"/>
       <c r="G33" s="13" t="s">
         <v>149</v>
       </c>
-      <c r="H33" s="66" t="s">
+      <c r="H33" s="67" t="s">
         <v>129</v>
       </c>
-      <c r="I33" s="66"/>
-      <c r="J33" s="66"/>
-      <c r="K33" s="66"/>
+      <c r="I33" s="67"/>
+      <c r="J33" s="67"/>
+      <c r="K33" s="67"/>
       <c r="M33" s="13" t="s">
         <v>262</v>
       </c>
-      <c r="N33" s="66" t="s">
+      <c r="N33" s="67" t="s">
         <v>129</v>
       </c>
-      <c r="O33" s="66"/>
-      <c r="P33" s="66"/>
-      <c r="Q33" s="66"/>
-    </row>
-    <row r="34" spans="1:17">
+      <c r="O33" s="67"/>
+      <c r="P33" s="67"/>
+      <c r="Q33" s="67"/>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A34" s="13" t="s">
         <v>137</v>
       </c>
-      <c r="B34" s="66" t="s">
+      <c r="B34" s="67" t="s">
         <v>132</v>
       </c>
-      <c r="C34" s="66"/>
-      <c r="D34" s="66"/>
-      <c r="E34" s="66"/>
+      <c r="C34" s="67"/>
+      <c r="D34" s="67"/>
+      <c r="E34" s="67"/>
       <c r="G34" s="13" t="s">
         <v>150</v>
       </c>
-      <c r="H34" s="66" t="s">
+      <c r="H34" s="67" t="s">
         <v>132</v>
       </c>
-      <c r="I34" s="66"/>
-      <c r="J34" s="66"/>
-      <c r="K34" s="66"/>
+      <c r="I34" s="67"/>
+      <c r="J34" s="67"/>
+      <c r="K34" s="67"/>
       <c r="M34" s="13" t="s">
         <v>263</v>
       </c>
-      <c r="N34" s="66" t="s">
+      <c r="N34" s="67" t="s">
         <v>132</v>
       </c>
-      <c r="O34" s="66"/>
-      <c r="P34" s="66"/>
-      <c r="Q34" s="66"/>
-    </row>
-    <row r="35" spans="1:17">
+      <c r="O34" s="67"/>
+      <c r="P34" s="67"/>
+      <c r="Q34" s="67"/>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A35" s="13" t="s">
         <v>138</v>
       </c>
-      <c r="B35" s="66" t="s">
+      <c r="B35" s="67" t="s">
         <v>132</v>
       </c>
-      <c r="C35" s="66"/>
-      <c r="D35" s="66"/>
-      <c r="E35" s="66"/>
+      <c r="C35" s="67"/>
+      <c r="D35" s="67"/>
+      <c r="E35" s="67"/>
       <c r="G35" s="13" t="s">
         <v>151</v>
       </c>
-      <c r="H35" s="66" t="s">
+      <c r="H35" s="67" t="s">
         <v>132</v>
       </c>
-      <c r="I35" s="66"/>
-      <c r="J35" s="66"/>
-      <c r="K35" s="66"/>
+      <c r="I35" s="67"/>
+      <c r="J35" s="67"/>
+      <c r="K35" s="67"/>
       <c r="M35" s="13" t="s">
         <v>264</v>
       </c>
-      <c r="N35" s="66" t="s">
+      <c r="N35" s="67" t="s">
         <v>132</v>
       </c>
-      <c r="O35" s="66"/>
-      <c r="P35" s="66"/>
-      <c r="Q35" s="66"/>
+      <c r="O35" s="67"/>
+      <c r="P35" s="67"/>
+      <c r="Q35" s="67"/>
     </row>
   </sheetData>
   <mergeCells count="54">
-    <mergeCell ref="B32:E32"/>
-    <mergeCell ref="B33:E33"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="H32:K32"/>
-    <mergeCell ref="H33:K33"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="J27:K27"/>
-    <mergeCell ref="H31:I31"/>
-    <mergeCell ref="H23:I23"/>
-    <mergeCell ref="J23:K23"/>
+    <mergeCell ref="N33:Q33"/>
+    <mergeCell ref="N34:Q34"/>
+    <mergeCell ref="N35:Q35"/>
+    <mergeCell ref="N23:O23"/>
+    <mergeCell ref="P23:Q23"/>
+    <mergeCell ref="P27:Q27"/>
+    <mergeCell ref="N31:O31"/>
+    <mergeCell ref="N32:Q32"/>
+    <mergeCell ref="N15:O15"/>
+    <mergeCell ref="N16:Q16"/>
+    <mergeCell ref="N17:Q17"/>
+    <mergeCell ref="N18:Q18"/>
+    <mergeCell ref="N19:Q19"/>
+    <mergeCell ref="N3:O3"/>
+    <mergeCell ref="P3:Q3"/>
+    <mergeCell ref="N7:O7"/>
+    <mergeCell ref="P7:Q7"/>
+    <mergeCell ref="P11:Q11"/>
+    <mergeCell ref="B17:E17"/>
+    <mergeCell ref="B18:E18"/>
+    <mergeCell ref="B19:E19"/>
+    <mergeCell ref="B16:E16"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="J11:K11"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="J3:K3"/>
     <mergeCell ref="H34:K34"/>
     <mergeCell ref="H35:K35"/>
     <mergeCell ref="B3:C3"/>
@@ -6826,34 +6903,16 @@
     <mergeCell ref="H19:K19"/>
     <mergeCell ref="D23:E23"/>
     <mergeCell ref="D27:E27"/>
-    <mergeCell ref="J7:K7"/>
-    <mergeCell ref="J11:K11"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="J3:K3"/>
-    <mergeCell ref="B17:E17"/>
-    <mergeCell ref="B18:E18"/>
-    <mergeCell ref="B19:E19"/>
-    <mergeCell ref="B16:E16"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="N3:O3"/>
-    <mergeCell ref="P3:Q3"/>
-    <mergeCell ref="N7:O7"/>
-    <mergeCell ref="P7:Q7"/>
-    <mergeCell ref="P11:Q11"/>
-    <mergeCell ref="N15:O15"/>
-    <mergeCell ref="N16:Q16"/>
-    <mergeCell ref="N17:Q17"/>
-    <mergeCell ref="N18:Q18"/>
-    <mergeCell ref="N19:Q19"/>
-    <mergeCell ref="N33:Q33"/>
-    <mergeCell ref="N34:Q34"/>
-    <mergeCell ref="N35:Q35"/>
-    <mergeCell ref="N23:O23"/>
-    <mergeCell ref="P23:Q23"/>
-    <mergeCell ref="P27:Q27"/>
-    <mergeCell ref="N31:O31"/>
-    <mergeCell ref="N32:Q32"/>
+    <mergeCell ref="B32:E32"/>
+    <mergeCell ref="B33:E33"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="H32:K32"/>
+    <mergeCell ref="H33:K33"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="J27:K27"/>
+    <mergeCell ref="H31:I31"/>
+    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="J23:K23"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6865,14 +6924,14 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:P23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A23" sqref="A23:N23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="5.140625" customWidth="1"/>
     <col min="3" max="3" width="4.7109375" customWidth="1"/>
@@ -6886,7 +6945,7 @@
     <col min="16" max="16" width="14.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
         <v>359</v>
       </c>
@@ -6894,13 +6953,13 @@
       <c r="C1" s="19"/>
       <c r="D1" s="19"/>
     </row>
-    <row r="2" spans="1:16">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="45"/>
       <c r="B2" s="45"/>
       <c r="C2" s="45"/>
       <c r="D2" s="45"/>
     </row>
-    <row r="3" spans="1:16">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="45"/>
       <c r="B3" s="38" t="s">
         <v>325</v>
@@ -6916,7 +6975,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="4" spans="1:16">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="45"/>
       <c r="B4" s="48" t="s">
         <v>316</v>
@@ -6934,7 +6993,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:16">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="45"/>
       <c r="B5" s="48" t="s">
         <v>319</v>
@@ -6952,7 +7011,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="6" spans="1:16">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="45"/>
       <c r="B6" s="48" t="s">
         <v>321</v>
@@ -6970,7 +7029,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="7" spans="1:16">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="45"/>
       <c r="B7" s="48" t="s">
         <v>323</v>
@@ -6988,7 +7047,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="8" spans="1:16">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="45"/>
       <c r="B8" s="45"/>
       <c r="C8" s="45"/>
@@ -7003,30 +7062,30 @@
         <v>281</v>
       </c>
     </row>
-    <row r="9" spans="1:16">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="45"/>
       <c r="B9" s="45"/>
       <c r="C9" s="45"/>
       <c r="D9" s="45"/>
       <c r="F9" s="3"/>
     </row>
-    <row r="10" spans="1:16" ht="17.25">
+    <row r="10" spans="1:16" ht="17.25" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>75</v>
       </c>
-      <c r="F10" s="72" t="s">
+      <c r="F10" s="73" t="s">
         <v>326</v>
       </c>
-      <c r="G10" s="72"/>
-      <c r="H10" s="72"/>
-      <c r="I10" s="72"/>
-      <c r="J10" s="72"/>
-      <c r="K10" s="72"/>
-      <c r="L10" s="72"/>
-      <c r="M10" s="72"/>
-      <c r="N10" s="72"/>
-    </row>
-    <row r="11" spans="1:16">
+      <c r="G10" s="73"/>
+      <c r="H10" s="73"/>
+      <c r="I10" s="73"/>
+      <c r="J10" s="73"/>
+      <c r="K10" s="73"/>
+      <c r="L10" s="73"/>
+      <c r="M10" s="73"/>
+      <c r="N10" s="73"/>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C11" s="38" t="s">
         <v>282</v>
       </c>
@@ -7060,7 +7119,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="12" spans="1:16">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C12" s="32">
         <v>0</v>
       </c>
@@ -7097,7 +7156,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="13" spans="1:16">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C13" s="32">
         <v>1</v>
       </c>
@@ -7130,7 +7189,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="14" spans="1:16">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C14" s="32">
         <v>2</v>
       </c>
@@ -7156,7 +7215,7 @@
       </c>
       <c r="N14" s="43"/>
     </row>
-    <row r="15" spans="1:16">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C15" s="32">
         <v>3</v>
       </c>
@@ -7184,7 +7243,7 @@
       </c>
       <c r="N15" s="43"/>
     </row>
-    <row r="16" spans="1:16">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C16" s="32">
         <v>4</v>
       </c>
@@ -7208,7 +7267,7 @@
       <c r="M16" s="33"/>
       <c r="N16" s="33"/>
     </row>
-    <row r="17" spans="1:14">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C17" s="32" t="s">
         <v>283</v>
       </c>
@@ -7234,7 +7293,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="18" spans="1:14">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="G18" s="33">
         <v>5</v>
       </c>
@@ -7256,7 +7315,7 @@
       </c>
       <c r="N18" s="33"/>
     </row>
-    <row r="19" spans="1:14">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="G19" s="33">
         <v>6</v>
       </c>
@@ -7276,7 +7335,7 @@
       <c r="M19" s="33"/>
       <c r="N19" s="33"/>
     </row>
-    <row r="20" spans="1:14">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="G20" s="33">
         <v>7</v>
       </c>
@@ -7296,7 +7355,7 @@
       <c r="M20" s="33"/>
       <c r="N20" s="33"/>
     </row>
-    <row r="21" spans="1:14">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="G21" s="33">
         <v>8</v>
       </c>
@@ -7318,23 +7377,23 @@
         <v>314</v>
       </c>
     </row>
-    <row r="23" spans="1:14" s="63" customFormat="1" ht="30" customHeight="1">
-      <c r="A23" s="73" t="s">
-        <v>478</v>
-      </c>
-      <c r="B23" s="73"/>
-      <c r="C23" s="73"/>
-      <c r="D23" s="73"/>
-      <c r="E23" s="73"/>
-      <c r="F23" s="73"/>
-      <c r="G23" s="73"/>
-      <c r="H23" s="73"/>
-      <c r="I23" s="73"/>
-      <c r="J23" s="73"/>
-      <c r="K23" s="73"/>
-      <c r="L23" s="73"/>
-      <c r="M23" s="73"/>
-      <c r="N23" s="73"/>
+    <row r="23" spans="1:14" s="63" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="74" t="s">
+        <v>477</v>
+      </c>
+      <c r="B23" s="74"/>
+      <c r="C23" s="74"/>
+      <c r="D23" s="74"/>
+      <c r="E23" s="74"/>
+      <c r="F23" s="74"/>
+      <c r="G23" s="74"/>
+      <c r="H23" s="74"/>
+      <c r="I23" s="74"/>
+      <c r="J23" s="74"/>
+      <c r="K23" s="74"/>
+      <c r="L23" s="74"/>
+      <c r="M23" s="74"/>
+      <c r="N23" s="74"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -7350,27 +7409,27 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:C34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="12.85546875" customWidth="1"/>
     <col min="3" max="3" width="37.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="76" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="77" t="s">
         <v>358</v>
       </c>
-      <c r="B1" s="76"/>
-      <c r="C1" s="76"/>
-    </row>
-    <row r="3" spans="1:3">
+      <c r="B1" s="77"/>
+      <c r="C1" s="77"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B3" s="13" t="s">
         <v>336</v>
       </c>
@@ -7378,7 +7437,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B4" s="13" t="s">
         <v>337</v>
       </c>
@@ -7386,7 +7445,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B5" s="56" t="s">
         <v>328</v>
       </c>
@@ -7394,7 +7453,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B6" s="56" t="s">
         <v>329</v>
       </c>
@@ -7402,7 +7461,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B7" s="56" t="s">
         <v>330</v>
       </c>
@@ -7410,7 +7469,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B8" s="56" t="s">
         <v>331</v>
       </c>
@@ -7418,7 +7477,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B9" s="56" t="s">
         <v>332</v>
       </c>
@@ -7426,7 +7485,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B10" s="56" t="s">
         <v>333</v>
       </c>
@@ -7434,7 +7493,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B11" s="56" t="s">
         <v>334</v>
       </c>
@@ -7442,7 +7501,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B12" s="56" t="s">
         <v>335</v>
       </c>
@@ -7450,18 +7509,18 @@
         <v>84</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
-      <c r="A14" s="75" t="s">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="76" t="s">
         <v>343</v>
       </c>
-      <c r="B14" s="75"/>
-      <c r="C14" s="75"/>
-    </row>
-    <row r="15" spans="1:3">
+      <c r="B14" s="76"/>
+      <c r="C14" s="76"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B15" s="35"/>
       <c r="C15" s="36"/>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B16" s="54" t="s">
         <v>223</v>
       </c>
@@ -7469,7 +7528,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="17" spans="2:3">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17" s="44">
         <v>0</v>
       </c>
@@ -7477,7 +7536,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="18" spans="2:3">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B18" s="44">
         <v>1</v>
       </c>
@@ -7485,7 +7544,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="19" spans="2:3">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B19" s="44">
         <v>2</v>
       </c>
@@ -7493,7 +7552,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="20" spans="2:3">
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B20" s="44">
         <v>3</v>
       </c>
@@ -7501,7 +7560,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="21" spans="2:3">
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B21" s="44">
         <v>4</v>
       </c>
@@ -7509,7 +7568,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="22" spans="2:3">
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B22" s="44">
         <v>5</v>
       </c>
@@ -7517,7 +7576,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="23" spans="2:3">
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B23" s="44">
         <v>6</v>
       </c>
@@ -7525,7 +7584,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="24" spans="2:3">
+    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B24" s="44">
         <v>7</v>
       </c>
@@ -7533,45 +7592,45 @@
         <v>352</v>
       </c>
     </row>
-    <row r="25" spans="2:3">
-      <c r="B25" s="74" t="s">
+    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B25" s="75" t="s">
         <v>344</v>
       </c>
       <c r="C25" s="51" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="26" spans="2:3">
-      <c r="B26" s="74"/>
+    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B26" s="75"/>
       <c r="C26" s="52" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="27" spans="2:3">
-      <c r="B27" s="74"/>
+    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B27" s="75"/>
       <c r="C27" s="52" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="28" spans="2:3">
-      <c r="B28" s="74"/>
+    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B28" s="75"/>
       <c r="C28" s="52" t="s">
         <v>340</v>
       </c>
     </row>
-    <row r="29" spans="2:3">
-      <c r="B29" s="74"/>
+    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B29" s="75"/>
       <c r="C29" s="52" t="s">
         <v>341</v>
       </c>
     </row>
-    <row r="30" spans="2:3">
-      <c r="B30" s="74"/>
+    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B30" s="75"/>
       <c r="C30" s="53" t="s">
         <v>342</v>
       </c>
     </row>
-    <row r="31" spans="2:3">
+    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B31" s="44">
         <v>12</v>
       </c>
@@ -7579,7 +7638,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="32" spans="2:3">
+    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B32" s="44">
         <v>13</v>
       </c>
@@ -7587,7 +7646,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="33" spans="2:3">
+    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B33" s="44">
         <v>14</v>
       </c>
@@ -7595,7 +7654,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="34" spans="2:3">
+    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B34" s="44">
         <v>15</v>
       </c>
@@ -7616,19 +7675,19 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="31.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
         <v>227</v>
       </c>
@@ -7638,7 +7697,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>226</v>
       </c>
@@ -7655,7 +7714,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>229</v>
       </c>
@@ -7672,7 +7731,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>231</v>
       </c>
@@ -7689,7 +7748,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>233</v>
       </c>
@@ -7700,7 +7759,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>236</v>
       </c>
@@ -7711,7 +7770,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>238</v>
       </c>
@@ -7722,7 +7781,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>239</v>
       </c>
@@ -7733,54 +7792,54 @@
         <v>240</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
-      <c r="A10" s="77" t="s">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="78" t="s">
         <v>228</v>
       </c>
-      <c r="B10" s="77"/>
-      <c r="C10" s="77"/>
-    </row>
-    <row r="11" spans="1:8">
+      <c r="B10" s="78"/>
+      <c r="C10" s="78"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>362</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>363</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>364</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>365</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>367</v>
       </c>
     </row>
-    <row r="17" spans="1:1">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>368</v>
       </c>
     </row>
-    <row r="18" spans="1:1">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>369</v>
       </c>
     </row>
-    <row r="19" spans="1:1">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>370</v>
       </c>

</xml_diff>